<commit_message>
Update web reports - 2025-09-17 09:22:11
</commit_message>
<xml_diff>
--- a/labor_hour_summary.xlsx
+++ b/labor_hour_summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaos\Downloads\budget analysis\pythonProject1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaos\Downloads\budget analysis\pythonProject old2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60648C40-5990-4488-A884-374875FEE6CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D752D0F-DFF6-4C05-B3CA-F64F5151C525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
   </bookViews>
@@ -643,8 +643,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73E7749-6E67-46D7-9EAD-69069F7CE8A5}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -950,11 +950,11 @@
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="0"/>
-        <v>536</v>
+        <v>671</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
@@ -1131,10 +1131,10 @@
   <dimension ref="A1:X71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="G10" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V24" sqref="V24"/>
+      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1193,7 +1193,7 @@
       </c>
       <c r="M1" s="8" t="str">
         <f>_xlfn.XLOOKUP(M$3, personalist!$A:$A, personalist!$B:$B, NA())</f>
-        <v>Engineer/supervisor</v>
+        <v>Manager/senior Engineer</v>
       </c>
       <c r="N1" s="8" t="str">
         <f>_xlfn.XLOOKUP(N$3, personalist!$A:$A, personalist!$B:$B, NA())</f>
@@ -1281,7 +1281,7 @@
       </c>
       <c r="M2" s="12">
         <f>_xlfn.XLOOKUP(M$3, personalist!$A:$A, personalist!$C:$C, NA())</f>
-        <v>536</v>
+        <v>671</v>
       </c>
       <c r="N2" s="12">
         <f>_xlfn.XLOOKUP(N$3, personalist!$A:$A, personalist!$C:$C, NA())</f>
@@ -1722,8 +1722,12 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
+      <c r="G13" s="3">
+        <v>10</v>
+      </c>
+      <c r="H13" s="3">
+        <v>20</v>
+      </c>
       <c r="I13" s="3"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
@@ -1756,7 +1760,9 @@
       <c r="E14" s="3"/>
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
+      <c r="H14" s="3">
+        <v>20</v>
+      </c>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
@@ -1821,8 +1827,12 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+      <c r="G16" s="3">
+        <v>10</v>
+      </c>
+      <c r="H16" s="3">
+        <v>20</v>
+      </c>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
@@ -2196,7 +2206,7 @@
         <v>16</v>
       </c>
       <c r="H25" s="3">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="I25" s="3">
         <v>8</v>
@@ -3464,7 +3474,7 @@
       </c>
       <c r="M1" t="str">
         <f>'weekly hours'!M1</f>
-        <v>Engineer/supervisor</v>
+        <v>Manager/senior Engineer</v>
       </c>
       <c r="N1" t="str">
         <f>'weekly hours'!N1</f>
@@ -3553,7 +3563,7 @@
       </c>
       <c r="M2" s="13">
         <f>'weekly hours'!M2</f>
-        <v>536</v>
+        <v>671</v>
       </c>
       <c r="N2" s="13">
         <f>'weekly hours'!N2</f>
@@ -4561,13 +4571,13 @@
         <f>IF('weekly hours'!F13=0," ",'weekly hours'!F13/8*'weekly hours'!F$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G13" s="1" t="str">
+      <c r="G13" s="1">
         <f>IF('weekly hours'!G13=0," ",'weekly hours'!G13/8*'weekly hours'!G$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H13" s="1" t="str">
+        <v>838.75</v>
+      </c>
+      <c r="H13" s="1">
         <f>IF('weekly hours'!H13=0," ",'weekly hours'!H13/8*'weekly hours'!H$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>1340</v>
       </c>
       <c r="I13" s="1" t="str">
         <f>IF('weekly hours'!I13=0," ",'weekly hours'!I13/8*'weekly hours'!I$2)</f>
@@ -4659,9 +4669,9 @@
         <f>IF('weekly hours'!G14=0," ",'weekly hours'!G14/8*'weekly hours'!G$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H14" s="1" t="str">
+      <c r="H14" s="1">
         <f>IF('weekly hours'!H14=0," ",'weekly hours'!H14/8*'weekly hours'!H$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>1340</v>
       </c>
       <c r="I14" s="1" t="str">
         <f>IF('weekly hours'!I14=0," ",'weekly hours'!I14/8*'weekly hours'!I$2)</f>
@@ -4843,13 +4853,13 @@
         <f>IF('weekly hours'!F16=0," ",'weekly hours'!F16/8*'weekly hours'!F$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G16" s="1" t="str">
+      <c r="G16" s="1">
         <f>IF('weekly hours'!G16=0," ",'weekly hours'!G16/8*'weekly hours'!G$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H16" s="1" t="str">
+        <v>838.75</v>
+      </c>
+      <c r="H16" s="1">
         <f>IF('weekly hours'!H16=0," ",'weekly hours'!H16/8*'weekly hours'!H$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>1340</v>
       </c>
       <c r="I16" s="1" t="str">
         <f>IF('weekly hours'!I16=0," ",'weekly hours'!I16/8*'weekly hours'!I$2)</f>
@@ -5151,7 +5161,7 @@
       </c>
       <c r="M19" s="1">
         <f>IF('weekly hours'!M19=0," ",'weekly hours'!M19/8*'weekly hours'!M$2)</f>
-        <v>1072</v>
+        <v>1342</v>
       </c>
       <c r="N19" s="1" t="str">
         <f>IF('weekly hours'!N19=0," ",'weekly hours'!N19/8*'weekly hours'!N$2)</f>
@@ -5245,7 +5255,7 @@
       </c>
       <c r="M20" s="1">
         <f>IF('weekly hours'!M20=0," ",'weekly hours'!M20/8*'weekly hours'!M$2)</f>
-        <v>2144</v>
+        <v>2684</v>
       </c>
       <c r="N20" s="1" t="str">
         <f>IF('weekly hours'!N20=0," ",'weekly hours'!N20/8*'weekly hours'!N$2)</f>
@@ -5433,7 +5443,7 @@
       </c>
       <c r="M22" s="1">
         <f>IF('weekly hours'!M22=0," ",'weekly hours'!M22/8*'weekly hours'!M$2)</f>
-        <v>2680</v>
+        <v>3355</v>
       </c>
       <c r="N22" s="1" t="str">
         <f>IF('weekly hours'!N22=0," ",'weekly hours'!N22/8*'weekly hours'!N$2)</f>
@@ -5527,7 +5537,7 @@
       </c>
       <c r="M23" s="1">
         <f>IF('weekly hours'!M23=0," ",'weekly hours'!M23/8*'weekly hours'!M$2)</f>
-        <v>2680</v>
+        <v>3355</v>
       </c>
       <c r="N23" s="1" t="str">
         <f>IF('weekly hours'!N23=0," ",'weekly hours'!N23/8*'weekly hours'!N$2)</f>
@@ -5621,7 +5631,7 @@
       </c>
       <c r="M24" s="1">
         <f>IF('weekly hours'!M24=0," ",'weekly hours'!M24/8*'weekly hours'!M$2)</f>
-        <v>1608</v>
+        <v>2013</v>
       </c>
       <c r="N24" s="1" t="str">
         <f>IF('weekly hours'!N24=0," ",'weekly hours'!N24/8*'weekly hours'!N$2)</f>
@@ -5695,7 +5705,7 @@
       </c>
       <c r="H25" s="1">
         <f>IF('weekly hours'!H25=0," ",'weekly hours'!H25/8*'weekly hours'!H$2)</f>
-        <v>1072</v>
+        <v>1608</v>
       </c>
       <c r="I25" s="1">
         <f>IF('weekly hours'!I25=0," ",'weekly hours'!I25/8*'weekly hours'!I$2)</f>
@@ -5809,7 +5819,7 @@
       </c>
       <c r="M26" s="1">
         <f>IF('weekly hours'!M26=0," ",'weekly hours'!M26/8*'weekly hours'!M$2)</f>
-        <v>2680</v>
+        <v>3355</v>
       </c>
       <c r="N26" s="1" t="str">
         <f>IF('weekly hours'!N26=0," ",'weekly hours'!N26/8*'weekly hours'!N$2)</f>

</xml_diff>

<commit_message>
Update web reports - 2025-09-28 22:33:28
</commit_message>
<xml_diff>
--- a/labor_hour_summary.xlsx
+++ b/labor_hour_summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaos\Downloads\budget analysis\pythonProject old2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\GEO Inc\Projects\Current\2025 Ohio Medproperties - CEC\Schedule - MS project\project tracker tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D752D0F-DFF6-4C05-B3CA-F64F5151C525}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B650D31A-0943-4ADE-B808-2A3F5BF0FFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
   </bookViews>
   <sheets>
     <sheet name="personalist" sheetId="1" r:id="rId1"/>
@@ -647,18 +647,18 @@
       <selection activeCell="E23" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5234375" customWidth="1"/>
-    <col min="2" max="2" width="26.20703125" customWidth="1"/>
-    <col min="3" max="3" width="12.41796875" customWidth="1"/>
-    <col min="4" max="4" width="20.20703125" customWidth="1"/>
-    <col min="6" max="6" width="18.1015625" customWidth="1"/>
-    <col min="11" max="11" width="28.3125" customWidth="1"/>
-    <col min="12" max="12" width="11.41796875" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="11" max="11" width="28.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -669,7 +669,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -687,7 +687,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -705,7 +705,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -723,7 +723,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -741,7 +741,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -759,7 +759,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -777,7 +777,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -795,7 +795,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -813,7 +813,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -825,7 +825,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -837,7 +837,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -849,7 +849,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -861,7 +861,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -873,7 +873,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -885,7 +885,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -897,7 +897,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -909,7 +909,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -921,7 +921,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -933,7 +933,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -945,7 +945,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -957,7 +957,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -969,7 +969,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -981,7 +981,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -993,7 +993,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -1131,25 +1131,21 @@
   <dimension ref="A1:X71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="G4" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J25" sqref="J25"/>
+      <selection pane="bottomRight" activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.1015625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.68359375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.3125" style="2" customWidth="1"/>
-    <col min="4" max="6" width="8.89453125" style="2"/>
-    <col min="7" max="11" width="8.83984375" style="2"/>
-    <col min="12" max="18" width="8.89453125" style="2"/>
-    <col min="19" max="19" width="8.83984375" style="2"/>
-    <col min="20" max="24" width="8.89453125" style="2"/>
+    <col min="1" max="1" width="10.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
+    <col min="4" max="24" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="10" customFormat="1" ht="62.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:24" s="10" customFormat="1" ht="62.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>45</v>
       </c>
@@ -1237,7 +1233,7 @@
       </c>
       <c r="X1" s="9"/>
     </row>
-    <row r="2" spans="1:24" s="10" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:24" s="10" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>48</v>
       </c>
@@ -1325,7 +1321,7 @@
       </c>
       <c r="X2" s="9"/>
     </row>
-    <row r="3" spans="1:24" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:24" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -1397,7 +1393,7 @@
       </c>
       <c r="X3" s="9"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1435,7 +1431,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -1470,7 +1466,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -1503,7 +1499,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -1536,7 +1532,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -1569,7 +1565,7 @@
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -1602,7 +1598,7 @@
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -1641,7 +1637,7 @@
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -1674,7 +1670,7 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -1707,7 +1703,7 @@
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -1744,7 +1740,7 @@
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -1779,7 +1775,7 @@
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -1812,7 +1808,7 @@
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -1851,7 +1847,7 @@
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -1890,7 +1886,7 @@
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -1931,7 +1927,7 @@
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -1972,7 +1968,7 @@
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -2013,7 +2009,7 @@
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -2054,7 +2050,7 @@
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -2097,7 +2093,7 @@
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -2140,7 +2136,7 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -2187,7 +2183,7 @@
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -2228,7 +2224,7 @@
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -2273,7 +2269,7 @@
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -2288,25 +2284,45 @@
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
-      <c r="H27" s="3"/>
-      <c r="I27" s="3"/>
+      <c r="G27" s="3">
+        <v>5</v>
+      </c>
+      <c r="H27" s="3">
+        <v>10</v>
+      </c>
+      <c r="I27" s="3">
+        <v>1</v>
+      </c>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
       <c r="L27" s="3"/>
-      <c r="M27" s="3"/>
+      <c r="M27" s="3">
+        <v>40</v>
+      </c>
       <c r="N27" s="3"/>
       <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3"/>
-      <c r="R27" s="3"/>
-      <c r="S27" s="3"/>
+      <c r="P27" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>40</v>
+      </c>
+      <c r="R27" s="3">
+        <v>40</v>
+      </c>
+      <c r="S27" s="3">
+        <v>40</v>
+      </c>
       <c r="T27" s="3"/>
       <c r="U27" s="3"/>
-      <c r="V27" s="3"/>
-      <c r="W27" s="3"/>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="V27" s="3">
+        <v>40</v>
+      </c>
+      <c r="W27" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -2321,25 +2337,39 @@
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="G28" s="3">
+        <v>6</v>
+      </c>
       <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
+      <c r="I28" s="3">
+        <v>1</v>
+      </c>
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
       <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3"/>
-      <c r="R28" s="3"/>
+      <c r="P28" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>40</v>
+      </c>
+      <c r="R28" s="3">
+        <v>40</v>
+      </c>
       <c r="S28" s="3"/>
       <c r="T28" s="3"/>
       <c r="U28" s="3"/>
-      <c r="V28" s="3"/>
-      <c r="W28" s="3"/>
-    </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="V28" s="3">
+        <v>16</v>
+      </c>
+      <c r="W28" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -2372,7 +2402,7 @@
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -2405,7 +2435,7 @@
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -2438,7 +2468,7 @@
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -2471,7 +2501,7 @@
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -2504,7 +2534,7 @@
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -2537,7 +2567,7 @@
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>32</v>
       </c>
@@ -2570,7 +2600,7 @@
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>33</v>
       </c>
@@ -2603,7 +2633,7 @@
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>34</v>
       </c>
@@ -2636,7 +2666,7 @@
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>35</v>
       </c>
@@ -2669,7 +2699,7 @@
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>36</v>
       </c>
@@ -2702,7 +2732,7 @@
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>37</v>
       </c>
@@ -2735,7 +2765,7 @@
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>38</v>
       </c>
@@ -2768,7 +2798,7 @@
       <c r="V41" s="3"/>
       <c r="W41" s="3"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>39</v>
       </c>
@@ -2801,7 +2831,7 @@
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>40</v>
       </c>
@@ -2834,7 +2864,7 @@
       <c r="V43" s="3"/>
       <c r="W43" s="3"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>41</v>
       </c>
@@ -2867,7 +2897,7 @@
       <c r="V44" s="3"/>
       <c r="W44" s="3"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>42</v>
       </c>
@@ -2900,7 +2930,7 @@
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>43</v>
       </c>
@@ -2933,7 +2963,7 @@
       <c r="V46" s="3"/>
       <c r="W46" s="3"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>44</v>
       </c>
@@ -2966,7 +2996,7 @@
       <c r="V47" s="3"/>
       <c r="W47" s="3"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>45</v>
       </c>
@@ -2999,7 +3029,7 @@
       <c r="V48" s="3"/>
       <c r="W48" s="3"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>46</v>
       </c>
@@ -3032,7 +3062,7 @@
       <c r="V49" s="3"/>
       <c r="W49" s="3"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>47</v>
       </c>
@@ -3065,7 +3095,7 @@
       <c r="V50" s="3"/>
       <c r="W50" s="3"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>48</v>
       </c>
@@ -3098,7 +3128,7 @@
       <c r="V51" s="3"/>
       <c r="W51" s="3"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>49</v>
       </c>
@@ -3131,7 +3161,7 @@
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>50</v>
       </c>
@@ -3164,7 +3194,7 @@
       <c r="V53" s="3"/>
       <c r="W53" s="3"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>51</v>
       </c>
@@ -3177,7 +3207,7 @@
         <v>46110</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>52</v>
       </c>
@@ -3190,7 +3220,7 @@
         <v>46117</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>53</v>
       </c>
@@ -3203,7 +3233,7 @@
         <v>46124</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>54</v>
       </c>
@@ -3216,7 +3246,7 @@
         <v>46131</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>55</v>
       </c>
@@ -3229,7 +3259,7 @@
         <v>46138</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>56</v>
       </c>
@@ -3242,7 +3272,7 @@
         <v>46145</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>57</v>
       </c>
@@ -3255,7 +3285,7 @@
         <v>46152</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>58</v>
       </c>
@@ -3268,7 +3298,7 @@
         <v>46159</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>59</v>
       </c>
@@ -3281,7 +3311,7 @@
         <v>46166</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>60</v>
       </c>
@@ -3294,7 +3324,7 @@
         <v>46173</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>61</v>
       </c>
@@ -3307,7 +3337,7 @@
         <v>46180</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>62</v>
       </c>
@@ -3320,7 +3350,7 @@
         <v>46187</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>63</v>
       </c>
@@ -3333,7 +3363,7 @@
         <v>46194</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>64</v>
       </c>
@@ -3346,7 +3376,7 @@
         <v>46201</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>65</v>
       </c>
@@ -3359,7 +3389,7 @@
         <v>46208</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>66</v>
       </c>
@@ -3372,7 +3402,7 @@
         <v>46215</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>67</v>
       </c>
@@ -3385,7 +3415,7 @@
         <v>46222</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>68</v>
       </c>
@@ -3423,13 +3453,13 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="8.89453125" style="11"/>
-    <col min="14" max="14" width="9.7890625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" style="11"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>'weekly hours'!A1</f>
         <v>position</v>
@@ -3520,7 +3550,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="str">
         <f>'weekly hours'!A2</f>
         <v>Salary $/day</v>
@@ -3606,7 +3636,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>'weekly hours'!A3</f>
         <v>Week #</v>
@@ -3700,7 +3730,7 @@
         <v>Robert W</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>'weekly hours'!A4</f>
         <v>1</v>
@@ -3794,7 +3824,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>'weekly hours'!A5</f>
         <v>2</v>
@@ -3888,7 +3918,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>'weekly hours'!A6</f>
         <v>3</v>
@@ -3982,7 +4012,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>'weekly hours'!A7</f>
         <v>4</v>
@@ -4076,7 +4106,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>'weekly hours'!A8</f>
         <v>5</v>
@@ -4170,7 +4200,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>'weekly hours'!A9</f>
         <v>6</v>
@@ -4264,7 +4294,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>'weekly hours'!A10</f>
         <v>7</v>
@@ -4358,7 +4388,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>'weekly hours'!A11</f>
         <v>8</v>
@@ -4452,7 +4482,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>'weekly hours'!A12</f>
         <v>9</v>
@@ -4546,7 +4576,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>'weekly hours'!A13</f>
         <v>10</v>
@@ -4640,7 +4670,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>'weekly hours'!A14</f>
         <v>11</v>
@@ -4734,7 +4764,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15">
         <f>'weekly hours'!A15</f>
         <v>12</v>
@@ -4828,7 +4858,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>'weekly hours'!A16</f>
         <v>13</v>
@@ -4922,7 +4952,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17">
         <f>'weekly hours'!A17</f>
         <v>14</v>
@@ -5016,7 +5046,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18">
         <f>'weekly hours'!A18</f>
         <v>15</v>
@@ -5110,7 +5140,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19">
         <f>'weekly hours'!A19</f>
         <v>16</v>
@@ -5204,7 +5234,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20">
         <f>'weekly hours'!A20</f>
         <v>17</v>
@@ -5298,7 +5328,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21">
         <f>'weekly hours'!A21</f>
         <v>18</v>
@@ -5392,7 +5422,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22">
         <f>'weekly hours'!A22</f>
         <v>19</v>
@@ -5486,7 +5516,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23">
         <f>'weekly hours'!A23</f>
         <v>20</v>
@@ -5580,7 +5610,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24">
         <f>'weekly hours'!A24</f>
         <v>21</v>
@@ -5674,7 +5704,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25">
         <f>'weekly hours'!A25</f>
         <v>22</v>
@@ -5768,7 +5798,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26">
         <f>'weekly hours'!A26</f>
         <v>23</v>
@@ -5862,7 +5892,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27">
         <f>'weekly hours'!A27</f>
         <v>24</v>
@@ -5887,17 +5917,17 @@
         <f>IF('weekly hours'!F27=0," ",'weekly hours'!F27/8*'weekly hours'!F$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G27" s="1" t="str">
+      <c r="G27" s="1">
         <f>IF('weekly hours'!G27=0," ",'weekly hours'!G27/8*'weekly hours'!G$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H27" s="1" t="str">
+        <v>419.375</v>
+      </c>
+      <c r="H27" s="1">
         <f>IF('weekly hours'!H27=0," ",'weekly hours'!H27/8*'weekly hours'!H$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I27" s="1" t="str">
+        <v>670</v>
+      </c>
+      <c r="I27" s="1">
         <f>IF('weekly hours'!I27=0," ",'weekly hours'!I27/8*'weekly hours'!I$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>67</v>
       </c>
       <c r="J27" s="1" t="str">
         <f>IF('weekly hours'!J27=0," ",'weekly hours'!J27/8*'weekly hours'!J$2)</f>
@@ -5911,9 +5941,9 @@
         <f>IF('weekly hours'!L27=0," ",'weekly hours'!L27/8*'weekly hours'!L$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="M27" s="1" t="str">
+      <c r="M27" s="1">
         <f>IF('weekly hours'!M27=0," ",'weekly hours'!M27/8*'weekly hours'!M$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>3355</v>
       </c>
       <c r="N27" s="1" t="str">
         <f>IF('weekly hours'!N27=0," ",'weekly hours'!N27/8*'weekly hours'!N$2)</f>
@@ -5923,17 +5953,17 @@
         <f>IF('weekly hours'!O27=0," ",'weekly hours'!O27/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P27" s="1" t="str">
+      <c r="P27" s="1">
         <f>IF('weekly hours'!P27=0," ",'weekly hours'!P27/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q27" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q27" s="1">
         <f>IF('weekly hours'!Q27=0," ",'weekly hours'!Q27/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="R27" s="1" t="str">
+        <v>2280</v>
+      </c>
+      <c r="R27" s="1">
         <f>IF('weekly hours'!R27=0," ",'weekly hours'!R27/8*'weekly hours'!R$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="S27" s="1" t="str">
         <f>IF('weekly hours'!T27=0," ",'weekly hours'!T27/8*'weekly hours'!T$2)</f>
@@ -5943,20 +5973,20 @@
         <f>IF('weekly hours'!U27=0," ",'weekly hours'!U27/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U27" s="1" t="str">
+      <c r="U27" s="1">
         <f>IF('weekly hours'!V27=0," ",'weekly hours'!V27/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V27" s="1" t="str">
+        <v>2345</v>
+      </c>
+      <c r="V27" s="1">
         <f>IF('weekly hours'!W27=0," ",'weekly hours'!W27/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W27" s="1" t="str">
+        <v>2345</v>
+      </c>
+      <c r="W27" s="1">
         <f>IF('weekly hours'!S27=0," ",'weekly hours'!S27/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+        <v>2280</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28">
         <f>'weekly hours'!A28</f>
         <v>25</v>
@@ -5981,17 +6011,17 @@
         <f>IF('weekly hours'!F28=0," ",'weekly hours'!F28/8*'weekly hours'!F$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G28" s="1" t="str">
+      <c r="G28" s="1">
         <f>IF('weekly hours'!G28=0," ",'weekly hours'!G28/8*'weekly hours'!G$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>503.25</v>
       </c>
       <c r="H28" s="1" t="str">
         <f>IF('weekly hours'!H28=0," ",'weekly hours'!H28/8*'weekly hours'!H$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I28" s="1" t="str">
+      <c r="I28" s="1">
         <f>IF('weekly hours'!I28=0," ",'weekly hours'!I28/8*'weekly hours'!I$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>67</v>
       </c>
       <c r="J28" s="1" t="str">
         <f>IF('weekly hours'!J28=0," ",'weekly hours'!J28/8*'weekly hours'!J$2)</f>
@@ -6017,17 +6047,17 @@
         <f>IF('weekly hours'!O28=0," ",'weekly hours'!O28/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P28" s="1" t="str">
+      <c r="P28" s="1">
         <f>IF('weekly hours'!P28=0," ",'weekly hours'!P28/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q28" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q28" s="1">
         <f>IF('weekly hours'!Q28=0," ",'weekly hours'!Q28/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="R28" s="1" t="str">
+        <v>2280</v>
+      </c>
+      <c r="R28" s="1">
         <f>IF('weekly hours'!R28=0," ",'weekly hours'!R28/8*'weekly hours'!R$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="S28" s="1" t="str">
         <f>IF('weekly hours'!T28=0," ",'weekly hours'!T28/8*'weekly hours'!T$2)</f>
@@ -6037,20 +6067,20 @@
         <f>IF('weekly hours'!U28=0," ",'weekly hours'!U28/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U28" s="1" t="str">
+      <c r="U28" s="1">
         <f>IF('weekly hours'!V28=0," ",'weekly hours'!V28/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V28" s="1" t="str">
+        <v>938</v>
+      </c>
+      <c r="V28" s="1">
         <f>IF('weekly hours'!W28=0," ",'weekly hours'!W28/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="W28" s="1" t="str">
         <f>IF('weekly hours'!S28=0," ",'weekly hours'!S28/8*'weekly hours'!S$2)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29">
         <f>'weekly hours'!A29</f>
         <v>26</v>
@@ -6144,7 +6174,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30">
         <f>'weekly hours'!A30</f>
         <v>27</v>
@@ -6238,7 +6268,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31">
         <f>'weekly hours'!A31</f>
         <v>28</v>
@@ -6332,7 +6362,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32">
         <f>'weekly hours'!A32</f>
         <v>29</v>
@@ -6426,7 +6456,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33">
         <f>'weekly hours'!A33</f>
         <v>30</v>
@@ -6520,7 +6550,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34">
         <f>'weekly hours'!A34</f>
         <v>31</v>
@@ -6614,7 +6644,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35">
         <f>'weekly hours'!A35</f>
         <v>32</v>
@@ -6708,7 +6738,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36">
         <f>'weekly hours'!A36</f>
         <v>33</v>
@@ -6802,7 +6832,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37">
         <f>'weekly hours'!A37</f>
         <v>34</v>
@@ -6896,7 +6926,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38">
         <f>'weekly hours'!A38</f>
         <v>35</v>
@@ -6990,7 +7020,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39">
         <f>'weekly hours'!A39</f>
         <v>36</v>
@@ -7084,7 +7114,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40">
         <f>'weekly hours'!A40</f>
         <v>37</v>
@@ -7178,7 +7208,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41">
         <f>'weekly hours'!A41</f>
         <v>38</v>
@@ -7272,7 +7302,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42">
         <f>'weekly hours'!A42</f>
         <v>39</v>
@@ -7366,7 +7396,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43">
         <f>'weekly hours'!A43</f>
         <v>40</v>
@@ -7460,7 +7490,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44">
         <f>'weekly hours'!A44</f>
         <v>41</v>
@@ -7554,7 +7584,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45">
         <f>'weekly hours'!A45</f>
         <v>42</v>
@@ -7648,7 +7678,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46">
         <f>'weekly hours'!A46</f>
         <v>43</v>
@@ -7742,7 +7772,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47">
         <f>'weekly hours'!A47</f>
         <v>44</v>
@@ -7836,7 +7866,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48">
         <f>'weekly hours'!A48</f>
         <v>45</v>
@@ -7930,7 +7960,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49">
         <f>'weekly hours'!A49</f>
         <v>46</v>
@@ -8024,7 +8054,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50">
         <f>'weekly hours'!A50</f>
         <v>47</v>
@@ -8118,7 +8148,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51">
         <f>'weekly hours'!A51</f>
         <v>48</v>
@@ -8212,7 +8242,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52">
         <f>'weekly hours'!A52</f>
         <v>49</v>
@@ -8306,7 +8336,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53">
         <f>'weekly hours'!A53</f>
         <v>50</v>
@@ -8400,7 +8430,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54">
         <f>'weekly hours'!A54</f>
         <v>51</v>
@@ -8494,7 +8524,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55">
         <f>'weekly hours'!A55</f>
         <v>52</v>
@@ -8588,7 +8618,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56">
         <f>'weekly hours'!A56</f>
         <v>53</v>
@@ -8682,7 +8712,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57">
         <f>'weekly hours'!A57</f>
         <v>54</v>
@@ -8776,7 +8806,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58">
         <f>'weekly hours'!A58</f>
         <v>55</v>
@@ -8870,7 +8900,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59">
         <f>'weekly hours'!A59</f>
         <v>56</v>
@@ -8964,7 +8994,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60">
         <f>'weekly hours'!A60</f>
         <v>57</v>
@@ -9058,7 +9088,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61">
         <f>'weekly hours'!A61</f>
         <v>58</v>
@@ -9152,7 +9182,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62">
         <f>'weekly hours'!A62</f>
         <v>59</v>
@@ -9246,7 +9276,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63">
         <f>'weekly hours'!A63</f>
         <v>60</v>
@@ -9340,7 +9370,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64">
         <f>'weekly hours'!A64</f>
         <v>61</v>
@@ -9434,7 +9464,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A65">
         <f>'weekly hours'!A65</f>
         <v>62</v>
@@ -9528,7 +9558,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A66">
         <f>'weekly hours'!A66</f>
         <v>63</v>
@@ -9622,7 +9652,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A67">
         <f>'weekly hours'!A67</f>
         <v>64</v>
@@ -9716,7 +9746,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A68">
         <f>'weekly hours'!A68</f>
         <v>65</v>
@@ -9810,7 +9840,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A69">
         <f>'weekly hours'!A69</f>
         <v>66</v>
@@ -9904,7 +9934,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A70">
         <f>'weekly hours'!A70</f>
         <v>67</v>
@@ -9998,7 +10028,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A71">
         <f>'weekly hours'!A71</f>
         <v>68</v>

</xml_diff>

<commit_message>
Update web reports - 2025-10-02 15:47:37
</commit_message>
<xml_diff>
--- a/labor_hour_summary.xlsx
+++ b/labor_hour_summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\GEO Inc\Projects\Current\2025 Ohio Medproperties - CEC\Schedule - MS project\project tracker tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B650D31A-0943-4ADE-B808-2A3F5BF0FFC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CABDA9-DD54-4DC0-82A2-2BC0BC5E2336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
   </bookViews>
@@ -1131,10 +1131,10 @@
   <dimension ref="A1:X71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H27" sqref="H27"/>
+      <selection pane="bottomRight" activeCell="U29" sqref="U29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2386,21 +2386,35 @@
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
       <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
+      <c r="I29" s="3">
+        <v>1</v>
+      </c>
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
       <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3"/>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3"/>
+      <c r="P29" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>40</v>
+      </c>
+      <c r="R29" s="3">
+        <v>40</v>
+      </c>
+      <c r="S29" s="3">
+        <v>40</v>
+      </c>
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
-      <c r="V29" s="3"/>
-      <c r="W29" s="3"/>
+      <c r="V29" s="3">
+        <v>40</v>
+      </c>
+      <c r="W29" s="3">
+        <v>40</v>
+      </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
@@ -6113,9 +6127,9 @@
         <f>IF('weekly hours'!H29=0," ",'weekly hours'!H29/8*'weekly hours'!H$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I29" s="1" t="str">
+      <c r="I29" s="1">
         <f>IF('weekly hours'!I29=0," ",'weekly hours'!I29/8*'weekly hours'!I$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>67</v>
       </c>
       <c r="J29" s="1" t="str">
         <f>IF('weekly hours'!J29=0," ",'weekly hours'!J29/8*'weekly hours'!J$2)</f>
@@ -6141,17 +6155,17 @@
         <f>IF('weekly hours'!O29=0," ",'weekly hours'!O29/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P29" s="1" t="str">
+      <c r="P29" s="1">
         <f>IF('weekly hours'!P29=0," ",'weekly hours'!P29/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q29" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q29" s="1">
         <f>IF('weekly hours'!Q29=0," ",'weekly hours'!Q29/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="R29" s="1" t="str">
+        <v>2280</v>
+      </c>
+      <c r="R29" s="1">
         <f>IF('weekly hours'!R29=0," ",'weekly hours'!R29/8*'weekly hours'!R$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="S29" s="1" t="str">
         <f>IF('weekly hours'!T29=0," ",'weekly hours'!T29/8*'weekly hours'!T$2)</f>
@@ -6161,17 +6175,17 @@
         <f>IF('weekly hours'!U29=0," ",'weekly hours'!U29/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U29" s="1" t="str">
+      <c r="U29" s="1">
         <f>IF('weekly hours'!V29=0," ",'weekly hours'!V29/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V29" s="1" t="str">
+        <v>2345</v>
+      </c>
+      <c r="V29" s="1">
         <f>IF('weekly hours'!W29=0," ",'weekly hours'!W29/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W29" s="1" t="str">
+        <v>2345</v>
+      </c>
+      <c r="W29" s="1">
         <f>IF('weekly hours'!S29=0," ",'weekly hours'!S29/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2280</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Update web reports - 2025-10-09 20:42:57
</commit_message>
<xml_diff>
--- a/labor_hour_summary.xlsx
+++ b/labor_hour_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\GEO Inc\Projects\Current\2025 Ohio Medproperties - CEC\Schedule - MS project\project tracker tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25CABDA9-DD54-4DC0-82A2-2BC0BC5E2336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FD0114-CB99-4061-942B-10959022FE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
   </bookViews>
@@ -1131,10 +1131,10 @@
   <dimension ref="A1:X71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="U29" sqref="U29"/>
+      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2384,7 +2384,9 @@
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="G29" s="3">
+        <v>1</v>
+      </c>
       <c r="H29" s="3"/>
       <c r="I29" s="3">
         <v>1</v>
@@ -2410,10 +2412,11 @@
       <c r="T29" s="3"/>
       <c r="U29" s="3"/>
       <c r="V29" s="3">
-        <v>40</v>
+        <f>40-16</f>
+        <v>24</v>
       </c>
       <c r="W29" s="3">
-        <v>40</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.3">
@@ -2431,17 +2434,25 @@
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
+      <c r="G30" s="3">
+        <v>1</v>
+      </c>
       <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
+      <c r="I30" s="3">
+        <v>1</v>
+      </c>
       <c r="J30" s="3"/>
       <c r="K30" s="3"/>
       <c r="L30" s="3"/>
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3"/>
+      <c r="P30" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>40</v>
+      </c>
       <c r="R30" s="3"/>
       <c r="S30" s="3"/>
       <c r="T30" s="3"/>
@@ -6119,9 +6130,9 @@
         <f>IF('weekly hours'!F29=0," ",'weekly hours'!F29/8*'weekly hours'!F$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G29" s="1" t="str">
+      <c r="G29" s="1">
         <f>IF('weekly hours'!G29=0," ",'weekly hours'!G29/8*'weekly hours'!G$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>83.875</v>
       </c>
       <c r="H29" s="1" t="str">
         <f>IF('weekly hours'!H29=0," ",'weekly hours'!H29/8*'weekly hours'!H$2)</f>
@@ -6177,11 +6188,11 @@
       </c>
       <c r="U29" s="1">
         <f>IF('weekly hours'!V29=0," ",'weekly hours'!V29/8*'weekly hours'!V$2)</f>
-        <v>2345</v>
+        <v>1407</v>
       </c>
       <c r="V29" s="1">
         <f>IF('weekly hours'!W29=0," ",'weekly hours'!W29/8*'weekly hours'!W$2)</f>
-        <v>2345</v>
+        <v>1407</v>
       </c>
       <c r="W29" s="1">
         <f>IF('weekly hours'!S29=0," ",'weekly hours'!S29/8*'weekly hours'!S$2)</f>
@@ -6213,17 +6224,17 @@
         <f>IF('weekly hours'!F30=0," ",'weekly hours'!F30/8*'weekly hours'!F$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G30" s="1" t="str">
+      <c r="G30" s="1">
         <f>IF('weekly hours'!G30=0," ",'weekly hours'!G30/8*'weekly hours'!G$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>83.875</v>
       </c>
       <c r="H30" s="1" t="str">
         <f>IF('weekly hours'!H30=0," ",'weekly hours'!H30/8*'weekly hours'!H$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I30" s="1" t="str">
+      <c r="I30" s="1">
         <f>IF('weekly hours'!I30=0," ",'weekly hours'!I30/8*'weekly hours'!I$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>67</v>
       </c>
       <c r="J30" s="1" t="str">
         <f>IF('weekly hours'!J30=0," ",'weekly hours'!J30/8*'weekly hours'!J$2)</f>
@@ -6249,13 +6260,13 @@
         <f>IF('weekly hours'!O30=0," ",'weekly hours'!O30/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P30" s="1" t="str">
+      <c r="P30" s="1">
         <f>IF('weekly hours'!P30=0," ",'weekly hours'!P30/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q30" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q30" s="1">
         <f>IF('weekly hours'!Q30=0," ",'weekly hours'!Q30/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2280</v>
       </c>
       <c r="R30" s="1" t="str">
         <f>IF('weekly hours'!R30=0," ",'weekly hours'!R30/8*'weekly hours'!R$2)</f>

</xml_diff>

<commit_message>
Update web reports - 2025-10-17 20:46:02
</commit_message>
<xml_diff>
--- a/labor_hour_summary.xlsx
+++ b/labor_hour_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\GEO Inc\Projects\Current\2025 Ohio Medproperties - CEC\Schedule - MS project\project tracker tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6FD0114-CB99-4061-942B-10959022FE88}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907D29A3-086A-4D60-81F4-9FA2B78B0C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
   </bookViews>
@@ -1131,10 +1131,10 @@
   <dimension ref="A1:X71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="F22" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2475,23 +2475,37 @@
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
+      <c r="G31" s="3">
+        <v>1</v>
+      </c>
+      <c r="H31" s="3">
+        <v>5</v>
+      </c>
+      <c r="I31" s="3">
+        <v>1</v>
+      </c>
       <c r="J31" s="3"/>
       <c r="K31" s="3"/>
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
       <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
+      <c r="P31" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q31" s="3">
+        <v>40</v>
+      </c>
       <c r="R31" s="3"/>
       <c r="S31" s="3"/>
       <c r="T31" s="3"/>
       <c r="U31" s="3"/>
-      <c r="V31" s="3"/>
-      <c r="W31" s="3"/>
+      <c r="V31" s="3">
+        <v>40</v>
+      </c>
+      <c r="W31" s="3">
+        <v>40</v>
+      </c>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
@@ -6318,17 +6332,17 @@
         <f>IF('weekly hours'!F31=0," ",'weekly hours'!F31/8*'weekly hours'!F$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="G31" s="1" t="str">
+      <c r="G31" s="1">
         <f>IF('weekly hours'!G31=0," ",'weekly hours'!G31/8*'weekly hours'!G$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="H31" s="1" t="str">
+        <v>83.875</v>
+      </c>
+      <c r="H31" s="1">
         <f>IF('weekly hours'!H31=0," ",'weekly hours'!H31/8*'weekly hours'!H$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I31" s="1" t="str">
+        <v>335</v>
+      </c>
+      <c r="I31" s="1">
         <f>IF('weekly hours'!I31=0," ",'weekly hours'!I31/8*'weekly hours'!I$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>67</v>
       </c>
       <c r="J31" s="1" t="str">
         <f>IF('weekly hours'!J31=0," ",'weekly hours'!J31/8*'weekly hours'!J$2)</f>
@@ -6354,13 +6368,13 @@
         <f>IF('weekly hours'!O31=0," ",'weekly hours'!O31/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P31" s="1" t="str">
+      <c r="P31" s="1">
         <f>IF('weekly hours'!P31=0," ",'weekly hours'!P31/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q31" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q31" s="1">
         <f>IF('weekly hours'!Q31=0," ",'weekly hours'!Q31/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2280</v>
       </c>
       <c r="R31" s="1" t="str">
         <f>IF('weekly hours'!R31=0," ",'weekly hours'!R31/8*'weekly hours'!R$2)</f>
@@ -6374,13 +6388,13 @@
         <f>IF('weekly hours'!U31=0," ",'weekly hours'!U31/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U31" s="1" t="str">
+      <c r="U31" s="1">
         <f>IF('weekly hours'!V31=0," ",'weekly hours'!V31/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V31" s="1" t="str">
+        <v>2345</v>
+      </c>
+      <c r="V31" s="1">
         <f>IF('weekly hours'!W31=0," ",'weekly hours'!W31/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="W31" s="1" t="str">
         <f>IF('weekly hours'!S31=0," ",'weekly hours'!S31/8*'weekly hours'!S$2)</f>

</xml_diff>

<commit_message>
Update web reports - 2025-10-25 22:28:58
</commit_message>
<xml_diff>
--- a/labor_hour_summary.xlsx
+++ b/labor_hour_summary.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\GEO Inc\Projects\Current\2025 Ohio Medproperties - CEC\Schedule - MS project\project tracker tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907D29A3-086A-4D60-81F4-9FA2B78B0C69}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8960D07D-FEDE-4F58-B94A-1C50B83AEBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
   </bookViews>
@@ -1134,7 +1134,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2524,21 +2524,35 @@
       <c r="F32" s="3"/>
       <c r="G32" s="3"/>
       <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
+      <c r="I32" s="3">
+        <v>1</v>
+      </c>
       <c r="J32" s="3"/>
       <c r="K32" s="3"/>
-      <c r="L32" s="3"/>
+      <c r="L32" s="3">
+        <v>32</v>
+      </c>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
       <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3"/>
-      <c r="R32" s="3"/>
+      <c r="P32" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q32" s="3">
+        <v>40</v>
+      </c>
+      <c r="R32" s="3">
+        <v>40</v>
+      </c>
       <c r="S32" s="3"/>
       <c r="T32" s="3"/>
       <c r="U32" s="3"/>
-      <c r="V32" s="3"/>
-      <c r="W32" s="3"/>
+      <c r="V32" s="3">
+        <v>40</v>
+      </c>
+      <c r="W32" s="3">
+        <v>40</v>
+      </c>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
@@ -6434,9 +6448,9 @@
         <f>IF('weekly hours'!H32=0," ",'weekly hours'!H32/8*'weekly hours'!H$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I32" s="1" t="str">
+      <c r="I32" s="1">
         <f>IF('weekly hours'!I32=0," ",'weekly hours'!I32/8*'weekly hours'!I$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>67</v>
       </c>
       <c r="J32" s="1" t="str">
         <f>IF('weekly hours'!J32=0," ",'weekly hours'!J32/8*'weekly hours'!J$2)</f>
@@ -6446,9 +6460,9 @@
         <f>IF('weekly hours'!K32=0," ",'weekly hours'!K32/8*'weekly hours'!K$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="L32" s="1" t="str">
+      <c r="L32" s="1">
         <f>IF('weekly hours'!L32=0," ",'weekly hours'!L32/8*'weekly hours'!L$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2684</v>
       </c>
       <c r="M32" s="1" t="str">
         <f>IF('weekly hours'!M32=0," ",'weekly hours'!M32/8*'weekly hours'!M$2)</f>
@@ -6462,17 +6476,17 @@
         <f>IF('weekly hours'!O32=0," ",'weekly hours'!O32/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P32" s="1" t="str">
+      <c r="P32" s="1">
         <f>IF('weekly hours'!P32=0," ",'weekly hours'!P32/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q32" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q32" s="1">
         <f>IF('weekly hours'!Q32=0," ",'weekly hours'!Q32/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="R32" s="1" t="str">
+        <v>2280</v>
+      </c>
+      <c r="R32" s="1">
         <f>IF('weekly hours'!R32=0," ",'weekly hours'!R32/8*'weekly hours'!R$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="S32" s="1" t="str">
         <f>IF('weekly hours'!T32=0," ",'weekly hours'!T32/8*'weekly hours'!T$2)</f>
@@ -6482,13 +6496,13 @@
         <f>IF('weekly hours'!U32=0," ",'weekly hours'!U32/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U32" s="1" t="str">
+      <c r="U32" s="1">
         <f>IF('weekly hours'!V32=0," ",'weekly hours'!V32/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V32" s="1" t="str">
+        <v>2345</v>
+      </c>
+      <c r="V32" s="1">
         <f>IF('weekly hours'!W32=0," ",'weekly hours'!W32/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="W32" s="1" t="str">
         <f>IF('weekly hours'!S32=0," ",'weekly hours'!S32/8*'weekly hours'!S$2)</f>

</xml_diff>

<commit_message>
Update web reports - 2025-11-15 23:20:32
</commit_message>
<xml_diff>
--- a/labor_hour_summary.xlsx
+++ b/labor_hour_summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\GEO Inc\Projects\Current\2025 Ohio Medproperties - CEC\Schedule - MS project\project tracker tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8960D07D-FEDE-4F58-B94A-1C50B83AEBD8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B4E18A-3B0D-4FFA-8BB2-31C30DC71FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
   </bookViews>
@@ -1134,7 +1134,7 @@
       <pane xSplit="3" ySplit="3" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="G32" sqref="G32"/>
+      <selection pane="bottomRight" activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2578,13 +2578,21 @@
       <c r="M33" s="3"/>
       <c r="N33" s="3"/>
       <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
+      <c r="P33" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q33" s="3">
+        <v>40</v>
+      </c>
+      <c r="R33" s="3">
+        <v>40</v>
+      </c>
       <c r="S33" s="3"/>
       <c r="T33" s="3"/>
       <c r="U33" s="3"/>
-      <c r="V33" s="3"/>
+      <c r="V33" s="3">
+        <v>40</v>
+      </c>
       <c r="W33" s="3"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.3">
@@ -2611,14 +2619,20 @@
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
       <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3"/>
+      <c r="P34" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q34" s="3">
+        <v>40</v>
+      </c>
       <c r="R34" s="3"/>
       <c r="S34" s="3"/>
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
-      <c r="W34" s="3"/>
+      <c r="W34" s="3">
+        <v>8</v>
+      </c>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
@@ -2646,12 +2660,18 @@
       <c r="O35" s="3"/>
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
-      <c r="R35" s="3"/>
+      <c r="R35" s="3">
+        <v>40</v>
+      </c>
       <c r="S35" s="3"/>
       <c r="T35" s="3"/>
       <c r="U35" s="3"/>
-      <c r="V35" s="3"/>
-      <c r="W35" s="3"/>
+      <c r="V35" s="3">
+        <v>40</v>
+      </c>
+      <c r="W35" s="3">
+        <v>40</v>
+      </c>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
@@ -6570,17 +6590,17 @@
         <f>IF('weekly hours'!O33=0," ",'weekly hours'!O33/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P33" s="1" t="str">
+      <c r="P33" s="1">
         <f>IF('weekly hours'!P33=0," ",'weekly hours'!P33/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q33" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q33" s="1">
         <f>IF('weekly hours'!Q33=0," ",'weekly hours'!Q33/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="R33" s="1" t="str">
+        <v>2280</v>
+      </c>
+      <c r="R33" s="1">
         <f>IF('weekly hours'!R33=0," ",'weekly hours'!R33/8*'weekly hours'!R$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="S33" s="1" t="str">
         <f>IF('weekly hours'!T33=0," ",'weekly hours'!T33/8*'weekly hours'!T$2)</f>
@@ -6590,9 +6610,9 @@
         <f>IF('weekly hours'!U33=0," ",'weekly hours'!U33/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U33" s="1" t="str">
+      <c r="U33" s="1">
         <f>IF('weekly hours'!V33=0," ",'weekly hours'!V33/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="V33" s="1" t="str">
         <f>IF('weekly hours'!W33=0," ",'weekly hours'!W33/8*'weekly hours'!W$2)</f>
@@ -6664,13 +6684,13 @@
         <f>IF('weekly hours'!O34=0," ",'weekly hours'!O34/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P34" s="1" t="str">
+      <c r="P34" s="1">
         <f>IF('weekly hours'!P34=0," ",'weekly hours'!P34/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q34" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q34" s="1">
         <f>IF('weekly hours'!Q34=0," ",'weekly hours'!Q34/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2280</v>
       </c>
       <c r="R34" s="1" t="str">
         <f>IF('weekly hours'!R34=0," ",'weekly hours'!R34/8*'weekly hours'!R$2)</f>
@@ -6688,9 +6708,9 @@
         <f>IF('weekly hours'!V34=0," ",'weekly hours'!V34/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V34" s="1" t="str">
+      <c r="V34" s="1">
         <f>IF('weekly hours'!W34=0," ",'weekly hours'!W34/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>469</v>
       </c>
       <c r="W34" s="1" t="str">
         <f>IF('weekly hours'!S34=0," ",'weekly hours'!S34/8*'weekly hours'!S$2)</f>
@@ -6766,9 +6786,9 @@
         <f>IF('weekly hours'!Q35=0," ",'weekly hours'!Q35/8*'weekly hours'!Q$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="R35" s="1" t="str">
+      <c r="R35" s="1">
         <f>IF('weekly hours'!R35=0," ",'weekly hours'!R35/8*'weekly hours'!R$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="S35" s="1" t="str">
         <f>IF('weekly hours'!T35=0," ",'weekly hours'!T35/8*'weekly hours'!T$2)</f>
@@ -6778,13 +6798,13 @@
         <f>IF('weekly hours'!U35=0," ",'weekly hours'!U35/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U35" s="1" t="str">
+      <c r="U35" s="1">
         <f>IF('weekly hours'!V35=0," ",'weekly hours'!V35/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V35" s="1" t="str">
+        <v>2345</v>
+      </c>
+      <c r="V35" s="1">
         <f>IF('weekly hours'!W35=0," ",'weekly hours'!W35/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="W35" s="1" t="str">
         <f>IF('weekly hours'!S35=0," ",'weekly hours'!S35/8*'weekly hours'!S$2)</f>

</xml_diff>

<commit_message>
Update web reports - 2025-12-01 14:54:39
</commit_message>
<xml_diff>
--- a/labor_hour_summary.xlsx
+++ b/labor_hour_summary.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\GEO Inc\Projects\Current\2025 Ohio Medproperties - CEC\Schedule - MS project\project tracker tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaos\Downloads\budget analysis\pythonProject-ohio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32B4E18A-3B0D-4FFA-8BB2-31C30DC71FC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6D0280-E559-4F6B-9DF1-DD87D3CCDA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
+    <workbookView xWindow="-28920" yWindow="9030" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
   </bookViews>
   <sheets>
     <sheet name="personalist" sheetId="1" r:id="rId1"/>
@@ -643,22 +643,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73E7749-6E67-46D7-9EAD-69069F7CE8A5}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" customWidth="1"/>
-    <col min="11" max="11" width="28.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.5234375" customWidth="1"/>
+    <col min="2" max="2" width="26.3125" customWidth="1"/>
+    <col min="3" max="3" width="12.41796875" customWidth="1"/>
+    <col min="4" max="4" width="20.3125" customWidth="1"/>
+    <col min="6" max="6" width="18.1015625" customWidth="1"/>
+    <col min="11" max="11" width="28.3125" customWidth="1"/>
+    <col min="12" max="12" width="11.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -669,7 +669,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -687,7 +687,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -705,7 +705,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -723,7 +723,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -741,7 +741,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -759,7 +759,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -777,7 +777,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -795,7 +795,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -813,7 +813,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -825,7 +825,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -837,7 +837,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -849,7 +849,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -861,7 +861,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -873,7 +873,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -885,7 +885,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -897,7 +897,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -909,7 +909,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -921,7 +921,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -933,7 +933,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -945,7 +945,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -957,7 +957,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -969,7 +969,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -981,7 +981,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -993,7 +993,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1053,7 +1053,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1065,7 +1065,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1089,7 +1089,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -1101,7 +1101,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -1134,18 +1134,18 @@
       <pane xSplit="3" ySplit="3" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="P35" sqref="P35"/>
+      <selection pane="bottomRight" activeCell="A37" sqref="A37:XFD37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="24" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="10.1015625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.68359375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.3125" style="2" customWidth="1"/>
+    <col min="4" max="24" width="8.89453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="10" customFormat="1" ht="62.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" s="10" customFormat="1" ht="62.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
         <v>45</v>
       </c>
@@ -1233,7 +1233,7 @@
       </c>
       <c r="X1" s="9"/>
     </row>
-    <row r="2" spans="1:24" s="10" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" s="10" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
         <v>48</v>
       </c>
@@ -1321,7 +1321,7 @@
       </c>
       <c r="X2" s="9"/>
     </row>
-    <row r="3" spans="1:24" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -1365,7 +1365,7 @@
         <v>19</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>38</v>
@@ -1393,7 +1393,7 @@
       </c>
       <c r="X3" s="9"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1431,7 +1431,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -1466,7 +1466,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -1499,7 +1499,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -1532,7 +1532,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -1565,7 +1565,7 @@
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -1598,7 +1598,7 @@
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -1637,7 +1637,7 @@
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -1670,7 +1670,7 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -1703,7 +1703,7 @@
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -1740,7 +1740,7 @@
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -1775,7 +1775,7 @@
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -1808,7 +1808,7 @@
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -1847,7 +1847,7 @@
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -1886,7 +1886,7 @@
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -1927,7 +1927,7 @@
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -1968,7 +1968,7 @@
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -2009,7 +2009,7 @@
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -2050,7 +2050,7 @@
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -2093,7 +2093,7 @@
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -2136,7 +2136,7 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -2183,7 +2183,7 @@
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -2224,7 +2224,7 @@
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -2269,7 +2269,7 @@
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -2369,7 +2369,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -2419,7 +2419,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -2460,7 +2460,7 @@
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -2507,7 +2507,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -2554,7 +2554,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -2571,7 +2571,9 @@
       <c r="F33" s="3"/>
       <c r="G33" s="3"/>
       <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
+      <c r="I33" s="3">
+        <v>1</v>
+      </c>
       <c r="J33" s="3"/>
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
@@ -2595,7 +2597,7 @@
       </c>
       <c r="W33" s="3"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -2612,7 +2614,9 @@
       <c r="F34" s="3"/>
       <c r="G34" s="3"/>
       <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
+      <c r="I34" s="3">
+        <v>1</v>
+      </c>
       <c r="J34" s="3"/>
       <c r="K34" s="3"/>
       <c r="L34" s="3"/>
@@ -2634,7 +2638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3">
         <v>32</v>
       </c>
@@ -2651,13 +2655,17 @@
       <c r="F35" s="3"/>
       <c r="G35" s="3"/>
       <c r="H35" s="3"/>
-      <c r="I35" s="3"/>
+      <c r="I35" s="3">
+        <v>1</v>
+      </c>
       <c r="J35" s="3"/>
       <c r="K35" s="3"/>
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
+      <c r="O35" s="3">
+        <v>32</v>
+      </c>
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="3">
@@ -2673,7 +2681,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3">
         <v>33</v>
       </c>
@@ -2689,24 +2697,36 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
       <c r="G36" s="3"/>
-      <c r="H36" s="3"/>
-      <c r="I36" s="3"/>
+      <c r="H36" s="3">
+        <v>1</v>
+      </c>
+      <c r="I36" s="3">
+        <v>1</v>
+      </c>
       <c r="J36" s="3"/>
       <c r="K36" s="3"/>
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
+      <c r="O36" s="3">
+        <v>40</v>
+      </c>
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
-      <c r="R36" s="3"/>
+      <c r="R36" s="3">
+        <v>40</v>
+      </c>
       <c r="S36" s="3"/>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
-      <c r="V36" s="3"/>
-      <c r="W36" s="3"/>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+      <c r="V36" s="3">
+        <v>40</v>
+      </c>
+      <c r="W36" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="3">
         <v>34</v>
       </c>
@@ -2730,7 +2750,9 @@
       <c r="M37" s="3"/>
       <c r="N37" s="3"/>
       <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
+      <c r="P37" s="3">
+        <v>16</v>
+      </c>
       <c r="Q37" s="3"/>
       <c r="R37" s="3"/>
       <c r="S37" s="3"/>
@@ -2739,7 +2761,7 @@
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="3">
         <v>35</v>
       </c>
@@ -2772,7 +2794,7 @@
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3">
         <v>36</v>
       </c>
@@ -2805,7 +2827,7 @@
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3">
         <v>37</v>
       </c>
@@ -2838,7 +2860,7 @@
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="3">
         <v>38</v>
       </c>
@@ -2871,7 +2893,7 @@
       <c r="V41" s="3"/>
       <c r="W41" s="3"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="3">
         <v>39</v>
       </c>
@@ -2904,7 +2926,7 @@
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="3">
         <v>40</v>
       </c>
@@ -2937,7 +2959,7 @@
       <c r="V43" s="3"/>
       <c r="W43" s="3"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="3">
         <v>41</v>
       </c>
@@ -2970,7 +2992,7 @@
       <c r="V44" s="3"/>
       <c r="W44" s="3"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3">
         <v>42</v>
       </c>
@@ -3003,7 +3025,7 @@
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="3">
         <v>43</v>
       </c>
@@ -3036,7 +3058,7 @@
       <c r="V46" s="3"/>
       <c r="W46" s="3"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="3">
         <v>44</v>
       </c>
@@ -3069,7 +3091,7 @@
       <c r="V47" s="3"/>
       <c r="W47" s="3"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="3">
         <v>45</v>
       </c>
@@ -3102,7 +3124,7 @@
       <c r="V48" s="3"/>
       <c r="W48" s="3"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="3">
         <v>46</v>
       </c>
@@ -3135,7 +3157,7 @@
       <c r="V49" s="3"/>
       <c r="W49" s="3"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="3">
         <v>47</v>
       </c>
@@ -3168,7 +3190,7 @@
       <c r="V50" s="3"/>
       <c r="W50" s="3"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="3">
         <v>48</v>
       </c>
@@ -3201,7 +3223,7 @@
       <c r="V51" s="3"/>
       <c r="W51" s="3"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="3">
         <v>49</v>
       </c>
@@ -3234,7 +3256,7 @@
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="3">
         <v>50</v>
       </c>
@@ -3267,7 +3289,7 @@
       <c r="V53" s="3"/>
       <c r="W53" s="3"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="3">
         <v>51</v>
       </c>
@@ -3280,7 +3302,7 @@
         <v>46110</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="3">
         <v>52</v>
       </c>
@@ -3293,7 +3315,7 @@
         <v>46117</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="3">
         <v>53</v>
       </c>
@@ -3306,7 +3328,7 @@
         <v>46124</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="3">
         <v>54</v>
       </c>
@@ -3319,7 +3341,7 @@
         <v>46131</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="3">
         <v>55</v>
       </c>
@@ -3332,7 +3354,7 @@
         <v>46138</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="3">
         <v>56</v>
       </c>
@@ -3345,7 +3367,7 @@
         <v>46145</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="3">
         <v>57</v>
       </c>
@@ -3358,7 +3380,7 @@
         <v>46152</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="3">
         <v>58</v>
       </c>
@@ -3371,7 +3393,7 @@
         <v>46159</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="3">
         <v>59</v>
       </c>
@@ -3384,7 +3406,7 @@
         <v>46166</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="3">
         <v>60</v>
       </c>
@@ -3397,7 +3419,7 @@
         <v>46173</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="3">
         <v>61</v>
       </c>
@@ -3410,7 +3432,7 @@
         <v>46180</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="3">
         <v>62</v>
       </c>
@@ -3423,7 +3445,7 @@
         <v>46187</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="3">
         <v>63</v>
       </c>
@@ -3436,7 +3458,7 @@
         <v>46194</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="3">
         <v>64</v>
       </c>
@@ -3449,7 +3471,7 @@
         <v>46201</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="3">
         <v>65</v>
       </c>
@@ -3462,7 +3484,7 @@
         <v>46208</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="3">
         <v>66</v>
       </c>
@@ -3475,7 +3497,7 @@
         <v>46215</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="3">
         <v>67</v>
       </c>
@@ -3488,7 +3510,7 @@
         <v>46222</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="3">
         <v>68</v>
       </c>
@@ -3510,7 +3532,7 @@
           <x14:formula1>
             <xm:f>personalist!$A$2:$A$159</xm:f>
           </x14:formula1>
-          <xm:sqref>G3:K3 D3:W3</xm:sqref>
+          <xm:sqref>D3:W3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3526,13 +3548,13 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="3" width="8.88671875" style="11"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.89453125" style="11"/>
+    <col min="14" max="14" width="9.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="str">
         <f>'weekly hours'!A1</f>
         <v>position</v>
@@ -3623,7 +3645,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="13" t="str">
         <f>'weekly hours'!A2</f>
         <v>Salary $/day</v>
@@ -3709,7 +3731,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="str">
         <f>'weekly hours'!A3</f>
         <v>Week #</v>
@@ -3768,7 +3790,7 @@
       </c>
       <c r="O3" t="str">
         <f>'weekly hours'!O3</f>
-        <v>Brian M</v>
+        <v>Vu T</v>
       </c>
       <c r="P3" t="str">
         <f>'weekly hours'!P3</f>
@@ -3803,7 +3825,7 @@
         <v>Robert W</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <f>'weekly hours'!A4</f>
         <v>1</v>
@@ -3897,7 +3919,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <f>'weekly hours'!A5</f>
         <v>2</v>
@@ -3991,7 +4013,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <f>'weekly hours'!A6</f>
         <v>3</v>
@@ -4085,7 +4107,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <f>'weekly hours'!A7</f>
         <v>4</v>
@@ -4179,7 +4201,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <f>'weekly hours'!A8</f>
         <v>5</v>
@@ -4273,7 +4295,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <f>'weekly hours'!A9</f>
         <v>6</v>
@@ -4367,7 +4389,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <f>'weekly hours'!A10</f>
         <v>7</v>
@@ -4461,7 +4483,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <f>'weekly hours'!A11</f>
         <v>8</v>
@@ -4555,7 +4577,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <f>'weekly hours'!A12</f>
         <v>9</v>
@@ -4649,7 +4671,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <f>'weekly hours'!A13</f>
         <v>10</v>
@@ -4743,7 +4765,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <f>'weekly hours'!A14</f>
         <v>11</v>
@@ -4837,7 +4859,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <f>'weekly hours'!A15</f>
         <v>12</v>
@@ -4931,7 +4953,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <f>'weekly hours'!A16</f>
         <v>13</v>
@@ -5025,7 +5047,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <f>'weekly hours'!A17</f>
         <v>14</v>
@@ -5119,7 +5141,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <f>'weekly hours'!A18</f>
         <v>15</v>
@@ -5213,7 +5235,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <f>'weekly hours'!A19</f>
         <v>16</v>
@@ -5307,7 +5329,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <f>'weekly hours'!A20</f>
         <v>17</v>
@@ -5401,7 +5423,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <f>'weekly hours'!A21</f>
         <v>18</v>
@@ -5495,7 +5517,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <f>'weekly hours'!A22</f>
         <v>19</v>
@@ -5589,7 +5611,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <f>'weekly hours'!A23</f>
         <v>20</v>
@@ -5683,7 +5705,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <f>'weekly hours'!A24</f>
         <v>21</v>
@@ -5777,7 +5799,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <f>'weekly hours'!A25</f>
         <v>22</v>
@@ -5871,7 +5893,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <f>'weekly hours'!A26</f>
         <v>23</v>
@@ -5965,7 +5987,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <f>'weekly hours'!A27</f>
         <v>24</v>
@@ -6059,7 +6081,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <f>'weekly hours'!A28</f>
         <v>25</v>
@@ -6153,7 +6175,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <f>'weekly hours'!A29</f>
         <v>26</v>
@@ -6247,7 +6269,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <f>'weekly hours'!A30</f>
         <v>27</v>
@@ -6341,7 +6363,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <f>'weekly hours'!A31</f>
         <v>28</v>
@@ -6435,7 +6457,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <f>'weekly hours'!A32</f>
         <v>29</v>
@@ -6529,7 +6551,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <f>'weekly hours'!A33</f>
         <v>30</v>
@@ -6562,9 +6584,9 @@
         <f>IF('weekly hours'!H33=0," ",'weekly hours'!H33/8*'weekly hours'!H$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I33" s="1" t="str">
+      <c r="I33" s="1">
         <f>IF('weekly hours'!I33=0," ",'weekly hours'!I33/8*'weekly hours'!I$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>67</v>
       </c>
       <c r="J33" s="1" t="str">
         <f>IF('weekly hours'!J33=0," ",'weekly hours'!J33/8*'weekly hours'!J$2)</f>
@@ -6623,7 +6645,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <f>'weekly hours'!A34</f>
         <v>31</v>
@@ -6656,9 +6678,9 @@
         <f>IF('weekly hours'!H34=0," ",'weekly hours'!H34/8*'weekly hours'!H$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I34" s="1" t="str">
+      <c r="I34" s="1">
         <f>IF('weekly hours'!I34=0," ",'weekly hours'!I34/8*'weekly hours'!I$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>67</v>
       </c>
       <c r="J34" s="1" t="str">
         <f>IF('weekly hours'!J34=0," ",'weekly hours'!J34/8*'weekly hours'!J$2)</f>
@@ -6717,7 +6739,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <f>'weekly hours'!A35</f>
         <v>32</v>
@@ -6750,9 +6772,9 @@
         <f>IF('weekly hours'!H35=0," ",'weekly hours'!H35/8*'weekly hours'!H$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I35" s="1" t="str">
+      <c r="I35" s="1">
         <f>IF('weekly hours'!I35=0," ",'weekly hours'!I35/8*'weekly hours'!I$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>67</v>
       </c>
       <c r="J35" s="1" t="str">
         <f>IF('weekly hours'!J35=0," ",'weekly hours'!J35/8*'weekly hours'!J$2)</f>
@@ -6774,9 +6796,9 @@
         <f>IF('weekly hours'!N35=0," ",'weekly hours'!N35/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O35" s="1" t="str">
+      <c r="O35" s="1">
         <f>IF('weekly hours'!O35=0," ",'weekly hours'!O35/8*'weekly hours'!O$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2144</v>
       </c>
       <c r="P35" s="1" t="str">
         <f>IF('weekly hours'!P35=0," ",'weekly hours'!P35/8*'weekly hours'!P$2)</f>
@@ -6811,7 +6833,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <f>'weekly hours'!A36</f>
         <v>33</v>
@@ -6840,13 +6862,13 @@
         <f>IF('weekly hours'!G36=0," ",'weekly hours'!G36/8*'weekly hours'!G$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H36" s="1" t="str">
+      <c r="H36" s="1">
         <f>IF('weekly hours'!H36=0," ",'weekly hours'!H36/8*'weekly hours'!H$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I36" s="1" t="str">
+        <v>67</v>
+      </c>
+      <c r="I36" s="1">
         <f>IF('weekly hours'!I36=0," ",'weekly hours'!I36/8*'weekly hours'!I$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>67</v>
       </c>
       <c r="J36" s="1" t="str">
         <f>IF('weekly hours'!J36=0," ",'weekly hours'!J36/8*'weekly hours'!J$2)</f>
@@ -6868,9 +6890,9 @@
         <f>IF('weekly hours'!N36=0," ",'weekly hours'!N36/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O36" s="1" t="str">
+      <c r="O36" s="1">
         <f>IF('weekly hours'!O36=0," ",'weekly hours'!O36/8*'weekly hours'!O$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2680</v>
       </c>
       <c r="P36" s="1" t="str">
         <f>IF('weekly hours'!P36=0," ",'weekly hours'!P36/8*'weekly hours'!P$2)</f>
@@ -6880,9 +6902,9 @@
         <f>IF('weekly hours'!Q36=0," ",'weekly hours'!Q36/8*'weekly hours'!Q$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="R36" s="1" t="str">
+      <c r="R36" s="1">
         <f>IF('weekly hours'!R36=0," ",'weekly hours'!R36/8*'weekly hours'!R$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="S36" s="1" t="str">
         <f>IF('weekly hours'!T36=0," ",'weekly hours'!T36/8*'weekly hours'!T$2)</f>
@@ -6892,20 +6914,20 @@
         <f>IF('weekly hours'!U36=0," ",'weekly hours'!U36/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U36" s="1" t="str">
+      <c r="U36" s="1">
         <f>IF('weekly hours'!V36=0," ",'weekly hours'!V36/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V36" s="1" t="str">
+        <v>2345</v>
+      </c>
+      <c r="V36" s="1">
         <f>IF('weekly hours'!W36=0," ",'weekly hours'!W36/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="W36" s="1" t="str">
         <f>IF('weekly hours'!S36=0," ",'weekly hours'!S36/8*'weekly hours'!S$2)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <f>'weekly hours'!A37</f>
         <v>34</v>
@@ -6966,9 +6988,9 @@
         <f>IF('weekly hours'!O37=0," ",'weekly hours'!O37/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P37" s="1" t="str">
+      <c r="P37" s="1">
         <f>IF('weekly hours'!P37=0," ",'weekly hours'!P37/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>1072</v>
       </c>
       <c r="Q37" s="1" t="str">
         <f>IF('weekly hours'!Q37=0," ",'weekly hours'!Q37/8*'weekly hours'!Q$2)</f>
@@ -6999,7 +7021,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <f>'weekly hours'!A38</f>
         <v>35</v>
@@ -7093,7 +7115,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <f>'weekly hours'!A39</f>
         <v>36</v>
@@ -7187,7 +7209,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <f>'weekly hours'!A40</f>
         <v>37</v>
@@ -7281,7 +7303,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <f>'weekly hours'!A41</f>
         <v>38</v>
@@ -7375,7 +7397,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <f>'weekly hours'!A42</f>
         <v>39</v>
@@ -7469,7 +7491,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <f>'weekly hours'!A43</f>
         <v>40</v>
@@ -7563,7 +7585,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <f>'weekly hours'!A44</f>
         <v>41</v>
@@ -7657,7 +7679,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <f>'weekly hours'!A45</f>
         <v>42</v>
@@ -7751,7 +7773,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <f>'weekly hours'!A46</f>
         <v>43</v>
@@ -7845,7 +7867,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <f>'weekly hours'!A47</f>
         <v>44</v>
@@ -7939,7 +7961,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <f>'weekly hours'!A48</f>
         <v>45</v>
@@ -8033,7 +8055,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <f>'weekly hours'!A49</f>
         <v>46</v>
@@ -8127,7 +8149,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <f>'weekly hours'!A50</f>
         <v>47</v>
@@ -8221,7 +8243,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <f>'weekly hours'!A51</f>
         <v>48</v>
@@ -8315,7 +8337,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <f>'weekly hours'!A52</f>
         <v>49</v>
@@ -8409,7 +8431,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <f>'weekly hours'!A53</f>
         <v>50</v>
@@ -8503,7 +8525,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <f>'weekly hours'!A54</f>
         <v>51</v>
@@ -8597,7 +8619,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <f>'weekly hours'!A55</f>
         <v>52</v>
@@ -8691,7 +8713,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <f>'weekly hours'!A56</f>
         <v>53</v>
@@ -8785,7 +8807,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <f>'weekly hours'!A57</f>
         <v>54</v>
@@ -8879,7 +8901,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <f>'weekly hours'!A58</f>
         <v>55</v>
@@ -8973,7 +8995,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <f>'weekly hours'!A59</f>
         <v>56</v>
@@ -9067,7 +9089,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <f>'weekly hours'!A60</f>
         <v>57</v>
@@ -9161,7 +9183,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
         <f>'weekly hours'!A61</f>
         <v>58</v>
@@ -9255,7 +9277,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <f>'weekly hours'!A62</f>
         <v>59</v>
@@ -9349,7 +9371,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <f>'weekly hours'!A63</f>
         <v>60</v>
@@ -9443,7 +9465,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <f>'weekly hours'!A64</f>
         <v>61</v>
@@ -9537,7 +9559,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <f>'weekly hours'!A65</f>
         <v>62</v>
@@ -9631,7 +9653,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <f>'weekly hours'!A66</f>
         <v>63</v>
@@ -9725,7 +9747,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
         <f>'weekly hours'!A67</f>
         <v>64</v>
@@ -9819,7 +9841,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <f>'weekly hours'!A68</f>
         <v>65</v>
@@ -9913,7 +9935,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <f>'weekly hours'!A69</f>
         <v>66</v>
@@ -10007,7 +10029,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <f>'weekly hours'!A70</f>
         <v>67</v>
@@ -10101,7 +10123,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
         <f>'weekly hours'!A71</f>
         <v>68</v>

</xml_diff>

<commit_message>
Update web reports - 2025-12-31 16:42:34
</commit_message>
<xml_diff>
--- a/labor_hour_summary.xlsx
+++ b/labor_hour_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaos\Downloads\budget analysis\pythonProject-ohio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\GEO Inc\Projects\Current\2025 Ohio Medproperties - CEC\Schedule - MS project\project tracker tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA6D0280-E559-4F6B-9DF1-DD87D3CCDA52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C033E729-8EFE-4E6D-BE28-AAB98955274E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="9030" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
   </bookViews>
   <sheets>
     <sheet name="personalist" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
   <si>
     <t>Jason C</t>
   </si>
@@ -185,6 +185,12 @@
   </si>
   <si>
     <t>Salary $/day</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Engineer/ supervisor  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tony M </t>
   </si>
 </sst>
 </file>
@@ -647,18 +653,18 @@
       <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.5234375" customWidth="1"/>
-    <col min="2" max="2" width="26.3125" customWidth="1"/>
-    <col min="3" max="3" width="12.41796875" customWidth="1"/>
-    <col min="4" max="4" width="20.3125" customWidth="1"/>
-    <col min="6" max="6" width="18.1015625" customWidth="1"/>
-    <col min="11" max="11" width="28.3125" customWidth="1"/>
-    <col min="12" max="12" width="11.41796875" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+    <col min="4" max="4" width="20.33203125" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
+    <col min="11" max="11" width="28.33203125" customWidth="1"/>
+    <col min="12" max="12" width="11.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -669,7 +675,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -687,7 +693,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>21</v>
       </c>
@@ -705,7 +711,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>38</v>
       </c>
@@ -723,7 +729,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -741,7 +747,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>24</v>
       </c>
@@ -759,7 +765,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -777,7 +783,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>19</v>
       </c>
@@ -795,7 +801,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>25</v>
       </c>
@@ -813,7 +819,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -825,7 +831,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -837,7 +843,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>23</v>
       </c>
@@ -849,7 +855,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -861,7 +867,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>7</v>
       </c>
@@ -873,7 +879,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -885,7 +891,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>26</v>
       </c>
@@ -897,7 +903,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>17</v>
       </c>
@@ -909,7 +915,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>6</v>
       </c>
@@ -921,7 +927,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>0</v>
       </c>
@@ -933,7 +939,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>35</v>
       </c>
@@ -945,7 +951,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>22</v>
       </c>
@@ -957,7 +963,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -969,7 +975,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>8</v>
       </c>
@@ -981,7 +987,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -993,7 +999,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>18</v>
       </c>
@@ -1005,7 +1011,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>29</v>
       </c>
@@ -1017,7 +1023,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>34</v>
       </c>
@@ -1029,7 +1035,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>9</v>
       </c>
@@ -1041,7 +1047,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1053,7 +1059,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>15</v>
       </c>
@@ -1065,7 +1071,7 @@
         <v>671</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>36</v>
       </c>
@@ -1077,7 +1083,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>27</v>
       </c>
@@ -1089,7 +1095,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>20</v>
       </c>
@@ -1101,7 +1107,7 @@
         <v>536</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -1128,24 +1134,24 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C09D152-DDC8-4DBE-9D9E-8C1B7612C220}">
-  <dimension ref="A1:X71"/>
+  <dimension ref="A1:Y71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="F25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="F31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A37" sqref="A37:XFD37"/>
+      <selection pane="bottomRight" activeCell="V40" sqref="V40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="10.1015625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.68359375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.3125" style="2" customWidth="1"/>
-    <col min="4" max="24" width="8.89453125" style="2"/>
+    <col min="1" max="1" width="10.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
+    <col min="4" max="24" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="10" customFormat="1" ht="62.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:25" s="10" customFormat="1" ht="62.7" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
         <v>45</v>
       </c>
@@ -1231,9 +1237,11 @@
         <f>_xlfn.XLOOKUP(W$3, personalist!$A:$A, personalist!$B:$B, NA())</f>
         <v>Welder</v>
       </c>
-      <c r="X1" s="9"/>
-    </row>
-    <row r="2" spans="1:24" s="10" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="X1" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="2" spans="1:25" s="10" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
         <v>48</v>
       </c>
@@ -1321,7 +1329,7 @@
       </c>
       <c r="X2" s="9"/>
     </row>
-    <row r="3" spans="1:24" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:25" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -1365,7 +1373,7 @@
         <v>19</v>
       </c>
       <c r="O3" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="P3" s="8" t="s">
         <v>38</v>
@@ -1391,9 +1399,14 @@
       <c r="W3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="X3" s="9"/>
-    </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+      <c r="X3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="Y3" s="9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1431,7 +1444,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -1466,7 +1479,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -1499,7 +1512,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -1532,7 +1545,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -1565,7 +1578,7 @@
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -1598,7 +1611,7 @@
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -1637,7 +1650,7 @@
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -1670,7 +1683,7 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -1703,7 +1716,7 @@
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -1740,7 +1753,7 @@
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -1775,7 +1788,7 @@
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -1808,7 +1821,7 @@
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -1847,7 +1860,7 @@
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -1886,7 +1899,7 @@
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -1927,7 +1940,7 @@
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -1968,7 +1981,7 @@
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -2009,7 +2022,7 @@
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -2050,7 +2063,7 @@
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -2093,7 +2106,7 @@
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -2136,7 +2149,7 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -2183,7 +2196,7 @@
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -2224,7 +2237,7 @@
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -2269,7 +2282,7 @@
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -2322,7 +2335,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -2369,7 +2382,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -2419,7 +2432,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -2460,7 +2473,7 @@
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -2507,7 +2520,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -2554,7 +2567,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -2597,7 +2610,7 @@
       </c>
       <c r="W33" s="3"/>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -2638,7 +2651,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A35" s="3">
         <v>32</v>
       </c>
@@ -2663,9 +2676,7 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
-      <c r="O35" s="3">
-        <v>32</v>
-      </c>
+      <c r="O35" s="3"/>
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="3">
@@ -2680,8 +2691,11 @@
       <c r="W35" s="3">
         <v>40</v>
       </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="X35" s="2">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A36" s="3">
         <v>33</v>
       </c>
@@ -2708,9 +2722,7 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
-      <c r="O36" s="3">
-        <v>40</v>
-      </c>
+      <c r="O36" s="3"/>
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3">
@@ -2725,8 +2737,11 @@
       <c r="W36" s="3">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="X36" s="2">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A37" s="3">
         <v>34</v>
       </c>
@@ -2743,7 +2758,9 @@
       <c r="F37" s="3"/>
       <c r="G37" s="3"/>
       <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
+      <c r="I37" s="3">
+        <v>1</v>
+      </c>
       <c r="J37" s="3"/>
       <c r="K37" s="3"/>
       <c r="L37" s="3"/>
@@ -2761,7 +2778,7 @@
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A38" s="3">
         <v>35</v>
       </c>
@@ -2778,23 +2795,33 @@
       <c r="F38" s="3"/>
       <c r="G38" s="3"/>
       <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
+      <c r="I38" s="3">
+        <v>1</v>
+      </c>
       <c r="J38" s="3"/>
       <c r="K38" s="3"/>
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
       <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
+      <c r="P38" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>40</v>
+      </c>
+      <c r="R38" s="3">
+        <v>40</v>
+      </c>
       <c r="S38" s="3"/>
       <c r="T38" s="3"/>
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
-      <c r="W38" s="3"/>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="W38" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A39" s="3">
         <v>36</v>
       </c>
@@ -2814,20 +2841,32 @@
       <c r="I39" s="3"/>
       <c r="J39" s="3"/>
       <c r="K39" s="3"/>
-      <c r="L39" s="3"/>
+      <c r="L39" s="3">
+        <v>40</v>
+      </c>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
       <c r="O39" s="3"/>
-      <c r="P39" s="3"/>
-      <c r="Q39" s="3"/>
-      <c r="R39" s="3"/>
+      <c r="P39" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>40</v>
+      </c>
+      <c r="R39" s="3">
+        <v>40</v>
+      </c>
       <c r="S39" s="3"/>
       <c r="T39" s="3"/>
       <c r="U39" s="3"/>
-      <c r="V39" s="3"/>
-      <c r="W39" s="3"/>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="V39" s="3">
+        <v>40</v>
+      </c>
+      <c r="W39" s="3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A40" s="3">
         <v>37</v>
       </c>
@@ -2847,20 +2886,35 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
       <c r="K40" s="3"/>
-      <c r="L40" s="3"/>
+      <c r="L40" s="3">
+        <v>40</v>
+      </c>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
       <c r="O40" s="3"/>
-      <c r="P40" s="3"/>
-      <c r="Q40" s="3"/>
-      <c r="R40" s="3"/>
+      <c r="P40" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>40</v>
+      </c>
+      <c r="R40" s="3">
+        <v>40</v>
+      </c>
       <c r="S40" s="3"/>
       <c r="T40" s="3"/>
       <c r="U40" s="3"/>
-      <c r="V40" s="3"/>
-      <c r="W40" s="3"/>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+      <c r="V40" s="3">
+        <v>40</v>
+      </c>
+      <c r="W40" s="3">
+        <v>40</v>
+      </c>
+      <c r="Y40">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A41" s="3">
         <v>38</v>
       </c>
@@ -2893,7 +2947,7 @@
       <c r="V41" s="3"/>
       <c r="W41" s="3"/>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A42" s="3">
         <v>39</v>
       </c>
@@ -2926,7 +2980,7 @@
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A43" s="3">
         <v>40</v>
       </c>
@@ -2959,7 +3013,7 @@
       <c r="V43" s="3"/>
       <c r="W43" s="3"/>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A44" s="3">
         <v>41</v>
       </c>
@@ -2992,7 +3046,7 @@
       <c r="V44" s="3"/>
       <c r="W44" s="3"/>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A45" s="3">
         <v>42</v>
       </c>
@@ -3025,7 +3079,7 @@
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A46" s="3">
         <v>43</v>
       </c>
@@ -3058,7 +3112,7 @@
       <c r="V46" s="3"/>
       <c r="W46" s="3"/>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A47" s="3">
         <v>44</v>
       </c>
@@ -3091,7 +3145,7 @@
       <c r="V47" s="3"/>
       <c r="W47" s="3"/>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A48" s="3">
         <v>45</v>
       </c>
@@ -3124,7 +3178,7 @@
       <c r="V48" s="3"/>
       <c r="W48" s="3"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49" s="3">
         <v>46</v>
       </c>
@@ -3157,7 +3211,7 @@
       <c r="V49" s="3"/>
       <c r="W49" s="3"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50" s="3">
         <v>47</v>
       </c>
@@ -3190,7 +3244,7 @@
       <c r="V50" s="3"/>
       <c r="W50" s="3"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51" s="3">
         <v>48</v>
       </c>
@@ -3223,7 +3277,7 @@
       <c r="V51" s="3"/>
       <c r="W51" s="3"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52" s="3">
         <v>49</v>
       </c>
@@ -3256,7 +3310,7 @@
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53" s="3">
         <v>50</v>
       </c>
@@ -3289,7 +3343,7 @@
       <c r="V53" s="3"/>
       <c r="W53" s="3"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54" s="3">
         <v>51</v>
       </c>
@@ -3302,7 +3356,7 @@
         <v>46110</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55" s="3">
         <v>52</v>
       </c>
@@ -3315,7 +3369,7 @@
         <v>46117</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56" s="3">
         <v>53</v>
       </c>
@@ -3328,7 +3382,7 @@
         <v>46124</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57" s="3">
         <v>54</v>
       </c>
@@ -3341,7 +3395,7 @@
         <v>46131</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58" s="3">
         <v>55</v>
       </c>
@@ -3354,7 +3408,7 @@
         <v>46138</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59" s="3">
         <v>56</v>
       </c>
@@ -3367,7 +3421,7 @@
         <v>46145</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60" s="3">
         <v>57</v>
       </c>
@@ -3380,7 +3434,7 @@
         <v>46152</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61" s="3">
         <v>58</v>
       </c>
@@ -3393,7 +3447,7 @@
         <v>46159</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62" s="3">
         <v>59</v>
       </c>
@@ -3406,7 +3460,7 @@
         <v>46166</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63" s="3">
         <v>60</v>
       </c>
@@ -3419,7 +3473,7 @@
         <v>46173</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64" s="3">
         <v>61</v>
       </c>
@@ -3432,7 +3486,7 @@
         <v>46180</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="3">
         <v>62</v>
       </c>
@@ -3445,7 +3499,7 @@
         <v>46187</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="3">
         <v>63</v>
       </c>
@@ -3458,7 +3512,7 @@
         <v>46194</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="3">
         <v>64</v>
       </c>
@@ -3471,7 +3525,7 @@
         <v>46201</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="3">
         <v>65</v>
       </c>
@@ -3484,7 +3538,7 @@
         <v>46208</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="3">
         <v>66</v>
       </c>
@@ -3497,7 +3551,7 @@
         <v>46215</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="3">
         <v>67</v>
       </c>
@@ -3510,7 +3564,7 @@
         <v>46222</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="3">
         <v>68</v>
       </c>
@@ -3548,13 +3602,13 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="3" width="8.89453125" style="11"/>
-    <col min="14" max="14" width="9.68359375" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.88671875" style="11"/>
+    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A1" t="str">
         <f>'weekly hours'!A1</f>
         <v>position</v>
@@ -3645,7 +3699,7 @@
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="13" t="str">
         <f>'weekly hours'!A2</f>
         <v>Salary $/day</v>
@@ -3731,7 +3785,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A3" t="str">
         <f>'weekly hours'!A3</f>
         <v>Week #</v>
@@ -3790,7 +3844,7 @@
       </c>
       <c r="O3" t="str">
         <f>'weekly hours'!O3</f>
-        <v>Vu T</v>
+        <v>Brian M</v>
       </c>
       <c r="P3" t="str">
         <f>'weekly hours'!P3</f>
@@ -3825,7 +3879,7 @@
         <v>Robert W</v>
       </c>
     </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A4">
         <f>'weekly hours'!A4</f>
         <v>1</v>
@@ -3919,7 +3973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A5">
         <f>'weekly hours'!A5</f>
         <v>2</v>
@@ -4013,7 +4067,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A6">
         <f>'weekly hours'!A6</f>
         <v>3</v>
@@ -4107,7 +4161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A7">
         <f>'weekly hours'!A7</f>
         <v>4</v>
@@ -4201,7 +4255,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A8">
         <f>'weekly hours'!A8</f>
         <v>5</v>
@@ -4295,7 +4349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A9">
         <f>'weekly hours'!A9</f>
         <v>6</v>
@@ -4389,7 +4443,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A10">
         <f>'weekly hours'!A10</f>
         <v>7</v>
@@ -4483,7 +4537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A11">
         <f>'weekly hours'!A11</f>
         <v>8</v>
@@ -4577,7 +4631,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A12">
         <f>'weekly hours'!A12</f>
         <v>9</v>
@@ -4671,7 +4725,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A13">
         <f>'weekly hours'!A13</f>
         <v>10</v>
@@ -4765,7 +4819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A14">
         <f>'weekly hours'!A14</f>
         <v>11</v>
@@ -4859,7 +4913,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A15">
         <f>'weekly hours'!A15</f>
         <v>12</v>
@@ -4953,7 +5007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
       <c r="A16">
         <f>'weekly hours'!A16</f>
         <v>13</v>
@@ -5047,7 +5101,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A17">
         <f>'weekly hours'!A17</f>
         <v>14</v>
@@ -5141,7 +5195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A18">
         <f>'weekly hours'!A18</f>
         <v>15</v>
@@ -5235,7 +5289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A19">
         <f>'weekly hours'!A19</f>
         <v>16</v>
@@ -5329,7 +5383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A20">
         <f>'weekly hours'!A20</f>
         <v>17</v>
@@ -5423,7 +5477,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A21">
         <f>'weekly hours'!A21</f>
         <v>18</v>
@@ -5517,7 +5571,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A22">
         <f>'weekly hours'!A22</f>
         <v>19</v>
@@ -5611,7 +5665,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A23">
         <f>'weekly hours'!A23</f>
         <v>20</v>
@@ -5705,7 +5759,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A24">
         <f>'weekly hours'!A24</f>
         <v>21</v>
@@ -5799,7 +5853,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A25">
         <f>'weekly hours'!A25</f>
         <v>22</v>
@@ -5893,7 +5947,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A26">
         <f>'weekly hours'!A26</f>
         <v>23</v>
@@ -5987,7 +6041,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A27">
         <f>'weekly hours'!A27</f>
         <v>24</v>
@@ -6081,7 +6135,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A28">
         <f>'weekly hours'!A28</f>
         <v>25</v>
@@ -6175,7 +6229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A29">
         <f>'weekly hours'!A29</f>
         <v>26</v>
@@ -6269,7 +6323,7 @@
         <v>2280</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A30">
         <f>'weekly hours'!A30</f>
         <v>27</v>
@@ -6363,7 +6417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A31">
         <f>'weekly hours'!A31</f>
         <v>28</v>
@@ -6457,7 +6511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A32">
         <f>'weekly hours'!A32</f>
         <v>29</v>
@@ -6551,7 +6605,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A33">
         <f>'weekly hours'!A33</f>
         <v>30</v>
@@ -6645,7 +6699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A34">
         <f>'weekly hours'!A34</f>
         <v>31</v>
@@ -6739,7 +6793,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A35">
         <f>'weekly hours'!A35</f>
         <v>32</v>
@@ -6796,9 +6850,9 @@
         <f>IF('weekly hours'!N35=0," ",'weekly hours'!N35/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O35" s="1">
+      <c r="O35" s="1" t="str">
         <f>IF('weekly hours'!O35=0," ",'weekly hours'!O35/8*'weekly hours'!O$2)</f>
-        <v>2144</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="P35" s="1" t="str">
         <f>IF('weekly hours'!P35=0," ",'weekly hours'!P35/8*'weekly hours'!P$2)</f>
@@ -6833,7 +6887,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A36">
         <f>'weekly hours'!A36</f>
         <v>33</v>
@@ -6890,9 +6944,9 @@
         <f>IF('weekly hours'!N36=0," ",'weekly hours'!N36/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O36" s="1">
+      <c r="O36" s="1" t="str">
         <f>IF('weekly hours'!O36=0," ",'weekly hours'!O36/8*'weekly hours'!O$2)</f>
-        <v>2680</v>
+        <v xml:space="preserve"> </v>
       </c>
       <c r="P36" s="1" t="str">
         <f>IF('weekly hours'!P36=0," ",'weekly hours'!P36/8*'weekly hours'!P$2)</f>
@@ -6927,7 +6981,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A37">
         <f>'weekly hours'!A37</f>
         <v>34</v>
@@ -6960,9 +7014,9 @@
         <f>IF('weekly hours'!H37=0," ",'weekly hours'!H37/8*'weekly hours'!H$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I37" s="1" t="str">
+      <c r="I37" s="1">
         <f>IF('weekly hours'!I37=0," ",'weekly hours'!I37/8*'weekly hours'!I$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>67</v>
       </c>
       <c r="J37" s="1" t="str">
         <f>IF('weekly hours'!J37=0," ",'weekly hours'!J37/8*'weekly hours'!J$2)</f>
@@ -7021,7 +7075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A38">
         <f>'weekly hours'!A38</f>
         <v>35</v>
@@ -7054,9 +7108,9 @@
         <f>IF('weekly hours'!H38=0," ",'weekly hours'!H38/8*'weekly hours'!H$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="I38" s="1" t="str">
+      <c r="I38" s="1">
         <f>IF('weekly hours'!I38=0," ",'weekly hours'!I38/8*'weekly hours'!I$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>67</v>
       </c>
       <c r="J38" s="1" t="str">
         <f>IF('weekly hours'!J38=0," ",'weekly hours'!J38/8*'weekly hours'!J$2)</f>
@@ -7082,17 +7136,17 @@
         <f>IF('weekly hours'!O38=0," ",'weekly hours'!O38/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P38" s="1" t="str">
+      <c r="P38" s="1">
         <f>IF('weekly hours'!P38=0," ",'weekly hours'!P38/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q38" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q38" s="1">
         <f>IF('weekly hours'!Q38=0," ",'weekly hours'!Q38/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="R38" s="1" t="str">
+        <v>2280</v>
+      </c>
+      <c r="R38" s="1">
         <f>IF('weekly hours'!R38=0," ",'weekly hours'!R38/8*'weekly hours'!R$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="S38" s="1" t="str">
         <f>IF('weekly hours'!T38=0," ",'weekly hours'!T38/8*'weekly hours'!T$2)</f>
@@ -7106,16 +7160,16 @@
         <f>IF('weekly hours'!V38=0," ",'weekly hours'!V38/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V38" s="1" t="str">
+      <c r="V38" s="1">
         <f>IF('weekly hours'!W38=0," ",'weekly hours'!W38/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="W38" s="1" t="str">
         <f>IF('weekly hours'!S38=0," ",'weekly hours'!S38/8*'weekly hours'!S$2)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A39">
         <f>'weekly hours'!A39</f>
         <v>36</v>
@@ -7160,9 +7214,9 @@
         <f>IF('weekly hours'!K39=0," ",'weekly hours'!K39/8*'weekly hours'!K$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="L39" s="1" t="str">
+      <c r="L39" s="1">
         <f>IF('weekly hours'!L39=0," ",'weekly hours'!L39/8*'weekly hours'!L$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>3355</v>
       </c>
       <c r="M39" s="1" t="str">
         <f>IF('weekly hours'!M39=0," ",'weekly hours'!M39/8*'weekly hours'!M$2)</f>
@@ -7176,17 +7230,17 @@
         <f>IF('weekly hours'!O39=0," ",'weekly hours'!O39/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P39" s="1" t="str">
+      <c r="P39" s="1">
         <f>IF('weekly hours'!P39=0," ",'weekly hours'!P39/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q39" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q39" s="1">
         <f>IF('weekly hours'!Q39=0," ",'weekly hours'!Q39/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="R39" s="1" t="str">
+        <v>2280</v>
+      </c>
+      <c r="R39" s="1">
         <f>IF('weekly hours'!R39=0," ",'weekly hours'!R39/8*'weekly hours'!R$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="S39" s="1" t="str">
         <f>IF('weekly hours'!T39=0," ",'weekly hours'!T39/8*'weekly hours'!T$2)</f>
@@ -7196,20 +7250,20 @@
         <f>IF('weekly hours'!U39=0," ",'weekly hours'!U39/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U39" s="1" t="str">
+      <c r="U39" s="1">
         <f>IF('weekly hours'!V39=0," ",'weekly hours'!V39/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V39" s="1" t="str">
+        <v>2345</v>
+      </c>
+      <c r="V39" s="1">
         <f>IF('weekly hours'!W39=0," ",'weekly hours'!W39/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="W39" s="1" t="str">
         <f>IF('weekly hours'!S39=0," ",'weekly hours'!S39/8*'weekly hours'!S$2)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A40">
         <f>'weekly hours'!A40</f>
         <v>37</v>
@@ -7254,9 +7308,9 @@
         <f>IF('weekly hours'!K40=0," ",'weekly hours'!K40/8*'weekly hours'!K$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="L40" s="1" t="str">
+      <c r="L40" s="1">
         <f>IF('weekly hours'!L40=0," ",'weekly hours'!L40/8*'weekly hours'!L$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>3355</v>
       </c>
       <c r="M40" s="1" t="str">
         <f>IF('weekly hours'!M40=0," ",'weekly hours'!M40/8*'weekly hours'!M$2)</f>
@@ -7270,17 +7324,17 @@
         <f>IF('weekly hours'!O40=0," ",'weekly hours'!O40/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P40" s="1" t="str">
+      <c r="P40" s="1">
         <f>IF('weekly hours'!P40=0," ",'weekly hours'!P40/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q40" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q40" s="1">
         <f>IF('weekly hours'!Q40=0," ",'weekly hours'!Q40/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="R40" s="1" t="str">
+        <v>2280</v>
+      </c>
+      <c r="R40" s="1">
         <f>IF('weekly hours'!R40=0," ",'weekly hours'!R40/8*'weekly hours'!R$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="S40" s="1" t="str">
         <f>IF('weekly hours'!T40=0," ",'weekly hours'!T40/8*'weekly hours'!T$2)</f>
@@ -7290,20 +7344,20 @@
         <f>IF('weekly hours'!U40=0," ",'weekly hours'!U40/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U40" s="1" t="str">
+      <c r="U40" s="1">
         <f>IF('weekly hours'!V40=0," ",'weekly hours'!V40/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V40" s="1" t="str">
+        <v>2345</v>
+      </c>
+      <c r="V40" s="1">
         <f>IF('weekly hours'!W40=0," ",'weekly hours'!W40/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="W40" s="1" t="str">
         <f>IF('weekly hours'!S40=0," ",'weekly hours'!S40/8*'weekly hours'!S$2)</f>
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A41">
         <f>'weekly hours'!A41</f>
         <v>38</v>
@@ -7397,7 +7451,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A42">
         <f>'weekly hours'!A42</f>
         <v>39</v>
@@ -7491,7 +7545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A43">
         <f>'weekly hours'!A43</f>
         <v>40</v>
@@ -7585,7 +7639,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A44">
         <f>'weekly hours'!A44</f>
         <v>41</v>
@@ -7679,7 +7733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A45">
         <f>'weekly hours'!A45</f>
         <v>42</v>
@@ -7773,7 +7827,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A46">
         <f>'weekly hours'!A46</f>
         <v>43</v>
@@ -7867,7 +7921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A47">
         <f>'weekly hours'!A47</f>
         <v>44</v>
@@ -7961,7 +8015,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A48">
         <f>'weekly hours'!A48</f>
         <v>45</v>
@@ -8055,7 +8109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A49">
         <f>'weekly hours'!A49</f>
         <v>46</v>
@@ -8149,7 +8203,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A50">
         <f>'weekly hours'!A50</f>
         <v>47</v>
@@ -8243,7 +8297,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A51">
         <f>'weekly hours'!A51</f>
         <v>48</v>
@@ -8337,7 +8391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A52">
         <f>'weekly hours'!A52</f>
         <v>49</v>
@@ -8431,7 +8485,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A53">
         <f>'weekly hours'!A53</f>
         <v>50</v>
@@ -8525,7 +8579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A54">
         <f>'weekly hours'!A54</f>
         <v>51</v>
@@ -8619,7 +8673,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A55">
         <f>'weekly hours'!A55</f>
         <v>52</v>
@@ -8713,7 +8767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A56">
         <f>'weekly hours'!A56</f>
         <v>53</v>
@@ -8807,7 +8861,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A57">
         <f>'weekly hours'!A57</f>
         <v>54</v>
@@ -8901,7 +8955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A58">
         <f>'weekly hours'!A58</f>
         <v>55</v>
@@ -8995,7 +9049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A59">
         <f>'weekly hours'!A59</f>
         <v>56</v>
@@ -9089,7 +9143,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A60">
         <f>'weekly hours'!A60</f>
         <v>57</v>
@@ -9183,7 +9237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A61">
         <f>'weekly hours'!A61</f>
         <v>58</v>
@@ -9277,7 +9331,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A62">
         <f>'weekly hours'!A62</f>
         <v>59</v>
@@ -9371,7 +9425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A63">
         <f>'weekly hours'!A63</f>
         <v>60</v>
@@ -9465,7 +9519,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A64">
         <f>'weekly hours'!A64</f>
         <v>61</v>
@@ -9559,7 +9613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A65">
         <f>'weekly hours'!A65</f>
         <v>62</v>
@@ -9653,7 +9707,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A66">
         <f>'weekly hours'!A66</f>
         <v>63</v>
@@ -9747,7 +9801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A67">
         <f>'weekly hours'!A67</f>
         <v>64</v>
@@ -9841,7 +9895,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A68">
         <f>'weekly hours'!A68</f>
         <v>65</v>
@@ -9935,7 +9989,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A69">
         <f>'weekly hours'!A69</f>
         <v>66</v>
@@ -10029,7 +10083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A70">
         <f>'weekly hours'!A70</f>
         <v>67</v>
@@ -10123,7 +10177,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A71">
         <f>'weekly hours'!A71</f>
         <v>68</v>

</xml_diff>

<commit_message>
Update web reports - 2026-01-20 18:02:25
</commit_message>
<xml_diff>
--- a/labor_hour_summary.xlsx
+++ b/labor_hour_summary.xlsx
@@ -5,17 +5,17 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\GEO Inc\Projects\Current\2025 Ohio Medproperties - CEC\Schedule - MS project\project tracker tool\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaos\Downloads\budget analysis\pythonProject-ohio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C033E729-8EFE-4E6D-BE28-AAB98955274E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD803C3-1A6A-42B8-99C6-5828AF002743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
+    <workbookView xWindow="12675" yWindow="-18120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
   </bookViews>
   <sheets>
     <sheet name="personalist" sheetId="1" r:id="rId1"/>
     <sheet name="weekly hours" sheetId="2" r:id="rId2"/>
-    <sheet name="labor Cost" sheetId="3" state="hidden" r:id="rId3"/>
+    <sheet name="labor Cost" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
   <si>
     <t>Jason C</t>
   </si>
@@ -142,9 +142,6 @@
     <t>Luke G</t>
   </si>
   <si>
-    <t>Robert W</t>
-  </si>
-  <si>
     <t>Joe F</t>
   </si>
   <si>
@@ -185,9 +182,6 @@
   </si>
   <si>
     <t>Salary $/day</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Engineer/ supervisor  </t>
   </si>
   <si>
     <t xml:space="preserve">Tony M </t>
@@ -282,7 +276,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -313,6 +307,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="4" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,21 +647,21 @@
   <dimension ref="A1:E34"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="26.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-    <col min="4" max="4" width="20.33203125" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" customWidth="1"/>
-    <col min="11" max="11" width="28.33203125" customWidth="1"/>
-    <col min="12" max="12" width="11.44140625" customWidth="1"/>
+    <col min="1" max="1" width="15.5234375" customWidth="1"/>
+    <col min="2" max="2" width="26.3125" customWidth="1"/>
+    <col min="3" max="3" width="12.41796875" customWidth="1"/>
+    <col min="4" max="4" width="20.3125" customWidth="1"/>
+    <col min="6" max="6" width="18.1015625" customWidth="1"/>
+    <col min="11" max="11" width="28.3125" customWidth="1"/>
+    <col min="12" max="12" width="11.41796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
         <v>12</v>
       </c>
@@ -672,69 +669,69 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
         <v>16</v>
       </c>
       <c r="B2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1">
         <f>VLOOKUP(B2, $D$3:$E$9, 2, FALSE)</f>
         <v>671</v>
       </c>
       <c r="D2" t="s">
+        <v>44</v>
+      </c>
+      <c r="E2" t="s">
         <v>45</v>
       </c>
-      <c r="E2" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
         <v>21</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:C34" si="0">VLOOKUP(B3, $D$3:$E$9, 2, FALSE)</f>
         <v>671</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E3" s="6">
         <v>295</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
         <v>536</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E4" s="6">
         <v>456</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
         <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
@@ -747,223 +744,223 @@
         <v>469</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
         <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E6" s="6">
         <v>536</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
         <v>671</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E7" s="7">
         <v>671</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
         <v>19</v>
       </c>
       <c r="B8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
         <v>536</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E8" s="6">
         <v>536</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
         <v>25</v>
       </c>
       <c r="B9" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="E9" s="7">
         <v>671</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
         <v>671</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
         <v>13</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
         <v>536</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
         <v>23</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" t="s">
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
         <v>536</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
         <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
         <v>671</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
         <v>26</v>
       </c>
       <c r="B16" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" t="s">
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="0"/>
         <v>671</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" t="s">
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="0"/>
         <v>671</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B20" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
         <v>22</v>
       </c>
       <c r="B21" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="0"/>
         <v>671</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
         <v>32</v>
       </c>
@@ -975,19 +972,19 @@
         <v>469</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" t="s">
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="0"/>
         <v>536</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
         <v>33</v>
       </c>
@@ -999,55 +996,55 @@
         <v>469</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
         <v>18</v>
       </c>
       <c r="B25" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
         <v>29</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>34</v>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
+      <c r="A27" s="14" t="s">
+        <v>48</v>
       </c>
       <c r="B27" t="s">
         <v>40</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" si="0"/>
-        <v>456</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
         <v>9</v>
       </c>
       <c r="B28" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" si="0"/>
         <v>536</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1059,55 +1056,55 @@
         <v>469</v>
       </c>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
         <v>15</v>
       </c>
       <c r="B30" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" si="0"/>
         <v>671</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
         <v>27</v>
       </c>
       <c r="B32" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
         <v>20</v>
       </c>
       <c r="B33" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" si="0"/>
         <v>536</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
         <v>30</v>
       </c>
@@ -1134,26 +1131,26 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C09D152-DDC8-4DBE-9D9E-8C1B7612C220}">
-  <dimension ref="A1:Y71"/>
+  <dimension ref="A1:W71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="F31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="D31" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="V40" sqref="V40"/>
+      <selection pane="bottomRight" activeCell="X1" sqref="X1:Z1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="10.109375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="2" customWidth="1"/>
-    <col min="4" max="24" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="10.1015625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="12.68359375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.3125" style="2" customWidth="1"/>
+    <col min="4" max="23" width="8.89453125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="10" customFormat="1" ht="62.7" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:23" s="10" customFormat="1" ht="62.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1219,11 +1216,11 @@
       </c>
       <c r="S1" s="8" t="str">
         <f>_xlfn.XLOOKUP(S$3, personalist!$A:$A, personalist!$B:$B, NA())</f>
-        <v>Technician II</v>
+        <v>Engineer/supervisor</v>
       </c>
       <c r="T1" s="8" t="str">
         <f>_xlfn.XLOOKUP(T$3, personalist!$A:$A, personalist!$B:$B, NA())</f>
-        <v>Technician II</v>
+        <v>Engineer/supervisor</v>
       </c>
       <c r="U1" s="8" t="str">
         <f>_xlfn.XLOOKUP(U$3, personalist!$A:$A, personalist!$B:$B, NA())</f>
@@ -1237,13 +1234,10 @@
         <f>_xlfn.XLOOKUP(W$3, personalist!$A:$A, personalist!$B:$B, NA())</f>
         <v>Welder</v>
       </c>
-      <c r="X1" s="9" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="2" spans="1:25" s="10" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:23" s="10" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1309,11 +1303,11 @@
       </c>
       <c r="S2" s="12">
         <f>_xlfn.XLOOKUP(S$3, personalist!$A:$A, personalist!$C:$C, NA())</f>
-        <v>456</v>
+        <v>536</v>
       </c>
       <c r="T2" s="12">
         <f>_xlfn.XLOOKUP(T$3, personalist!$A:$A, personalist!$C:$C, NA())</f>
-        <v>456</v>
+        <v>536</v>
       </c>
       <c r="U2" s="12">
         <f>_xlfn.XLOOKUP(U$3, personalist!$A:$A, personalist!$C:$C, NA())</f>
@@ -1327,9 +1321,8 @@
         <f>_xlfn.XLOOKUP(W$3, personalist!$A:$A, personalist!$C:$C, NA())</f>
         <v>469</v>
       </c>
-      <c r="X2" s="9"/>
-    </row>
-    <row r="3" spans="1:25" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:23" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8" t="s">
         <v>2</v>
       </c>
@@ -1376,7 +1369,7 @@
         <v>19</v>
       </c>
       <c r="P3" s="8" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="Q3" s="8" t="s">
         <v>29</v>
@@ -1384,13 +1377,13 @@
       <c r="R3" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="S3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="T3" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="U3" s="8" t="s">
+      <c r="S3" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="T3" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" s="9" t="s">
         <v>30</v>
       </c>
       <c r="V3" s="8" t="s">
@@ -1399,14 +1392,8 @@
       <c r="W3" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="X3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="Y3" s="9" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
         <v>1</v>
       </c>
@@ -1444,7 +1431,7 @@
       <c r="V4" s="3"/>
       <c r="W4" s="3"/>
     </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="3">
         <v>2</v>
       </c>
@@ -1479,7 +1466,7 @@
       <c r="V5" s="3"/>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="3">
         <v>3</v>
       </c>
@@ -1512,7 +1499,7 @@
       <c r="V6" s="3"/>
       <c r="W6" s="3"/>
     </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="3">
         <v>4</v>
       </c>
@@ -1545,7 +1532,7 @@
       <c r="V7" s="3"/>
       <c r="W7" s="3"/>
     </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="3">
         <v>5</v>
       </c>
@@ -1578,7 +1565,7 @@
       <c r="V8" s="3"/>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="3">
         <v>6</v>
       </c>
@@ -1611,7 +1598,7 @@
       <c r="V9" s="3"/>
       <c r="W9" s="3"/>
     </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="3">
         <v>7</v>
       </c>
@@ -1650,7 +1637,7 @@
       <c r="V10" s="3"/>
       <c r="W10" s="3"/>
     </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="3">
         <v>8</v>
       </c>
@@ -1683,7 +1670,7 @@
       <c r="V11" s="3"/>
       <c r="W11" s="3"/>
     </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="3">
         <v>9</v>
       </c>
@@ -1716,7 +1703,7 @@
       <c r="V12" s="3"/>
       <c r="W12" s="3"/>
     </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="3">
         <v>10</v>
       </c>
@@ -1753,7 +1740,7 @@
       <c r="V13" s="3"/>
       <c r="W13" s="3"/>
     </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="3">
         <v>11</v>
       </c>
@@ -1788,7 +1775,7 @@
       <c r="V14" s="3"/>
       <c r="W14" s="3"/>
     </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="3">
         <v>12</v>
       </c>
@@ -1821,7 +1808,7 @@
       <c r="V15" s="3"/>
       <c r="W15" s="3"/>
     </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="3">
         <v>13</v>
       </c>
@@ -1860,7 +1847,7 @@
       <c r="V16" s="3"/>
       <c r="W16" s="3"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" s="3">
         <v>14</v>
       </c>
@@ -1899,7 +1886,7 @@
       <c r="V17" s="3"/>
       <c r="W17" s="3"/>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A18" s="3">
         <v>15</v>
       </c>
@@ -1940,7 +1927,7 @@
       <c r="V18" s="3"/>
       <c r="W18" s="3"/>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A19" s="3">
         <v>16</v>
       </c>
@@ -1981,7 +1968,7 @@
       <c r="V19" s="3"/>
       <c r="W19" s="3"/>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" s="3">
         <v>17</v>
       </c>
@@ -2022,7 +2009,7 @@
       <c r="V20" s="3"/>
       <c r="W20" s="3"/>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" s="3">
         <v>18</v>
       </c>
@@ -2063,7 +2050,7 @@
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
     </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" s="3">
         <v>19</v>
       </c>
@@ -2106,7 +2093,7 @@
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
     </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A23" s="3">
         <v>20</v>
       </c>
@@ -2149,7 +2136,7 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
     </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" s="3">
         <v>21</v>
       </c>
@@ -2196,7 +2183,7 @@
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
     </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" s="3">
         <v>22</v>
       </c>
@@ -2237,7 +2224,7 @@
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" s="3">
         <v>23</v>
       </c>
@@ -2282,7 +2269,7 @@
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
     </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="3">
         <v>24</v>
       </c>
@@ -2335,7 +2322,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3">
         <v>25</v>
       </c>
@@ -2382,7 +2369,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3">
         <v>26</v>
       </c>
@@ -2432,7 +2419,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3">
         <v>27</v>
       </c>
@@ -2473,7 +2460,7 @@
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" s="3">
         <v>28</v>
       </c>
@@ -2520,7 +2507,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3">
         <v>29</v>
       </c>
@@ -2567,7 +2554,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3">
         <v>30</v>
       </c>
@@ -2610,7 +2597,7 @@
       </c>
       <c r="W33" s="3"/>
     </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" s="3">
         <v>31</v>
       </c>
@@ -2651,7 +2638,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3">
         <v>32</v>
       </c>
@@ -2682,7 +2669,9 @@
       <c r="R35" s="3">
         <v>40</v>
       </c>
-      <c r="S35" s="3"/>
+      <c r="S35" s="3">
+        <v>32</v>
+      </c>
       <c r="T35" s="3"/>
       <c r="U35" s="3"/>
       <c r="V35" s="3">
@@ -2691,11 +2680,8 @@
       <c r="W35" s="3">
         <v>40</v>
       </c>
-      <c r="X35" s="2">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3">
         <v>33</v>
       </c>
@@ -2728,7 +2714,9 @@
       <c r="R36" s="3">
         <v>40</v>
       </c>
-      <c r="S36" s="3"/>
+      <c r="S36" s="3">
+        <v>40</v>
+      </c>
       <c r="T36" s="3"/>
       <c r="U36" s="3"/>
       <c r="V36" s="3">
@@ -2737,11 +2725,8 @@
       <c r="W36" s="3">
         <v>40</v>
       </c>
-      <c r="X36" s="2">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="3">
         <v>34</v>
       </c>
@@ -2778,7 +2763,7 @@
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
     </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A38" s="3">
         <v>35</v>
       </c>
@@ -2821,7 +2806,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3">
         <v>36</v>
       </c>
@@ -2866,7 +2851,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3">
         <v>37</v>
       </c>
@@ -2902,7 +2887,9 @@
         <v>40</v>
       </c>
       <c r="S40" s="3"/>
-      <c r="T40" s="3"/>
+      <c r="T40" s="3">
+        <v>40</v>
+      </c>
       <c r="U40" s="3"/>
       <c r="V40" s="3">
         <v>40</v>
@@ -2910,11 +2897,8 @@
       <c r="W40" s="3">
         <v>40</v>
       </c>
-      <c r="Y40">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="3">
         <v>38</v>
       </c>
@@ -2938,7 +2922,9 @@
       <c r="M41" s="3"/>
       <c r="N41" s="3"/>
       <c r="O41" s="3"/>
-      <c r="P41" s="3"/>
+      <c r="P41" s="3">
+        <v>24</v>
+      </c>
       <c r="Q41" s="3"/>
       <c r="R41" s="3"/>
       <c r="S41" s="3"/>
@@ -2947,7 +2933,7 @@
       <c r="V41" s="3"/>
       <c r="W41" s="3"/>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A42" s="3">
         <v>39</v>
       </c>
@@ -2971,8 +2957,12 @@
       <c r="M42" s="3"/>
       <c r="N42" s="3"/>
       <c r="O42" s="3"/>
-      <c r="P42" s="3"/>
-      <c r="Q42" s="3"/>
+      <c r="P42" s="3">
+        <v>8</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>8</v>
+      </c>
       <c r="R42" s="3"/>
       <c r="S42" s="3"/>
       <c r="T42" s="3"/>
@@ -2980,7 +2970,7 @@
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A43" s="3">
         <v>40</v>
       </c>
@@ -3000,20 +2990,30 @@
       <c r="I43" s="3"/>
       <c r="J43" s="3"/>
       <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
+      <c r="L43" s="3">
+        <v>32</v>
+      </c>
       <c r="M43" s="3"/>
       <c r="N43" s="3"/>
       <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-      <c r="Q43" s="3"/>
+      <c r="P43" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>40</v>
+      </c>
       <c r="R43" s="3"/>
-      <c r="S43" s="3"/>
+      <c r="S43" s="3">
+        <v>32</v>
+      </c>
       <c r="T43" s="3"/>
-      <c r="U43" s="3"/>
+      <c r="U43" s="3">
+        <v>32</v>
+      </c>
       <c r="V43" s="3"/>
       <c r="W43" s="3"/>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A44" s="3">
         <v>41</v>
       </c>
@@ -3046,7 +3046,7 @@
       <c r="V44" s="3"/>
       <c r="W44" s="3"/>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A45" s="3">
         <v>42</v>
       </c>
@@ -3079,7 +3079,7 @@
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A46" s="3">
         <v>43</v>
       </c>
@@ -3112,7 +3112,7 @@
       <c r="V46" s="3"/>
       <c r="W46" s="3"/>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A47" s="3">
         <v>44</v>
       </c>
@@ -3145,7 +3145,7 @@
       <c r="V47" s="3"/>
       <c r="W47" s="3"/>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A48" s="3">
         <v>45</v>
       </c>
@@ -3178,7 +3178,7 @@
       <c r="V48" s="3"/>
       <c r="W48" s="3"/>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A49" s="3">
         <v>46</v>
       </c>
@@ -3211,7 +3211,7 @@
       <c r="V49" s="3"/>
       <c r="W49" s="3"/>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A50" s="3">
         <v>47</v>
       </c>
@@ -3244,7 +3244,7 @@
       <c r="V50" s="3"/>
       <c r="W50" s="3"/>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A51" s="3">
         <v>48</v>
       </c>
@@ -3277,7 +3277,7 @@
       <c r="V51" s="3"/>
       <c r="W51" s="3"/>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A52" s="3">
         <v>49</v>
       </c>
@@ -3310,7 +3310,7 @@
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A53" s="3">
         <v>50</v>
       </c>
@@ -3343,7 +3343,7 @@
       <c r="V53" s="3"/>
       <c r="W53" s="3"/>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A54" s="3">
         <v>51</v>
       </c>
@@ -3356,7 +3356,7 @@
         <v>46110</v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A55" s="3">
         <v>52</v>
       </c>
@@ -3369,7 +3369,7 @@
         <v>46117</v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A56" s="3">
         <v>53</v>
       </c>
@@ -3382,7 +3382,7 @@
         <v>46124</v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A57" s="3">
         <v>54</v>
       </c>
@@ -3395,7 +3395,7 @@
         <v>46131</v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A58" s="3">
         <v>55</v>
       </c>
@@ -3408,7 +3408,7 @@
         <v>46138</v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A59" s="3">
         <v>56</v>
       </c>
@@ -3421,7 +3421,7 @@
         <v>46145</v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A60" s="3">
         <v>57</v>
       </c>
@@ -3434,7 +3434,7 @@
         <v>46152</v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A61" s="3">
         <v>58</v>
       </c>
@@ -3447,7 +3447,7 @@
         <v>46159</v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A62" s="3">
         <v>59</v>
       </c>
@@ -3460,7 +3460,7 @@
         <v>46166</v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A63" s="3">
         <v>60</v>
       </c>
@@ -3473,7 +3473,7 @@
         <v>46173</v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A64" s="3">
         <v>61</v>
       </c>
@@ -3486,7 +3486,7 @@
         <v>46180</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A65" s="3">
         <v>62</v>
       </c>
@@ -3499,7 +3499,7 @@
         <v>46187</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A66" s="3">
         <v>63</v>
       </c>
@@ -3512,7 +3512,7 @@
         <v>46194</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A67" s="3">
         <v>64</v>
       </c>
@@ -3525,7 +3525,7 @@
         <v>46201</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A68" s="3">
         <v>65</v>
       </c>
@@ -3538,7 +3538,7 @@
         <v>46208</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A69" s="3">
         <v>66</v>
       </c>
@@ -3551,7 +3551,7 @@
         <v>46215</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A70" s="3">
         <v>67</v>
       </c>
@@ -3564,7 +3564,7 @@
         <v>46222</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A71" s="3">
         <v>68</v>
       </c>
@@ -3586,7 +3586,7 @@
           <x14:formula1>
             <xm:f>personalist!$A$2:$A$159</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:W3</xm:sqref>
+          <xm:sqref>D3:R3 V3:W3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3602,13 +3602,13 @@
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="2" max="3" width="8.88671875" style="11"/>
-    <col min="14" max="14" width="9.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="8.89453125" style="11"/>
+    <col min="14" max="14" width="9.68359375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="str">
         <f>'weekly hours'!A1</f>
         <v>position</v>
@@ -3677,7 +3677,7 @@
       </c>
       <c r="S1" t="str">
         <f>'weekly hours'!T1</f>
-        <v>Technician II</v>
+        <v>Engineer/supervisor</v>
       </c>
       <c r="T1" t="str">
         <f>'weekly hours'!U1</f>
@@ -3693,13 +3693,13 @@
       </c>
       <c r="W1" t="str">
         <f>'weekly hours'!S1</f>
-        <v>Technician II</v>
+        <v>Engineer/supervisor</v>
       </c>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
       <c r="Z1" s="1"/>
     </row>
-    <row r="2" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:26" s="13" customFormat="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="13" t="str">
         <f>'weekly hours'!A2</f>
         <v>Salary $/day</v>
@@ -3766,7 +3766,7 @@
       </c>
       <c r="S2" s="13">
         <f>'weekly hours'!T2</f>
-        <v>456</v>
+        <v>536</v>
       </c>
       <c r="T2" s="13">
         <f>'weekly hours'!U2</f>
@@ -3782,10 +3782,10 @@
       </c>
       <c r="W2" s="13">
         <f>'weekly hours'!S2</f>
-        <v>456</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.3">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="str">
         <f>'weekly hours'!A3</f>
         <v>Week #</v>
@@ -3860,7 +3860,7 @@
       </c>
       <c r="S3" t="str">
         <f>'weekly hours'!T3</f>
-        <v>Angie G</v>
+        <v xml:space="preserve">Tony M </v>
       </c>
       <c r="T3" t="str">
         <f>'weekly hours'!U3</f>
@@ -3876,10 +3876,10 @@
       </c>
       <c r="W3" t="str">
         <f>'weekly hours'!S3</f>
-        <v>Robert W</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.3">
+        <v>Vu T</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A4">
         <f>'weekly hours'!A4</f>
         <v>1</v>
@@ -3973,7 +3973,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
         <f>'weekly hours'!A5</f>
         <v>2</v>
@@ -4067,7 +4067,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
         <f>'weekly hours'!A6</f>
         <v>3</v>
@@ -4161,7 +4161,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
         <f>'weekly hours'!A7</f>
         <v>4</v>
@@ -4255,7 +4255,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
         <f>'weekly hours'!A8</f>
         <v>5</v>
@@ -4349,7 +4349,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="9" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
         <f>'weekly hours'!A9</f>
         <v>6</v>
@@ -4443,7 +4443,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="10" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
         <f>'weekly hours'!A10</f>
         <v>7</v>
@@ -4537,7 +4537,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="11" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
         <f>'weekly hours'!A11</f>
         <v>8</v>
@@ -4631,7 +4631,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="12" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
         <f>'weekly hours'!A12</f>
         <v>9</v>
@@ -4725,7 +4725,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="13" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
         <f>'weekly hours'!A13</f>
         <v>10</v>
@@ -4819,7 +4819,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="14" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
         <f>'weekly hours'!A14</f>
         <v>11</v>
@@ -4913,7 +4913,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="15" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
         <f>'weekly hours'!A15</f>
         <v>12</v>
@@ -5007,7 +5007,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="16" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
         <f>'weekly hours'!A16</f>
         <v>13</v>
@@ -5101,7 +5101,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
         <f>'weekly hours'!A17</f>
         <v>14</v>
@@ -5195,7 +5195,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="18" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
         <f>'weekly hours'!A18</f>
         <v>15</v>
@@ -5289,7 +5289,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="19" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
         <f>'weekly hours'!A19</f>
         <v>16</v>
@@ -5383,7 +5383,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="20" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
         <f>'weekly hours'!A20</f>
         <v>17</v>
@@ -5477,7 +5477,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="21" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
         <f>'weekly hours'!A21</f>
         <v>18</v>
@@ -5568,10 +5568,10 @@
       </c>
       <c r="W21" s="1">
         <f>IF('weekly hours'!S21=0," ",'weekly hours'!S21/8*'weekly hours'!S$2)</f>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="22" spans="1:23" x14ac:dyDescent="0.3">
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
         <f>'weekly hours'!A22</f>
         <v>19</v>
@@ -5662,10 +5662,10 @@
       </c>
       <c r="W22" s="1">
         <f>IF('weekly hours'!S22=0," ",'weekly hours'!S22/8*'weekly hours'!S$2)</f>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="23" spans="1:23" x14ac:dyDescent="0.3">
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
         <f>'weekly hours'!A23</f>
         <v>20</v>
@@ -5756,10 +5756,10 @@
       </c>
       <c r="W23" s="1">
         <f>IF('weekly hours'!S23=0," ",'weekly hours'!S23/8*'weekly hours'!S$2)</f>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="24" spans="1:23" x14ac:dyDescent="0.3">
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
         <f>'weekly hours'!A24</f>
         <v>21</v>
@@ -5850,10 +5850,10 @@
       </c>
       <c r="W24" s="1">
         <f>IF('weekly hours'!S24=0," ",'weekly hours'!S24/8*'weekly hours'!S$2)</f>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="25" spans="1:23" x14ac:dyDescent="0.3">
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
         <f>'weekly hours'!A25</f>
         <v>22</v>
@@ -5944,10 +5944,10 @@
       </c>
       <c r="W25" s="1">
         <f>IF('weekly hours'!S25=0," ",'weekly hours'!S25/8*'weekly hours'!S$2)</f>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.3">
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
         <f>'weekly hours'!A26</f>
         <v>23</v>
@@ -6038,10 +6038,10 @@
       </c>
       <c r="W26" s="1">
         <f>IF('weekly hours'!S26=0," ",'weekly hours'!S26/8*'weekly hours'!S$2)</f>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="27" spans="1:23" x14ac:dyDescent="0.3">
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
         <f>'weekly hours'!A27</f>
         <v>24</v>
@@ -6132,10 +6132,10 @@
       </c>
       <c r="W27" s="1">
         <f>IF('weekly hours'!S27=0," ",'weekly hours'!S27/8*'weekly hours'!S$2)</f>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="28" spans="1:23" x14ac:dyDescent="0.3">
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
         <f>'weekly hours'!A28</f>
         <v>25</v>
@@ -6229,7 +6229,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="29" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
         <f>'weekly hours'!A29</f>
         <v>26</v>
@@ -6320,10 +6320,10 @@
       </c>
       <c r="W29" s="1">
         <f>IF('weekly hours'!S29=0," ",'weekly hours'!S29/8*'weekly hours'!S$2)</f>
-        <v>2280</v>
-      </c>
-    </row>
-    <row r="30" spans="1:23" x14ac:dyDescent="0.3">
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
         <f>'weekly hours'!A30</f>
         <v>27</v>
@@ -6417,7 +6417,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="31" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
         <f>'weekly hours'!A31</f>
         <v>28</v>
@@ -6511,7 +6511,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="32" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
         <f>'weekly hours'!A32</f>
         <v>29</v>
@@ -6605,7 +6605,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
         <f>'weekly hours'!A33</f>
         <v>30</v>
@@ -6699,7 +6699,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
         <f>'weekly hours'!A34</f>
         <v>31</v>
@@ -6793,7 +6793,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
         <f>'weekly hours'!A35</f>
         <v>32</v>
@@ -6882,12 +6882,12 @@
         <f>IF('weekly hours'!W35=0," ",'weekly hours'!W35/8*'weekly hours'!W$2)</f>
         <v>2345</v>
       </c>
-      <c r="W35" s="1" t="str">
+      <c r="W35" s="1">
         <f>IF('weekly hours'!S35=0," ",'weekly hours'!S35/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.3">
+        <v>2144</v>
+      </c>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
         <f>'weekly hours'!A36</f>
         <v>33</v>
@@ -6976,12 +6976,12 @@
         <f>IF('weekly hours'!W36=0," ",'weekly hours'!W36/8*'weekly hours'!W$2)</f>
         <v>2345</v>
       </c>
-      <c r="W36" s="1" t="str">
+      <c r="W36" s="1">
         <f>IF('weekly hours'!S36=0," ",'weekly hours'!S36/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.3">
+        <v>2680</v>
+      </c>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
         <f>'weekly hours'!A37</f>
         <v>34</v>
@@ -7075,7 +7075,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
         <f>'weekly hours'!A38</f>
         <v>35</v>
@@ -7169,7 +7169,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
         <f>'weekly hours'!A39</f>
         <v>36</v>
@@ -7263,7 +7263,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
         <f>'weekly hours'!A40</f>
         <v>37</v>
@@ -7336,9 +7336,9 @@
         <f>IF('weekly hours'!R40=0," ",'weekly hours'!R40/8*'weekly hours'!R$2)</f>
         <v>2345</v>
       </c>
-      <c r="S40" s="1" t="str">
+      <c r="S40" s="1">
         <f>IF('weekly hours'!T40=0," ",'weekly hours'!T40/8*'weekly hours'!T$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2680</v>
       </c>
       <c r="T40" s="1" t="str">
         <f>IF('weekly hours'!U40=0," ",'weekly hours'!U40/8*'weekly hours'!U$2)</f>
@@ -7357,7 +7357,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
         <f>'weekly hours'!A41</f>
         <v>38</v>
@@ -7418,9 +7418,9 @@
         <f>IF('weekly hours'!O41=0," ",'weekly hours'!O41/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P41" s="1" t="str">
+      <c r="P41" s="1">
         <f>IF('weekly hours'!P41=0," ",'weekly hours'!P41/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>1608</v>
       </c>
       <c r="Q41" s="1" t="str">
         <f>IF('weekly hours'!Q41=0," ",'weekly hours'!Q41/8*'weekly hours'!Q$2)</f>
@@ -7451,7 +7451,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
         <f>'weekly hours'!A42</f>
         <v>39</v>
@@ -7512,13 +7512,13 @@
         <f>IF('weekly hours'!O42=0," ",'weekly hours'!O42/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P42" s="1" t="str">
+      <c r="P42" s="1">
         <f>IF('weekly hours'!P42=0," ",'weekly hours'!P42/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q42" s="1" t="str">
+        <v>536</v>
+      </c>
+      <c r="Q42" s="1">
         <f>IF('weekly hours'!Q42=0," ",'weekly hours'!Q42/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>456</v>
       </c>
       <c r="R42" s="1" t="str">
         <f>IF('weekly hours'!R42=0," ",'weekly hours'!R42/8*'weekly hours'!R$2)</f>
@@ -7545,7 +7545,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
         <f>'weekly hours'!A43</f>
         <v>40</v>
@@ -7590,9 +7590,9 @@
         <f>IF('weekly hours'!K43=0," ",'weekly hours'!K43/8*'weekly hours'!K$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="L43" s="1" t="str">
+      <c r="L43" s="1">
         <f>IF('weekly hours'!L43=0," ",'weekly hours'!L43/8*'weekly hours'!L$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2684</v>
       </c>
       <c r="M43" s="1" t="str">
         <f>IF('weekly hours'!M43=0," ",'weekly hours'!M43/8*'weekly hours'!M$2)</f>
@@ -7606,13 +7606,13 @@
         <f>IF('weekly hours'!O43=0," ",'weekly hours'!O43/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P43" s="1" t="str">
+      <c r="P43" s="1">
         <f>IF('weekly hours'!P43=0," ",'weekly hours'!P43/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q43" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q43" s="1">
         <f>IF('weekly hours'!Q43=0," ",'weekly hours'!Q43/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2280</v>
       </c>
       <c r="R43" s="1" t="str">
         <f>IF('weekly hours'!R43=0," ",'weekly hours'!R43/8*'weekly hours'!R$2)</f>
@@ -7622,9 +7622,9 @@
         <f>IF('weekly hours'!T43=0," ",'weekly hours'!T43/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T43" s="1" t="str">
+      <c r="T43" s="1">
         <f>IF('weekly hours'!U43=0," ",'weekly hours'!U43/8*'weekly hours'!U$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>1876</v>
       </c>
       <c r="U43" s="1" t="str">
         <f>IF('weekly hours'!V43=0," ",'weekly hours'!V43/8*'weekly hours'!V$2)</f>
@@ -7634,12 +7634,12 @@
         <f>IF('weekly hours'!W43=0," ",'weekly hours'!W43/8*'weekly hours'!W$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="W43" s="1" t="str">
+      <c r="W43" s="1">
         <f>IF('weekly hours'!S43=0," ",'weekly hours'!S43/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.3">
+        <v>2144</v>
+      </c>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
         <f>'weekly hours'!A44</f>
         <v>41</v>
@@ -7733,7 +7733,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
         <f>'weekly hours'!A45</f>
         <v>42</v>
@@ -7827,7 +7827,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
         <f>'weekly hours'!A46</f>
         <v>43</v>
@@ -7921,7 +7921,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
         <f>'weekly hours'!A47</f>
         <v>44</v>
@@ -8015,7 +8015,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
         <f>'weekly hours'!A48</f>
         <v>45</v>
@@ -8109,7 +8109,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="49" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
         <f>'weekly hours'!A49</f>
         <v>46</v>
@@ -8203,7 +8203,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="50" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
         <f>'weekly hours'!A50</f>
         <v>47</v>
@@ -8297,7 +8297,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="51" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
         <f>'weekly hours'!A51</f>
         <v>48</v>
@@ -8391,7 +8391,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="52" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
         <f>'weekly hours'!A52</f>
         <v>49</v>
@@ -8485,7 +8485,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="53" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
         <f>'weekly hours'!A53</f>
         <v>50</v>
@@ -8579,7 +8579,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="54" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
         <f>'weekly hours'!A54</f>
         <v>51</v>
@@ -8673,7 +8673,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="55" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
         <f>'weekly hours'!A55</f>
         <v>52</v>
@@ -8767,7 +8767,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="56" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
         <f>'weekly hours'!A56</f>
         <v>53</v>
@@ -8861,7 +8861,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="57" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
         <f>'weekly hours'!A57</f>
         <v>54</v>
@@ -8955,7 +8955,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="58" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
         <f>'weekly hours'!A58</f>
         <v>55</v>
@@ -9049,7 +9049,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="59" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
         <f>'weekly hours'!A59</f>
         <v>56</v>
@@ -9143,7 +9143,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="60" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
         <f>'weekly hours'!A60</f>
         <v>57</v>
@@ -9237,7 +9237,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="61" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
         <f>'weekly hours'!A61</f>
         <v>58</v>
@@ -9331,7 +9331,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="62" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
         <f>'weekly hours'!A62</f>
         <v>59</v>
@@ -9425,7 +9425,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="63" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
         <f>'weekly hours'!A63</f>
         <v>60</v>
@@ -9519,7 +9519,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="64" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
         <f>'weekly hours'!A64</f>
         <v>61</v>
@@ -9613,7 +9613,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="65" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
         <f>'weekly hours'!A65</f>
         <v>62</v>
@@ -9707,7 +9707,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="66" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
         <f>'weekly hours'!A66</f>
         <v>63</v>
@@ -9801,7 +9801,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="67" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
         <f>'weekly hours'!A67</f>
         <v>64</v>
@@ -9895,7 +9895,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="68" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
         <f>'weekly hours'!A68</f>
         <v>65</v>
@@ -9989,7 +9989,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="69" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
         <f>'weekly hours'!A69</f>
         <v>66</v>
@@ -10083,7 +10083,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="70" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
         <f>'weekly hours'!A70</f>
         <v>67</v>
@@ -10177,7 +10177,7 @@
         <v xml:space="preserve"> </v>
       </c>
     </row>
-    <row r="71" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
         <f>'weekly hours'!A71</f>
         <v>68</v>

</xml_diff>

<commit_message>
Update web reports - 2026-01-29 22:41:12
</commit_message>
<xml_diff>
--- a/labor_hour_summary.xlsx
+++ b/labor_hour_summary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29628"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\xiaos\Downloads\budget analysis\pythonProject-ohio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Shared drives\GEO Inc\Projects\Current\2025 Ohio Medproperties - CEC\Schedule - MS project\project tracker tool\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CD803C3-1A6A-42B8-99C6-5828AF002743}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{596803A8-B5E7-49F0-8D91-59E721A30756}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12675" yWindow="-18120" windowWidth="29040" windowHeight="17520" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13872" activeTab="1" xr2:uid="{ACB5E1F2-877B-4160-8533-688241076336}"/>
   </bookViews>
   <sheets>
     <sheet name="personalist" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="49">
   <si>
     <t>Jason C</t>
   </si>
@@ -65,9 +65,6 @@
   </si>
   <si>
     <t>Luis Z</t>
-  </si>
-  <si>
-    <t>Roy Z</t>
   </si>
   <si>
     <t>Brian K</t>
@@ -185,6 +182,9 @@
   </si>
   <si>
     <t xml:space="preserve">Tony M </t>
+  </si>
+  <si>
+    <t>Alsa G</t>
   </si>
 </sst>
 </file>
@@ -646,8 +646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B73E7749-6E67-46D7-9EAD-69069F7CE8A5}">
   <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E31" sqref="E31"/>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -663,46 +663,46 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C2" s="1">
         <f>VLOOKUP(B2, $D$3:$E$9, 2, FALSE)</f>
         <v>671</v>
       </c>
       <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
         <v>44</v>
-      </c>
-      <c r="E2" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1">
         <f t="shared" ref="C3:C34" si="0">VLOOKUP(B3, $D$3:$E$9, 2, FALSE)</f>
         <v>671</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E3" s="6">
         <v>295</v>
@@ -710,17 +710,17 @@
     </row>
     <row r="4" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C4" s="1">
         <f t="shared" si="0"/>
         <v>536</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E4" s="6">
         <v>456</v>
@@ -728,17 +728,17 @@
     </row>
     <row r="5" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C5" s="1">
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="E5" s="6">
         <v>469</v>
@@ -746,17 +746,17 @@
     </row>
     <row r="6" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C6" s="1">
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E6" s="6">
         <v>536</v>
@@ -764,17 +764,17 @@
     </row>
     <row r="7" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1">
         <f t="shared" si="0"/>
         <v>671</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E7" s="7">
         <v>671</v>
@@ -782,17 +782,17 @@
     </row>
     <row r="8" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1">
         <f t="shared" si="0"/>
         <v>536</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E8" s="6">
         <v>536</v>
@@ -800,17 +800,17 @@
     </row>
     <row r="9" spans="1:5" ht="18.600000000000001" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C9" s="1">
         <f t="shared" si="0"/>
         <v>456</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E9" s="7">
         <v>671</v>
@@ -821,7 +821,7 @@
         <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1">
         <f t="shared" si="0"/>
@@ -830,10 +830,10 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" s="1">
         <f t="shared" si="0"/>
@@ -842,10 +842,10 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B12" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1">
         <f t="shared" si="0"/>
@@ -854,10 +854,10 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C13" s="1">
         <f t="shared" si="0"/>
@@ -869,7 +869,7 @@
         <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C14" s="1">
         <f t="shared" si="0"/>
@@ -878,10 +878,10 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C15" s="1">
         <f t="shared" si="0"/>
@@ -890,10 +890,10 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B16" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C16" s="1">
         <f t="shared" si="0"/>
@@ -902,10 +902,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C17" s="1">
         <f t="shared" si="0"/>
@@ -917,7 +917,7 @@
         <v>6</v>
       </c>
       <c r="B18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C18" s="1">
         <f t="shared" si="0"/>
@@ -929,7 +929,7 @@
         <v>0</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C19" s="1">
         <f t="shared" si="0"/>
@@ -938,10 +938,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A20" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C20" s="1">
         <f t="shared" si="0"/>
@@ -950,10 +950,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C21" s="1">
         <f t="shared" si="0"/>
@@ -962,10 +962,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A22" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C22" s="1">
         <f t="shared" si="0"/>
@@ -977,7 +977,7 @@
         <v>8</v>
       </c>
       <c r="B23" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C23" s="1">
         <f t="shared" si="0"/>
@@ -986,10 +986,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A24" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B24" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C24" s="1">
         <f t="shared" si="0"/>
@@ -998,10 +998,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A25" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C25" s="1">
         <f t="shared" si="0"/>
@@ -1010,10 +1010,10 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C26" s="1">
         <f t="shared" si="0"/>
@@ -1022,10 +1022,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A27" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C27" s="1">
         <f t="shared" si="0"/>
@@ -1034,10 +1034,10 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" t="s">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="B28" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C28" s="1">
         <f t="shared" si="0"/>
@@ -1046,10 +1046,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B29" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C29" s="1">
         <f t="shared" si="0"/>
@@ -1058,10 +1058,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B30" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C30" s="1">
         <f t="shared" si="0"/>
@@ -1070,10 +1070,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A31" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B31" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C31" s="1">
         <f t="shared" si="0"/>
@@ -1082,10 +1082,10 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32" s="1">
         <f t="shared" si="0"/>
@@ -1094,10 +1094,10 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" s="1">
         <f t="shared" si="0"/>
@@ -1106,10 +1106,10 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.55000000000000004">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B34" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C34" s="1">
         <f t="shared" si="0"/>
@@ -1134,10 +1134,10 @@
   <dimension ref="A1:W71"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="3" ySplit="3" topLeftCell="D31" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="3" topLeftCell="G35" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="X1" sqref="X1:Z1048576"/>
+      <selection pane="bottomRight" activeCell="W1" sqref="W1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -1145,12 +1145,14 @@
     <col min="1" max="1" width="10.1015625" style="2" customWidth="1"/>
     <col min="2" max="2" width="12.68359375" style="2" customWidth="1"/>
     <col min="3" max="3" width="13.3125" style="2" customWidth="1"/>
-    <col min="4" max="23" width="8.89453125" style="2"/>
+    <col min="4" max="14" width="8.89453125" style="2"/>
+    <col min="15" max="15" width="8.83984375" style="2"/>
+    <col min="16" max="23" width="8.89453125" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:23" s="10" customFormat="1" ht="62.7" customHeight="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="8"/>
       <c r="C1" s="8"/>
@@ -1200,7 +1202,7 @@
       </c>
       <c r="O1" s="8" t="str">
         <f>_xlfn.XLOOKUP(O$3, personalist!$A:$A, personalist!$B:$B, NA())</f>
-        <v>Engineer/supervisor</v>
+        <v>Welder</v>
       </c>
       <c r="P1" s="8" t="str">
         <f>_xlfn.XLOOKUP(P$3, personalist!$A:$A, personalist!$B:$B, NA())</f>
@@ -1230,14 +1232,11 @@
         <f>_xlfn.XLOOKUP(V$3, personalist!$A:$A, personalist!$B:$B, NA())</f>
         <v>Welder</v>
       </c>
-      <c r="W1" s="8" t="str">
-        <f>_xlfn.XLOOKUP(W$3, personalist!$A:$A, personalist!$B:$B, NA())</f>
-        <v>Welder</v>
-      </c>
+      <c r="W1" s="8"/>
     </row>
     <row r="2" spans="1:23" s="10" customFormat="1" ht="28.8" hidden="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B2" s="8"/>
       <c r="C2" s="8"/>
@@ -1287,7 +1286,7 @@
       </c>
       <c r="O2" s="12">
         <f>_xlfn.XLOOKUP(O$3, personalist!$A:$A, personalist!$C:$C, NA())</f>
-        <v>536</v>
+        <v>469</v>
       </c>
       <c r="P2" s="12">
         <f>_xlfn.XLOOKUP(P$3, personalist!$A:$A, personalist!$C:$C, NA())</f>
@@ -1317,10 +1316,7 @@
         <f>_xlfn.XLOOKUP(V$3, personalist!$A:$A, personalist!$C:$C, NA())</f>
         <v>469</v>
       </c>
-      <c r="W2" s="12">
-        <f>_xlfn.XLOOKUP(W$3, personalist!$A:$A, personalist!$C:$C, NA())</f>
-        <v>469</v>
-      </c>
+      <c r="W2" s="12"/>
     </row>
     <row r="3" spans="1:23" s="10" customFormat="1" ht="28.8" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="8" t="s">
@@ -1339,7 +1335,7 @@
         <v>6</v>
       </c>
       <c r="F3" s="8" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="G3" s="8" t="s">
         <v>0</v>
@@ -1351,47 +1347,45 @@
         <v>8</v>
       </c>
       <c r="J3" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L3" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="M3" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="L3" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="M3" s="8" t="s">
-        <v>22</v>
-      </c>
       <c r="N3" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q3" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="R3" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="S3" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="O3" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="P3" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="Q3" s="8" t="s">
+      <c r="T3" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="U3" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="R3" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="S3" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="T3" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="U3" s="9" t="s">
+      <c r="V3" s="8" t="s">
         <v>30</v>
       </c>
-      <c r="V3" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="W3" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="W3" s="8"/>
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="3">
@@ -2300,7 +2294,9 @@
         <v>40</v>
       </c>
       <c r="N27" s="3"/>
-      <c r="O27" s="3"/>
+      <c r="O27" s="3">
+        <v>40</v>
+      </c>
       <c r="P27" s="3">
         <v>40</v>
       </c>
@@ -2318,9 +2314,7 @@
       <c r="V27" s="3">
         <v>40</v>
       </c>
-      <c r="W27" s="3">
-        <v>40</v>
-      </c>
+      <c r="W27" s="3"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A28" s="3">
@@ -2349,7 +2343,9 @@
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
       <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
+      <c r="O28" s="3">
+        <v>40</v>
+      </c>
       <c r="P28" s="3">
         <v>40</v>
       </c>
@@ -2365,9 +2361,7 @@
       <c r="V28" s="3">
         <v>16</v>
       </c>
-      <c r="W28" s="3">
-        <v>40</v>
-      </c>
+      <c r="W28" s="3"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A29" s="3">
@@ -2396,7 +2390,9 @@
       <c r="L29" s="3"/>
       <c r="M29" s="3"/>
       <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
+      <c r="O29" s="3">
+        <v>24</v>
+      </c>
       <c r="P29" s="3">
         <v>40</v>
       </c>
@@ -2415,9 +2411,7 @@
         <f>40-16</f>
         <v>24</v>
       </c>
-      <c r="W29" s="3">
-        <v>24</v>
-      </c>
+      <c r="W29" s="3"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A30" s="3">
@@ -2489,7 +2483,9 @@
       <c r="L31" s="3"/>
       <c r="M31" s="3"/>
       <c r="N31" s="3"/>
-      <c r="O31" s="3"/>
+      <c r="O31" s="3">
+        <v>40</v>
+      </c>
       <c r="P31" s="3">
         <v>40</v>
       </c>
@@ -2503,9 +2499,7 @@
       <c r="V31" s="3">
         <v>40</v>
       </c>
-      <c r="W31" s="3">
-        <v>40</v>
-      </c>
+      <c r="W31" s="3"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A32" s="3">
@@ -2534,7 +2528,9 @@
       </c>
       <c r="M32" s="3"/>
       <c r="N32" s="3"/>
-      <c r="O32" s="3"/>
+      <c r="O32" s="3">
+        <v>40</v>
+      </c>
       <c r="P32" s="3">
         <v>40</v>
       </c>
@@ -2550,9 +2546,7 @@
       <c r="V32" s="3">
         <v>40</v>
       </c>
-      <c r="W32" s="3">
-        <v>40</v>
-      </c>
+      <c r="W32" s="3"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A33" s="3">
@@ -2622,7 +2616,9 @@
       <c r="L34" s="3"/>
       <c r="M34" s="3"/>
       <c r="N34" s="3"/>
-      <c r="O34" s="3"/>
+      <c r="O34" s="3">
+        <v>8</v>
+      </c>
       <c r="P34" s="3">
         <v>40</v>
       </c>
@@ -2634,9 +2630,7 @@
       <c r="T34" s="3"/>
       <c r="U34" s="3"/>
       <c r="V34" s="3"/>
-      <c r="W34" s="3">
-        <v>8</v>
-      </c>
+      <c r="W34" s="3"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A35" s="3">
@@ -2663,7 +2657,9 @@
       <c r="L35" s="3"/>
       <c r="M35" s="3"/>
       <c r="N35" s="3"/>
-      <c r="O35" s="3"/>
+      <c r="O35" s="3">
+        <v>40</v>
+      </c>
       <c r="P35" s="3"/>
       <c r="Q35" s="3"/>
       <c r="R35" s="3">
@@ -2677,9 +2673,7 @@
       <c r="V35" s="3">
         <v>40</v>
       </c>
-      <c r="W35" s="3">
-        <v>40</v>
-      </c>
+      <c r="W35" s="3"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A36" s="3">
@@ -2708,7 +2702,9 @@
       <c r="L36" s="3"/>
       <c r="M36" s="3"/>
       <c r="N36" s="3"/>
-      <c r="O36" s="3"/>
+      <c r="O36" s="3">
+        <v>40</v>
+      </c>
       <c r="P36" s="3"/>
       <c r="Q36" s="3"/>
       <c r="R36" s="3">
@@ -2722,9 +2718,7 @@
       <c r="V36" s="3">
         <v>40</v>
       </c>
-      <c r="W36" s="3">
-        <v>40</v>
-      </c>
+      <c r="W36" s="3"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A37" s="3">
@@ -2788,7 +2782,9 @@
       <c r="L38" s="3"/>
       <c r="M38" s="3"/>
       <c r="N38" s="3"/>
-      <c r="O38" s="3"/>
+      <c r="O38" s="3">
+        <v>40</v>
+      </c>
       <c r="P38" s="3">
         <v>40</v>
       </c>
@@ -2802,9 +2798,7 @@
       <c r="T38" s="3"/>
       <c r="U38" s="3"/>
       <c r="V38" s="3"/>
-      <c r="W38" s="3">
-        <v>40</v>
-      </c>
+      <c r="W38" s="3"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A39" s="3">
@@ -2831,7 +2825,9 @@
       </c>
       <c r="M39" s="3"/>
       <c r="N39" s="3"/>
-      <c r="O39" s="3"/>
+      <c r="O39" s="3">
+        <v>40</v>
+      </c>
       <c r="P39" s="3">
         <v>40</v>
       </c>
@@ -2847,9 +2843,7 @@
       <c r="V39" s="3">
         <v>40</v>
       </c>
-      <c r="W39" s="3">
-        <v>40</v>
-      </c>
+      <c r="W39" s="3"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A40" s="3">
@@ -2876,7 +2870,9 @@
       </c>
       <c r="M40" s="3"/>
       <c r="N40" s="3"/>
-      <c r="O40" s="3"/>
+      <c r="O40" s="3">
+        <v>40</v>
+      </c>
       <c r="P40" s="3">
         <v>40</v>
       </c>
@@ -2894,9 +2890,7 @@
       <c r="V40" s="3">
         <v>40</v>
       </c>
-      <c r="W40" s="3">
-        <v>40</v>
-      </c>
+      <c r="W40" s="3"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A41" s="3">
@@ -3033,16 +3027,26 @@
       <c r="I44" s="3"/>
       <c r="J44" s="3"/>
       <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
+      <c r="L44" s="3">
+        <v>40</v>
+      </c>
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
+      <c r="P44" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>40</v>
+      </c>
       <c r="R44" s="3"/>
       <c r="S44" s="3"/>
-      <c r="T44" s="3"/>
-      <c r="U44" s="3"/>
+      <c r="T44" s="3">
+        <v>24</v>
+      </c>
+      <c r="U44" s="3">
+        <v>24</v>
+      </c>
       <c r="V44" s="3"/>
       <c r="W44" s="3"/>
     </row>
@@ -3066,15 +3070,23 @@
       <c r="I45" s="3"/>
       <c r="J45" s="3"/>
       <c r="K45" s="3"/>
-      <c r="L45" s="3"/>
+      <c r="L45" s="3">
+        <v>40</v>
+      </c>
       <c r="M45" s="3"/>
       <c r="N45" s="3"/>
       <c r="O45" s="3"/>
-      <c r="P45" s="3"/>
-      <c r="Q45" s="3"/>
+      <c r="P45" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q45" s="3">
+        <v>40</v>
+      </c>
       <c r="R45" s="3"/>
       <c r="S45" s="3"/>
-      <c r="T45" s="3"/>
+      <c r="T45" s="3">
+        <v>40</v>
+      </c>
       <c r="U45" s="3"/>
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
@@ -3095,19 +3107,31 @@
       <c r="E46" s="3"/>
       <c r="F46" s="3"/>
       <c r="G46" s="3"/>
-      <c r="H46" s="3"/>
-      <c r="I46" s="3"/>
+      <c r="H46" s="3">
+        <v>4</v>
+      </c>
+      <c r="I46" s="3">
+        <v>1</v>
+      </c>
       <c r="J46" s="3"/>
       <c r="K46" s="3"/>
-      <c r="L46" s="3"/>
+      <c r="L46" s="3">
+        <v>40</v>
+      </c>
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
-      <c r="P46" s="3"/>
-      <c r="Q46" s="3"/>
+      <c r="P46" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q46" s="3">
+        <v>40</v>
+      </c>
       <c r="R46" s="3"/>
       <c r="S46" s="3"/>
-      <c r="T46" s="3"/>
+      <c r="T46" s="3">
+        <v>40</v>
+      </c>
       <c r="U46" s="3"/>
       <c r="V46" s="3"/>
       <c r="W46" s="3"/>
@@ -3586,7 +3610,7 @@
           <x14:formula1>
             <xm:f>personalist!$A$2:$A$159</xm:f>
           </x14:formula1>
-          <xm:sqref>D3:R3 V3:W3</xm:sqref>
+          <xm:sqref>V3:W3 D3:R3</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3598,8 +3622,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47CCFCDD-5474-4738-99E7-D36CCA4BF033}">
   <dimension ref="A1:Z71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="X9" sqref="X9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -3661,7 +3685,7 @@
       </c>
       <c r="O1" t="str">
         <f>'weekly hours'!O1</f>
-        <v>Engineer/supervisor</v>
+        <v>Welder</v>
       </c>
       <c r="P1" t="str">
         <f>'weekly hours'!P1</f>
@@ -3676,24 +3700,20 @@
         <v>Welder</v>
       </c>
       <c r="S1" t="str">
+        <f>'weekly hours'!S1</f>
+        <v>Engineer/supervisor</v>
+      </c>
+      <c r="T1" t="str">
         <f>'weekly hours'!T1</f>
         <v>Engineer/supervisor</v>
       </c>
-      <c r="T1" t="str">
+      <c r="U1" t="str">
         <f>'weekly hours'!U1</f>
         <v>Welder</v>
       </c>
-      <c r="U1" t="str">
+      <c r="V1" t="str">
         <f>'weekly hours'!V1</f>
         <v>Welder</v>
-      </c>
-      <c r="V1" t="str">
-        <f>'weekly hours'!W1</f>
-        <v>Welder</v>
-      </c>
-      <c r="W1" t="str">
-        <f>'weekly hours'!S1</f>
-        <v>Engineer/supervisor</v>
       </c>
       <c r="X1" s="1"/>
       <c r="Y1" s="1"/>
@@ -3750,7 +3770,7 @@
       </c>
       <c r="O2" s="13">
         <f>'weekly hours'!O2</f>
-        <v>536</v>
+        <v>469</v>
       </c>
       <c r="P2" s="13">
         <f>'weekly hours'!P2</f>
@@ -3765,24 +3785,20 @@
         <v>469</v>
       </c>
       <c r="S2" s="13">
+        <f>'weekly hours'!S2</f>
+        <v>536</v>
+      </c>
+      <c r="T2" s="13">
         <f>'weekly hours'!T2</f>
         <v>536</v>
       </c>
-      <c r="T2" s="13">
+      <c r="U2" s="13">
         <f>'weekly hours'!U2</f>
         <v>469</v>
       </c>
-      <c r="U2" s="13">
+      <c r="V2" s="13">
         <f>'weekly hours'!V2</f>
         <v>469</v>
-      </c>
-      <c r="V2" s="13">
-        <f>'weekly hours'!W2</f>
-        <v>469</v>
-      </c>
-      <c r="W2" s="13">
-        <f>'weekly hours'!S2</f>
-        <v>536</v>
       </c>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -3824,7 +3840,7 @@
       </c>
       <c r="J3" t="str">
         <f>'weekly hours'!J3</f>
-        <v>Roy Z</v>
+        <v>Alsa G</v>
       </c>
       <c r="K3" t="str">
         <f>'weekly hours'!K3</f>
@@ -3844,7 +3860,7 @@
       </c>
       <c r="O3" t="str">
         <f>'weekly hours'!O3</f>
-        <v>Brian M</v>
+        <v>Levi W</v>
       </c>
       <c r="P3" t="str">
         <f>'weekly hours'!P3</f>
@@ -3859,24 +3875,20 @@
         <v>Luke G</v>
       </c>
       <c r="S3" t="str">
+        <f>'weekly hours'!S3</f>
+        <v>Vu T</v>
+      </c>
+      <c r="T3" t="str">
         <f>'weekly hours'!T3</f>
         <v xml:space="preserve">Tony M </v>
       </c>
-      <c r="T3" t="str">
+      <c r="U3" t="str">
         <f>'weekly hours'!U3</f>
         <v>Wyatt S</v>
       </c>
-      <c r="U3" t="str">
+      <c r="V3" t="str">
         <f>'weekly hours'!V3</f>
         <v>Ryan O</v>
-      </c>
-      <c r="V3" t="str">
-        <f>'weekly hours'!W3</f>
-        <v>Levi W</v>
-      </c>
-      <c r="W3" t="str">
-        <f>'weekly hours'!S3</f>
-        <v>Vu T</v>
       </c>
     </row>
     <row r="4" spans="1:26" x14ac:dyDescent="0.55000000000000004">
@@ -3953,25 +3965,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S4" s="1" t="str">
+        <f>IF('weekly hours'!S4=0," ",'weekly hours'!S4/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T4" s="1" t="str">
         <f>IF('weekly hours'!T4=0," ",'weekly hours'!T4/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T4" s="1" t="str">
+      <c r="U4" s="1" t="str">
         <f>IF('weekly hours'!U4=0," ",'weekly hours'!U4/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U4" s="1" t="str">
+      <c r="V4" s="1" t="str">
         <f>IF('weekly hours'!V4=0," ",'weekly hours'!V4/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V4" s="1" t="str">
-        <f>IF('weekly hours'!W4=0," ",'weekly hours'!W4/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W4" s="1" t="str">
-        <f>IF('weekly hours'!S4=0," ",'weekly hours'!S4/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W4" s="1"/>
     </row>
     <row r="5" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A5">
@@ -4047,25 +4056,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S5" s="1" t="str">
+        <f>IF('weekly hours'!S5=0," ",'weekly hours'!S5/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T5" s="1" t="str">
         <f>IF('weekly hours'!T5=0," ",'weekly hours'!T5/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T5" s="1" t="str">
+      <c r="U5" s="1" t="str">
         <f>IF('weekly hours'!U5=0," ",'weekly hours'!U5/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U5" s="1" t="str">
+      <c r="V5" s="1" t="str">
         <f>IF('weekly hours'!V5=0," ",'weekly hours'!V5/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V5" s="1" t="str">
-        <f>IF('weekly hours'!W5=0," ",'weekly hours'!W5/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W5" s="1" t="str">
-        <f>IF('weekly hours'!S5=0," ",'weekly hours'!S5/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W5" s="1"/>
     </row>
     <row r="6" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A6">
@@ -4141,25 +4147,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S6" s="1" t="str">
+        <f>IF('weekly hours'!S6=0," ",'weekly hours'!S6/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T6" s="1" t="str">
         <f>IF('weekly hours'!T6=0," ",'weekly hours'!T6/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T6" s="1" t="str">
+      <c r="U6" s="1" t="str">
         <f>IF('weekly hours'!U6=0," ",'weekly hours'!U6/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U6" s="1" t="str">
+      <c r="V6" s="1" t="str">
         <f>IF('weekly hours'!V6=0," ",'weekly hours'!V6/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V6" s="1" t="str">
-        <f>IF('weekly hours'!W6=0," ",'weekly hours'!W6/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W6" s="1" t="str">
-        <f>IF('weekly hours'!S6=0," ",'weekly hours'!S6/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W6" s="1"/>
     </row>
     <row r="7" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A7">
@@ -4235,25 +4238,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S7" s="1" t="str">
+        <f>IF('weekly hours'!S7=0," ",'weekly hours'!S7/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T7" s="1" t="str">
         <f>IF('weekly hours'!T7=0," ",'weekly hours'!T7/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T7" s="1" t="str">
+      <c r="U7" s="1" t="str">
         <f>IF('weekly hours'!U7=0," ",'weekly hours'!U7/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U7" s="1" t="str">
+      <c r="V7" s="1" t="str">
         <f>IF('weekly hours'!V7=0," ",'weekly hours'!V7/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V7" s="1" t="str">
-        <f>IF('weekly hours'!W7=0," ",'weekly hours'!W7/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W7" s="1" t="str">
-        <f>IF('weekly hours'!S7=0," ",'weekly hours'!S7/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W7" s="1"/>
     </row>
     <row r="8" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A8">
@@ -4329,25 +4329,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S8" s="1" t="str">
+        <f>IF('weekly hours'!S8=0," ",'weekly hours'!S8/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T8" s="1" t="str">
         <f>IF('weekly hours'!T8=0," ",'weekly hours'!T8/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T8" s="1" t="str">
+      <c r="U8" s="1" t="str">
         <f>IF('weekly hours'!U8=0," ",'weekly hours'!U8/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U8" s="1" t="str">
+      <c r="V8" s="1" t="str">
         <f>IF('weekly hours'!V8=0," ",'weekly hours'!V8/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V8" s="1" t="str">
-        <f>IF('weekly hours'!W8=0," ",'weekly hours'!W8/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W8" s="1" t="str">
-        <f>IF('weekly hours'!S8=0," ",'weekly hours'!S8/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W8" s="1"/>
     </row>
     <row r="9" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A9">
@@ -4423,25 +4420,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S9" s="1" t="str">
+        <f>IF('weekly hours'!S9=0," ",'weekly hours'!S9/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T9" s="1" t="str">
         <f>IF('weekly hours'!T9=0," ",'weekly hours'!T9/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T9" s="1" t="str">
+      <c r="U9" s="1" t="str">
         <f>IF('weekly hours'!U9=0," ",'weekly hours'!U9/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U9" s="1" t="str">
+      <c r="V9" s="1" t="str">
         <f>IF('weekly hours'!V9=0," ",'weekly hours'!V9/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V9" s="1" t="str">
-        <f>IF('weekly hours'!W9=0," ",'weekly hours'!W9/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W9" s="1" t="str">
-        <f>IF('weekly hours'!S9=0," ",'weekly hours'!S9/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W9" s="1"/>
     </row>
     <row r="10" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A10">
@@ -4517,25 +4511,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S10" s="1" t="str">
+        <f>IF('weekly hours'!S10=0," ",'weekly hours'!S10/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T10" s="1" t="str">
         <f>IF('weekly hours'!T10=0," ",'weekly hours'!T10/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T10" s="1" t="str">
+      <c r="U10" s="1" t="str">
         <f>IF('weekly hours'!U10=0," ",'weekly hours'!U10/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U10" s="1" t="str">
+      <c r="V10" s="1" t="str">
         <f>IF('weekly hours'!V10=0," ",'weekly hours'!V10/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V10" s="1" t="str">
-        <f>IF('weekly hours'!W10=0," ",'weekly hours'!W10/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W10" s="1" t="str">
-        <f>IF('weekly hours'!S10=0," ",'weekly hours'!S10/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W10" s="1"/>
     </row>
     <row r="11" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A11">
@@ -4611,25 +4602,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S11" s="1" t="str">
+        <f>IF('weekly hours'!S11=0," ",'weekly hours'!S11/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T11" s="1" t="str">
         <f>IF('weekly hours'!T11=0," ",'weekly hours'!T11/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T11" s="1" t="str">
+      <c r="U11" s="1" t="str">
         <f>IF('weekly hours'!U11=0," ",'weekly hours'!U11/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U11" s="1" t="str">
+      <c r="V11" s="1" t="str">
         <f>IF('weekly hours'!V11=0," ",'weekly hours'!V11/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V11" s="1" t="str">
-        <f>IF('weekly hours'!W11=0," ",'weekly hours'!W11/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W11" s="1" t="str">
-        <f>IF('weekly hours'!S11=0," ",'weekly hours'!S11/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W11" s="1"/>
     </row>
     <row r="12" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A12">
@@ -4705,25 +4693,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S12" s="1" t="str">
+        <f>IF('weekly hours'!S12=0," ",'weekly hours'!S12/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T12" s="1" t="str">
         <f>IF('weekly hours'!T12=0," ",'weekly hours'!T12/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T12" s="1" t="str">
+      <c r="U12" s="1" t="str">
         <f>IF('weekly hours'!U12=0," ",'weekly hours'!U12/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U12" s="1" t="str">
+      <c r="V12" s="1" t="str">
         <f>IF('weekly hours'!V12=0," ",'weekly hours'!V12/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V12" s="1" t="str">
-        <f>IF('weekly hours'!W12=0," ",'weekly hours'!W12/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W12" s="1" t="str">
-        <f>IF('weekly hours'!S12=0," ",'weekly hours'!S12/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W12" s="1"/>
     </row>
     <row r="13" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A13">
@@ -4799,25 +4784,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S13" s="1" t="str">
+        <f>IF('weekly hours'!S13=0," ",'weekly hours'!S13/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T13" s="1" t="str">
         <f>IF('weekly hours'!T13=0," ",'weekly hours'!T13/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T13" s="1" t="str">
+      <c r="U13" s="1" t="str">
         <f>IF('weekly hours'!U13=0," ",'weekly hours'!U13/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U13" s="1" t="str">
+      <c r="V13" s="1" t="str">
         <f>IF('weekly hours'!V13=0," ",'weekly hours'!V13/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V13" s="1" t="str">
-        <f>IF('weekly hours'!W13=0," ",'weekly hours'!W13/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W13" s="1" t="str">
-        <f>IF('weekly hours'!S13=0," ",'weekly hours'!S13/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W13" s="1"/>
     </row>
     <row r="14" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A14">
@@ -4893,25 +4875,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S14" s="1" t="str">
+        <f>IF('weekly hours'!S14=0," ",'weekly hours'!S14/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T14" s="1" t="str">
         <f>IF('weekly hours'!T14=0," ",'weekly hours'!T14/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T14" s="1" t="str">
+      <c r="U14" s="1" t="str">
         <f>IF('weekly hours'!U14=0," ",'weekly hours'!U14/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U14" s="1" t="str">
+      <c r="V14" s="1" t="str">
         <f>IF('weekly hours'!V14=0," ",'weekly hours'!V14/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V14" s="1" t="str">
-        <f>IF('weekly hours'!W14=0," ",'weekly hours'!W14/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W14" s="1" t="str">
-        <f>IF('weekly hours'!S14=0," ",'weekly hours'!S14/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W14" s="1"/>
     </row>
     <row r="15" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A15">
@@ -4987,25 +4966,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S15" s="1" t="str">
+        <f>IF('weekly hours'!S15=0," ",'weekly hours'!S15/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T15" s="1" t="str">
         <f>IF('weekly hours'!T15=0," ",'weekly hours'!T15/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T15" s="1" t="str">
+      <c r="U15" s="1" t="str">
         <f>IF('weekly hours'!U15=0," ",'weekly hours'!U15/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U15" s="1" t="str">
+      <c r="V15" s="1" t="str">
         <f>IF('weekly hours'!V15=0," ",'weekly hours'!V15/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V15" s="1" t="str">
-        <f>IF('weekly hours'!W15=0," ",'weekly hours'!W15/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W15" s="1" t="str">
-        <f>IF('weekly hours'!S15=0," ",'weekly hours'!S15/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W15" s="1"/>
     </row>
     <row r="16" spans="1:26" x14ac:dyDescent="0.55000000000000004">
       <c r="A16">
@@ -5081,25 +5057,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S16" s="1" t="str">
+        <f>IF('weekly hours'!S16=0," ",'weekly hours'!S16/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T16" s="1" t="str">
         <f>IF('weekly hours'!T16=0," ",'weekly hours'!T16/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T16" s="1" t="str">
+      <c r="U16" s="1" t="str">
         <f>IF('weekly hours'!U16=0," ",'weekly hours'!U16/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U16" s="1" t="str">
+      <c r="V16" s="1" t="str">
         <f>IF('weekly hours'!V16=0," ",'weekly hours'!V16/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V16" s="1" t="str">
-        <f>IF('weekly hours'!W16=0," ",'weekly hours'!W16/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W16" s="1" t="str">
-        <f>IF('weekly hours'!S16=0," ",'weekly hours'!S16/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W16" s="1"/>
     </row>
     <row r="17" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A17">
@@ -5175,25 +5148,22 @@
         <v>469</v>
       </c>
       <c r="S17" s="1" t="str">
+        <f>IF('weekly hours'!S17=0," ",'weekly hours'!S17/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T17" s="1" t="str">
         <f>IF('weekly hours'!T17=0," ",'weekly hours'!T17/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T17" s="1" t="str">
+      <c r="U17" s="1" t="str">
         <f>IF('weekly hours'!U17=0," ",'weekly hours'!U17/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U17" s="1" t="str">
+      <c r="V17" s="1" t="str">
         <f>IF('weekly hours'!V17=0," ",'weekly hours'!V17/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V17" s="1" t="str">
-        <f>IF('weekly hours'!W17=0," ",'weekly hours'!W17/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W17" s="1" t="str">
-        <f>IF('weekly hours'!S17=0," ",'weekly hours'!S17/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W17" s="1"/>
     </row>
     <row r="18" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A18">
@@ -5269,25 +5239,22 @@
         <v>2345</v>
       </c>
       <c r="S18" s="1" t="str">
+        <f>IF('weekly hours'!S18=0," ",'weekly hours'!S18/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T18" s="1" t="str">
         <f>IF('weekly hours'!T18=0," ",'weekly hours'!T18/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T18" s="1" t="str">
+      <c r="U18" s="1" t="str">
         <f>IF('weekly hours'!U18=0," ",'weekly hours'!U18/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U18" s="1" t="str">
+      <c r="V18" s="1" t="str">
         <f>IF('weekly hours'!V18=0," ",'weekly hours'!V18/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V18" s="1" t="str">
-        <f>IF('weekly hours'!W18=0," ",'weekly hours'!W18/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W18" s="1" t="str">
-        <f>IF('weekly hours'!S18=0," ",'weekly hours'!S18/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W18" s="1"/>
     </row>
     <row r="19" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A19">
@@ -5363,25 +5330,22 @@
         <v>2345</v>
       </c>
       <c r="S19" s="1" t="str">
+        <f>IF('weekly hours'!S19=0," ",'weekly hours'!S19/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T19" s="1" t="str">
         <f>IF('weekly hours'!T19=0," ",'weekly hours'!T19/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T19" s="1" t="str">
+      <c r="U19" s="1" t="str">
         <f>IF('weekly hours'!U19=0," ",'weekly hours'!U19/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U19" s="1" t="str">
+      <c r="V19" s="1" t="str">
         <f>IF('weekly hours'!V19=0," ",'weekly hours'!V19/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V19" s="1" t="str">
-        <f>IF('weekly hours'!W19=0," ",'weekly hours'!W19/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W19" s="1" t="str">
-        <f>IF('weekly hours'!S19=0," ",'weekly hours'!S19/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W19" s="1"/>
     </row>
     <row r="20" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A20">
@@ -5457,25 +5421,22 @@
         <v>2345</v>
       </c>
       <c r="S20" s="1" t="str">
+        <f>IF('weekly hours'!S20=0," ",'weekly hours'!S20/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T20" s="1" t="str">
         <f>IF('weekly hours'!T20=0," ",'weekly hours'!T20/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T20" s="1" t="str">
+      <c r="U20" s="1" t="str">
         <f>IF('weekly hours'!U20=0," ",'weekly hours'!U20/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U20" s="1" t="str">
+      <c r="V20" s="1" t="str">
         <f>IF('weekly hours'!V20=0," ",'weekly hours'!V20/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V20" s="1" t="str">
-        <f>IF('weekly hours'!W20=0," ",'weekly hours'!W20/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W20" s="1" t="str">
-        <f>IF('weekly hours'!S20=0," ",'weekly hours'!S20/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W20" s="1"/>
     </row>
     <row r="21" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A21">
@@ -5550,26 +5511,23 @@
         <f>IF('weekly hours'!R21=0," ",'weekly hours'!R21/8*'weekly hours'!R$2)</f>
         <v>2345</v>
       </c>
-      <c r="S21" s="1" t="str">
-        <f>IF('weekly hours'!T21=0," ",'weekly hours'!T21/8*'weekly hours'!T$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="T21" s="1" t="str">
-        <f>IF('weekly hours'!U21=0," ",'weekly hours'!U21/8*'weekly hours'!U$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="U21" s="1" t="str">
-        <f>IF('weekly hours'!V21=0," ",'weekly hours'!V21/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V21" s="1" t="str">
-        <f>IF('weekly hours'!W21=0," ",'weekly hours'!W21/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W21" s="1">
+      <c r="S21" s="1">
         <f>IF('weekly hours'!S21=0," ",'weekly hours'!S21/8*'weekly hours'!S$2)</f>
         <v>2680</v>
       </c>
+      <c r="T21" s="1" t="str">
+        <f>IF('weekly hours'!T21=0," ",'weekly hours'!T21/8*'weekly hours'!T$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="U21" s="1" t="str">
+        <f>IF('weekly hours'!U21=0," ",'weekly hours'!U21/8*'weekly hours'!U$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="V21" s="1" t="str">
+        <f>IF('weekly hours'!V21=0," ",'weekly hours'!V21/8*'weekly hours'!V$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W21" s="1"/>
     </row>
     <row r="22" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A22">
@@ -5644,26 +5602,23 @@
         <f>IF('weekly hours'!R22=0," ",'weekly hours'!R22/8*'weekly hours'!R$2)</f>
         <v>2345</v>
       </c>
-      <c r="S22" s="1" t="str">
-        <f>IF('weekly hours'!T22=0," ",'weekly hours'!T22/8*'weekly hours'!T$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="T22" s="1" t="str">
-        <f>IF('weekly hours'!U22=0," ",'weekly hours'!U22/8*'weekly hours'!U$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="U22" s="1" t="str">
-        <f>IF('weekly hours'!V22=0," ",'weekly hours'!V22/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V22" s="1" t="str">
-        <f>IF('weekly hours'!W22=0," ",'weekly hours'!W22/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W22" s="1">
+      <c r="S22" s="1">
         <f>IF('weekly hours'!S22=0," ",'weekly hours'!S22/8*'weekly hours'!S$2)</f>
         <v>2680</v>
       </c>
+      <c r="T22" s="1" t="str">
+        <f>IF('weekly hours'!T22=0," ",'weekly hours'!T22/8*'weekly hours'!T$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="U22" s="1" t="str">
+        <f>IF('weekly hours'!U22=0," ",'weekly hours'!U22/8*'weekly hours'!U$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="V22" s="1" t="str">
+        <f>IF('weekly hours'!V22=0," ",'weekly hours'!V22/8*'weekly hours'!V$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W22" s="1"/>
     </row>
     <row r="23" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A23">
@@ -5738,26 +5693,23 @@
         <f>IF('weekly hours'!R23=0," ",'weekly hours'!R23/8*'weekly hours'!R$2)</f>
         <v>2345</v>
       </c>
-      <c r="S23" s="1" t="str">
-        <f>IF('weekly hours'!T23=0," ",'weekly hours'!T23/8*'weekly hours'!T$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="T23" s="1" t="str">
-        <f>IF('weekly hours'!U23=0," ",'weekly hours'!U23/8*'weekly hours'!U$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="U23" s="1" t="str">
-        <f>IF('weekly hours'!V23=0," ",'weekly hours'!V23/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V23" s="1" t="str">
-        <f>IF('weekly hours'!W23=0," ",'weekly hours'!W23/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W23" s="1">
+      <c r="S23" s="1">
         <f>IF('weekly hours'!S23=0," ",'weekly hours'!S23/8*'weekly hours'!S$2)</f>
         <v>2680</v>
       </c>
+      <c r="T23" s="1" t="str">
+        <f>IF('weekly hours'!T23=0," ",'weekly hours'!T23/8*'weekly hours'!T$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="U23" s="1" t="str">
+        <f>IF('weekly hours'!U23=0," ",'weekly hours'!U23/8*'weekly hours'!U$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="V23" s="1" t="str">
+        <f>IF('weekly hours'!V23=0," ",'weekly hours'!V23/8*'weekly hours'!V$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W23" s="1"/>
     </row>
     <row r="24" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A24">
@@ -5832,26 +5784,23 @@
         <f>IF('weekly hours'!R24=0," ",'weekly hours'!R24/8*'weekly hours'!R$2)</f>
         <v>1876</v>
       </c>
-      <c r="S24" s="1" t="str">
-        <f>IF('weekly hours'!T24=0," ",'weekly hours'!T24/8*'weekly hours'!T$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="T24" s="1" t="str">
-        <f>IF('weekly hours'!U24=0," ",'weekly hours'!U24/8*'weekly hours'!U$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="U24" s="1" t="str">
-        <f>IF('weekly hours'!V24=0," ",'weekly hours'!V24/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V24" s="1" t="str">
-        <f>IF('weekly hours'!W24=0," ",'weekly hours'!W24/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W24" s="1">
+      <c r="S24" s="1">
         <f>IF('weekly hours'!S24=0," ",'weekly hours'!S24/8*'weekly hours'!S$2)</f>
         <v>2680</v>
       </c>
+      <c r="T24" s="1" t="str">
+        <f>IF('weekly hours'!T24=0," ",'weekly hours'!T24/8*'weekly hours'!T$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="U24" s="1" t="str">
+        <f>IF('weekly hours'!U24=0," ",'weekly hours'!U24/8*'weekly hours'!U$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="V24" s="1" t="str">
+        <f>IF('weekly hours'!V24=0," ",'weekly hours'!V24/8*'weekly hours'!V$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W24" s="1"/>
     </row>
     <row r="25" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A25">
@@ -5926,26 +5875,23 @@
         <f>IF('weekly hours'!R25=0," ",'weekly hours'!R25/8*'weekly hours'!R$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="S25" s="1" t="str">
-        <f>IF('weekly hours'!T25=0," ",'weekly hours'!T25/8*'weekly hours'!T$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="T25" s="1" t="str">
-        <f>IF('weekly hours'!U25=0," ",'weekly hours'!U25/8*'weekly hours'!U$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="U25" s="1" t="str">
-        <f>IF('weekly hours'!V25=0," ",'weekly hours'!V25/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V25" s="1" t="str">
-        <f>IF('weekly hours'!W25=0," ",'weekly hours'!W25/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W25" s="1">
+      <c r="S25" s="1">
         <f>IF('weekly hours'!S25=0," ",'weekly hours'!S25/8*'weekly hours'!S$2)</f>
         <v>2680</v>
       </c>
+      <c r="T25" s="1" t="str">
+        <f>IF('weekly hours'!T25=0," ",'weekly hours'!T25/8*'weekly hours'!T$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="U25" s="1" t="str">
+        <f>IF('weekly hours'!U25=0," ",'weekly hours'!U25/8*'weekly hours'!U$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="V25" s="1" t="str">
+        <f>IF('weekly hours'!V25=0," ",'weekly hours'!V25/8*'weekly hours'!V$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W25" s="1"/>
     </row>
     <row r="26" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A26">
@@ -6020,26 +5966,23 @@
         <f>IF('weekly hours'!R26=0," ",'weekly hours'!R26/8*'weekly hours'!R$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="S26" s="1" t="str">
-        <f>IF('weekly hours'!T26=0," ",'weekly hours'!T26/8*'weekly hours'!T$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="T26" s="1" t="str">
-        <f>IF('weekly hours'!U26=0," ",'weekly hours'!U26/8*'weekly hours'!U$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="U26" s="1" t="str">
-        <f>IF('weekly hours'!V26=0," ",'weekly hours'!V26/8*'weekly hours'!V$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="V26" s="1" t="str">
-        <f>IF('weekly hours'!W26=0," ",'weekly hours'!W26/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W26" s="1">
+      <c r="S26" s="1">
         <f>IF('weekly hours'!S26=0," ",'weekly hours'!S26/8*'weekly hours'!S$2)</f>
         <v>2680</v>
       </c>
+      <c r="T26" s="1" t="str">
+        <f>IF('weekly hours'!T26=0," ",'weekly hours'!T26/8*'weekly hours'!T$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="U26" s="1" t="str">
+        <f>IF('weekly hours'!U26=0," ",'weekly hours'!U26/8*'weekly hours'!U$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="V26" s="1" t="str">
+        <f>IF('weekly hours'!V26=0," ",'weekly hours'!V26/8*'weekly hours'!V$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="W26" s="1"/>
     </row>
     <row r="27" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A27">
@@ -6098,9 +6041,9 @@
         <f>IF('weekly hours'!N27=0," ",'weekly hours'!N27/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O27" s="1" t="str">
+      <c r="O27" s="1">
         <f>IF('weekly hours'!O27=0," ",'weekly hours'!O27/8*'weekly hours'!O$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="P27" s="1">
         <f>IF('weekly hours'!P27=0," ",'weekly hours'!P27/8*'weekly hours'!P$2)</f>
@@ -6114,26 +6057,23 @@
         <f>IF('weekly hours'!R27=0," ",'weekly hours'!R27/8*'weekly hours'!R$2)</f>
         <v>2345</v>
       </c>
-      <c r="S27" s="1" t="str">
+      <c r="S27" s="1">
+        <f>IF('weekly hours'!S27=0," ",'weekly hours'!S27/8*'weekly hours'!S$2)</f>
+        <v>2680</v>
+      </c>
+      <c r="T27" s="1" t="str">
         <f>IF('weekly hours'!T27=0," ",'weekly hours'!T27/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T27" s="1" t="str">
+      <c r="U27" s="1" t="str">
         <f>IF('weekly hours'!U27=0," ",'weekly hours'!U27/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U27" s="1">
+      <c r="V27" s="1">
         <f>IF('weekly hours'!V27=0," ",'weekly hours'!V27/8*'weekly hours'!V$2)</f>
         <v>2345</v>
       </c>
-      <c r="V27" s="1">
-        <f>IF('weekly hours'!W27=0," ",'weekly hours'!W27/8*'weekly hours'!W$2)</f>
-        <v>2345</v>
-      </c>
-      <c r="W27" s="1">
-        <f>IF('weekly hours'!S27=0," ",'weekly hours'!S27/8*'weekly hours'!S$2)</f>
-        <v>2680</v>
-      </c>
+      <c r="W27" s="1"/>
     </row>
     <row r="28" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A28">
@@ -6192,9 +6132,9 @@
         <f>IF('weekly hours'!N28=0," ",'weekly hours'!N28/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O28" s="1" t="str">
+      <c r="O28" s="1">
         <f>IF('weekly hours'!O28=0," ",'weekly hours'!O28/8*'weekly hours'!O$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="P28" s="1">
         <f>IF('weekly hours'!P28=0," ",'weekly hours'!P28/8*'weekly hours'!P$2)</f>
@@ -6209,25 +6149,22 @@
         <v>2345</v>
       </c>
       <c r="S28" s="1" t="str">
+        <f>IF('weekly hours'!S28=0," ",'weekly hours'!S28/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T28" s="1" t="str">
         <f>IF('weekly hours'!T28=0," ",'weekly hours'!T28/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T28" s="1" t="str">
+      <c r="U28" s="1" t="str">
         <f>IF('weekly hours'!U28=0," ",'weekly hours'!U28/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U28" s="1">
+      <c r="V28" s="1">
         <f>IF('weekly hours'!V28=0," ",'weekly hours'!V28/8*'weekly hours'!V$2)</f>
         <v>938</v>
       </c>
-      <c r="V28" s="1">
-        <f>IF('weekly hours'!W28=0," ",'weekly hours'!W28/8*'weekly hours'!W$2)</f>
-        <v>2345</v>
-      </c>
-      <c r="W28" s="1" t="str">
-        <f>IF('weekly hours'!S28=0," ",'weekly hours'!S28/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W28" s="1"/>
     </row>
     <row r="29" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A29">
@@ -6286,9 +6223,9 @@
         <f>IF('weekly hours'!N29=0," ",'weekly hours'!N29/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O29" s="1" t="str">
+      <c r="O29" s="1">
         <f>IF('weekly hours'!O29=0," ",'weekly hours'!O29/8*'weekly hours'!O$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>1407</v>
       </c>
       <c r="P29" s="1">
         <f>IF('weekly hours'!P29=0," ",'weekly hours'!P29/8*'weekly hours'!P$2)</f>
@@ -6302,26 +6239,23 @@
         <f>IF('weekly hours'!R29=0," ",'weekly hours'!R29/8*'weekly hours'!R$2)</f>
         <v>2345</v>
       </c>
-      <c r="S29" s="1" t="str">
+      <c r="S29" s="1">
+        <f>IF('weekly hours'!S29=0," ",'weekly hours'!S29/8*'weekly hours'!S$2)</f>
+        <v>2680</v>
+      </c>
+      <c r="T29" s="1" t="str">
         <f>IF('weekly hours'!T29=0," ",'weekly hours'!T29/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T29" s="1" t="str">
+      <c r="U29" s="1" t="str">
         <f>IF('weekly hours'!U29=0," ",'weekly hours'!U29/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U29" s="1">
+      <c r="V29" s="1">
         <f>IF('weekly hours'!V29=0," ",'weekly hours'!V29/8*'weekly hours'!V$2)</f>
         <v>1407</v>
       </c>
-      <c r="V29" s="1">
-        <f>IF('weekly hours'!W29=0," ",'weekly hours'!W29/8*'weekly hours'!W$2)</f>
-        <v>1407</v>
-      </c>
-      <c r="W29" s="1">
-        <f>IF('weekly hours'!S29=0," ",'weekly hours'!S29/8*'weekly hours'!S$2)</f>
-        <v>2680</v>
-      </c>
+      <c r="W29" s="1"/>
     </row>
     <row r="30" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A30">
@@ -6397,25 +6331,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S30" s="1" t="str">
+        <f>IF('weekly hours'!S30=0," ",'weekly hours'!S30/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T30" s="1" t="str">
         <f>IF('weekly hours'!T30=0," ",'weekly hours'!T30/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T30" s="1" t="str">
+      <c r="U30" s="1" t="str">
         <f>IF('weekly hours'!U30=0," ",'weekly hours'!U30/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U30" s="1" t="str">
+      <c r="V30" s="1" t="str">
         <f>IF('weekly hours'!V30=0," ",'weekly hours'!V30/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V30" s="1" t="str">
-        <f>IF('weekly hours'!W30=0," ",'weekly hours'!W30/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W30" s="1" t="str">
-        <f>IF('weekly hours'!S30=0," ",'weekly hours'!S30/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W30" s="1"/>
     </row>
     <row r="31" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A31">
@@ -6474,9 +6405,9 @@
         <f>IF('weekly hours'!N31=0," ",'weekly hours'!N31/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O31" s="1" t="str">
+      <c r="O31" s="1">
         <f>IF('weekly hours'!O31=0," ",'weekly hours'!O31/8*'weekly hours'!O$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="P31" s="1">
         <f>IF('weekly hours'!P31=0," ",'weekly hours'!P31/8*'weekly hours'!P$2)</f>
@@ -6491,25 +6422,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S31" s="1" t="str">
+        <f>IF('weekly hours'!S31=0," ",'weekly hours'!S31/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T31" s="1" t="str">
         <f>IF('weekly hours'!T31=0," ",'weekly hours'!T31/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T31" s="1" t="str">
+      <c r="U31" s="1" t="str">
         <f>IF('weekly hours'!U31=0," ",'weekly hours'!U31/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U31" s="1">
+      <c r="V31" s="1">
         <f>IF('weekly hours'!V31=0," ",'weekly hours'!V31/8*'weekly hours'!V$2)</f>
         <v>2345</v>
       </c>
-      <c r="V31" s="1">
-        <f>IF('weekly hours'!W31=0," ",'weekly hours'!W31/8*'weekly hours'!W$2)</f>
-        <v>2345</v>
-      </c>
-      <c r="W31" s="1" t="str">
-        <f>IF('weekly hours'!S31=0," ",'weekly hours'!S31/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W31" s="1"/>
     </row>
     <row r="32" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A32">
@@ -6568,9 +6496,9 @@
         <f>IF('weekly hours'!N32=0," ",'weekly hours'!N32/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O32" s="1" t="str">
+      <c r="O32" s="1">
         <f>IF('weekly hours'!O32=0," ",'weekly hours'!O32/8*'weekly hours'!O$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="P32" s="1">
         <f>IF('weekly hours'!P32=0," ",'weekly hours'!P32/8*'weekly hours'!P$2)</f>
@@ -6585,25 +6513,22 @@
         <v>2345</v>
       </c>
       <c r="S32" s="1" t="str">
+        <f>IF('weekly hours'!S32=0," ",'weekly hours'!S32/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T32" s="1" t="str">
         <f>IF('weekly hours'!T32=0," ",'weekly hours'!T32/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T32" s="1" t="str">
+      <c r="U32" s="1" t="str">
         <f>IF('weekly hours'!U32=0," ",'weekly hours'!U32/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U32" s="1">
+      <c r="V32" s="1">
         <f>IF('weekly hours'!V32=0," ",'weekly hours'!V32/8*'weekly hours'!V$2)</f>
         <v>2345</v>
       </c>
-      <c r="V32" s="1">
-        <f>IF('weekly hours'!W32=0," ",'weekly hours'!W32/8*'weekly hours'!W$2)</f>
-        <v>2345</v>
-      </c>
-      <c r="W32" s="1" t="str">
-        <f>IF('weekly hours'!S32=0," ",'weekly hours'!S32/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W32" s="1"/>
     </row>
     <row r="33" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A33">
@@ -6679,25 +6604,22 @@
         <v>2345</v>
       </c>
       <c r="S33" s="1" t="str">
+        <f>IF('weekly hours'!S33=0," ",'weekly hours'!S33/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T33" s="1" t="str">
         <f>IF('weekly hours'!T33=0," ",'weekly hours'!T33/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T33" s="1" t="str">
+      <c r="U33" s="1" t="str">
         <f>IF('weekly hours'!U33=0," ",'weekly hours'!U33/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U33" s="1">
+      <c r="V33" s="1">
         <f>IF('weekly hours'!V33=0," ",'weekly hours'!V33/8*'weekly hours'!V$2)</f>
         <v>2345</v>
       </c>
-      <c r="V33" s="1" t="str">
-        <f>IF('weekly hours'!W33=0," ",'weekly hours'!W33/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W33" s="1" t="str">
-        <f>IF('weekly hours'!S33=0," ",'weekly hours'!S33/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W33" s="1"/>
     </row>
     <row r="34" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A34">
@@ -6756,9 +6678,9 @@
         <f>IF('weekly hours'!N34=0," ",'weekly hours'!N34/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O34" s="1" t="str">
+      <c r="O34" s="1">
         <f>IF('weekly hours'!O34=0," ",'weekly hours'!O34/8*'weekly hours'!O$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>469</v>
       </c>
       <c r="P34" s="1">
         <f>IF('weekly hours'!P34=0," ",'weekly hours'!P34/8*'weekly hours'!P$2)</f>
@@ -6773,25 +6695,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S34" s="1" t="str">
+        <f>IF('weekly hours'!S34=0," ",'weekly hours'!S34/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T34" s="1" t="str">
         <f>IF('weekly hours'!T34=0," ",'weekly hours'!T34/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T34" s="1" t="str">
+      <c r="U34" s="1" t="str">
         <f>IF('weekly hours'!U34=0," ",'weekly hours'!U34/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U34" s="1" t="str">
+      <c r="V34" s="1" t="str">
         <f>IF('weekly hours'!V34=0," ",'weekly hours'!V34/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V34" s="1">
-        <f>IF('weekly hours'!W34=0," ",'weekly hours'!W34/8*'weekly hours'!W$2)</f>
-        <v>469</v>
-      </c>
-      <c r="W34" s="1" t="str">
-        <f>IF('weekly hours'!S34=0," ",'weekly hours'!S34/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W34" s="1"/>
     </row>
     <row r="35" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A35">
@@ -6850,9 +6769,9 @@
         <f>IF('weekly hours'!N35=0," ",'weekly hours'!N35/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O35" s="1" t="str">
+      <c r="O35" s="1">
         <f>IF('weekly hours'!O35=0," ",'weekly hours'!O35/8*'weekly hours'!O$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="P35" s="1" t="str">
         <f>IF('weekly hours'!P35=0," ",'weekly hours'!P35/8*'weekly hours'!P$2)</f>
@@ -6866,26 +6785,23 @@
         <f>IF('weekly hours'!R35=0," ",'weekly hours'!R35/8*'weekly hours'!R$2)</f>
         <v>2345</v>
       </c>
-      <c r="S35" s="1" t="str">
+      <c r="S35" s="1">
+        <f>IF('weekly hours'!S35=0," ",'weekly hours'!S35/8*'weekly hours'!S$2)</f>
+        <v>2144</v>
+      </c>
+      <c r="T35" s="1" t="str">
         <f>IF('weekly hours'!T35=0," ",'weekly hours'!T35/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T35" s="1" t="str">
+      <c r="U35" s="1" t="str">
         <f>IF('weekly hours'!U35=0," ",'weekly hours'!U35/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U35" s="1">
+      <c r="V35" s="1">
         <f>IF('weekly hours'!V35=0," ",'weekly hours'!V35/8*'weekly hours'!V$2)</f>
         <v>2345</v>
       </c>
-      <c r="V35" s="1">
-        <f>IF('weekly hours'!W35=0," ",'weekly hours'!W35/8*'weekly hours'!W$2)</f>
-        <v>2345</v>
-      </c>
-      <c r="W35" s="1">
-        <f>IF('weekly hours'!S35=0," ",'weekly hours'!S35/8*'weekly hours'!S$2)</f>
-        <v>2144</v>
-      </c>
+      <c r="W35" s="1"/>
     </row>
     <row r="36" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A36">
@@ -6944,9 +6860,9 @@
         <f>IF('weekly hours'!N36=0," ",'weekly hours'!N36/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O36" s="1" t="str">
+      <c r="O36" s="1">
         <f>IF('weekly hours'!O36=0," ",'weekly hours'!O36/8*'weekly hours'!O$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="P36" s="1" t="str">
         <f>IF('weekly hours'!P36=0," ",'weekly hours'!P36/8*'weekly hours'!P$2)</f>
@@ -6960,26 +6876,23 @@
         <f>IF('weekly hours'!R36=0," ",'weekly hours'!R36/8*'weekly hours'!R$2)</f>
         <v>2345</v>
       </c>
-      <c r="S36" s="1" t="str">
+      <c r="S36" s="1">
+        <f>IF('weekly hours'!S36=0," ",'weekly hours'!S36/8*'weekly hours'!S$2)</f>
+        <v>2680</v>
+      </c>
+      <c r="T36" s="1" t="str">
         <f>IF('weekly hours'!T36=0," ",'weekly hours'!T36/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T36" s="1" t="str">
+      <c r="U36" s="1" t="str">
         <f>IF('weekly hours'!U36=0," ",'weekly hours'!U36/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U36" s="1">
+      <c r="V36" s="1">
         <f>IF('weekly hours'!V36=0," ",'weekly hours'!V36/8*'weekly hours'!V$2)</f>
         <v>2345</v>
       </c>
-      <c r="V36" s="1">
-        <f>IF('weekly hours'!W36=0," ",'weekly hours'!W36/8*'weekly hours'!W$2)</f>
-        <v>2345</v>
-      </c>
-      <c r="W36" s="1">
-        <f>IF('weekly hours'!S36=0," ",'weekly hours'!S36/8*'weekly hours'!S$2)</f>
-        <v>2680</v>
-      </c>
+      <c r="W36" s="1"/>
     </row>
     <row r="37" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A37">
@@ -7055,25 +6968,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S37" s="1" t="str">
+        <f>IF('weekly hours'!S37=0," ",'weekly hours'!S37/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T37" s="1" t="str">
         <f>IF('weekly hours'!T37=0," ",'weekly hours'!T37/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T37" s="1" t="str">
+      <c r="U37" s="1" t="str">
         <f>IF('weekly hours'!U37=0," ",'weekly hours'!U37/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U37" s="1" t="str">
+      <c r="V37" s="1" t="str">
         <f>IF('weekly hours'!V37=0," ",'weekly hours'!V37/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V37" s="1" t="str">
-        <f>IF('weekly hours'!W37=0," ",'weekly hours'!W37/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W37" s="1" t="str">
-        <f>IF('weekly hours'!S37=0," ",'weekly hours'!S37/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W37" s="1"/>
     </row>
     <row r="38" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A38">
@@ -7132,9 +7042,9 @@
         <f>IF('weekly hours'!N38=0," ",'weekly hours'!N38/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O38" s="1" t="str">
+      <c r="O38" s="1">
         <f>IF('weekly hours'!O38=0," ",'weekly hours'!O38/8*'weekly hours'!O$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="P38" s="1">
         <f>IF('weekly hours'!P38=0," ",'weekly hours'!P38/8*'weekly hours'!P$2)</f>
@@ -7149,25 +7059,22 @@
         <v>2345</v>
       </c>
       <c r="S38" s="1" t="str">
+        <f>IF('weekly hours'!S38=0," ",'weekly hours'!S38/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T38" s="1" t="str">
         <f>IF('weekly hours'!T38=0," ",'weekly hours'!T38/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T38" s="1" t="str">
+      <c r="U38" s="1" t="str">
         <f>IF('weekly hours'!U38=0," ",'weekly hours'!U38/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U38" s="1" t="str">
+      <c r="V38" s="1" t="str">
         <f>IF('weekly hours'!V38=0," ",'weekly hours'!V38/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V38" s="1">
-        <f>IF('weekly hours'!W38=0," ",'weekly hours'!W38/8*'weekly hours'!W$2)</f>
-        <v>2345</v>
-      </c>
-      <c r="W38" s="1" t="str">
-        <f>IF('weekly hours'!S38=0," ",'weekly hours'!S38/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W38" s="1"/>
     </row>
     <row r="39" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A39">
@@ -7226,9 +7133,9 @@
         <f>IF('weekly hours'!N39=0," ",'weekly hours'!N39/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O39" s="1" t="str">
+      <c r="O39" s="1">
         <f>IF('weekly hours'!O39=0," ",'weekly hours'!O39/8*'weekly hours'!O$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="P39" s="1">
         <f>IF('weekly hours'!P39=0," ",'weekly hours'!P39/8*'weekly hours'!P$2)</f>
@@ -7243,25 +7150,22 @@
         <v>2345</v>
       </c>
       <c r="S39" s="1" t="str">
+        <f>IF('weekly hours'!S39=0," ",'weekly hours'!S39/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T39" s="1" t="str">
         <f>IF('weekly hours'!T39=0," ",'weekly hours'!T39/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T39" s="1" t="str">
+      <c r="U39" s="1" t="str">
         <f>IF('weekly hours'!U39=0," ",'weekly hours'!U39/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U39" s="1">
+      <c r="V39" s="1">
         <f>IF('weekly hours'!V39=0," ",'weekly hours'!V39/8*'weekly hours'!V$2)</f>
         <v>2345</v>
       </c>
-      <c r="V39" s="1">
-        <f>IF('weekly hours'!W39=0," ",'weekly hours'!W39/8*'weekly hours'!W$2)</f>
-        <v>2345</v>
-      </c>
-      <c r="W39" s="1" t="str">
-        <f>IF('weekly hours'!S39=0," ",'weekly hours'!S39/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W39" s="1"/>
     </row>
     <row r="40" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A40">
@@ -7320,9 +7224,9 @@
         <f>IF('weekly hours'!N40=0," ",'weekly hours'!N40/8*'weekly hours'!N$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="O40" s="1" t="str">
+      <c r="O40" s="1">
         <f>IF('weekly hours'!O40=0," ",'weekly hours'!O40/8*'weekly hours'!O$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2345</v>
       </c>
       <c r="P40" s="1">
         <f>IF('weekly hours'!P40=0," ",'weekly hours'!P40/8*'weekly hours'!P$2)</f>
@@ -7336,26 +7240,23 @@
         <f>IF('weekly hours'!R40=0," ",'weekly hours'!R40/8*'weekly hours'!R$2)</f>
         <v>2345</v>
       </c>
-      <c r="S40" s="1">
+      <c r="S40" s="1" t="str">
+        <f>IF('weekly hours'!S40=0," ",'weekly hours'!S40/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T40" s="1">
         <f>IF('weekly hours'!T40=0," ",'weekly hours'!T40/8*'weekly hours'!T$2)</f>
         <v>2680</v>
       </c>
-      <c r="T40" s="1" t="str">
+      <c r="U40" s="1" t="str">
         <f>IF('weekly hours'!U40=0," ",'weekly hours'!U40/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U40" s="1">
+      <c r="V40" s="1">
         <f>IF('weekly hours'!V40=0," ",'weekly hours'!V40/8*'weekly hours'!V$2)</f>
         <v>2345</v>
       </c>
-      <c r="V40" s="1">
-        <f>IF('weekly hours'!W40=0," ",'weekly hours'!W40/8*'weekly hours'!W$2)</f>
-        <v>2345</v>
-      </c>
-      <c r="W40" s="1" t="str">
-        <f>IF('weekly hours'!S40=0," ",'weekly hours'!S40/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W40" s="1"/>
     </row>
     <row r="41" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A41">
@@ -7431,25 +7332,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S41" s="1" t="str">
+        <f>IF('weekly hours'!S41=0," ",'weekly hours'!S41/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T41" s="1" t="str">
         <f>IF('weekly hours'!T41=0," ",'weekly hours'!T41/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T41" s="1" t="str">
+      <c r="U41" s="1" t="str">
         <f>IF('weekly hours'!U41=0," ",'weekly hours'!U41/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U41" s="1" t="str">
+      <c r="V41" s="1" t="str">
         <f>IF('weekly hours'!V41=0," ",'weekly hours'!V41/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V41" s="1" t="str">
-        <f>IF('weekly hours'!W41=0," ",'weekly hours'!W41/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W41" s="1" t="str">
-        <f>IF('weekly hours'!S41=0," ",'weekly hours'!S41/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W41" s="1"/>
     </row>
     <row r="42" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A42">
@@ -7525,25 +7423,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S42" s="1" t="str">
+        <f>IF('weekly hours'!S42=0," ",'weekly hours'!S42/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T42" s="1" t="str">
         <f>IF('weekly hours'!T42=0," ",'weekly hours'!T42/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T42" s="1" t="str">
+      <c r="U42" s="1" t="str">
         <f>IF('weekly hours'!U42=0," ",'weekly hours'!U42/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U42" s="1" t="str">
+      <c r="V42" s="1" t="str">
         <f>IF('weekly hours'!V42=0," ",'weekly hours'!V42/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V42" s="1" t="str">
-        <f>IF('weekly hours'!W42=0," ",'weekly hours'!W42/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W42" s="1" t="str">
-        <f>IF('weekly hours'!S42=0," ",'weekly hours'!S42/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W42" s="1"/>
     </row>
     <row r="43" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A43">
@@ -7618,26 +7513,23 @@
         <f>IF('weekly hours'!R43=0," ",'weekly hours'!R43/8*'weekly hours'!R$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="S43" s="1" t="str">
+      <c r="S43" s="1">
+        <f>IF('weekly hours'!S43=0," ",'weekly hours'!S43/8*'weekly hours'!S$2)</f>
+        <v>2144</v>
+      </c>
+      <c r="T43" s="1" t="str">
         <f>IF('weekly hours'!T43=0," ",'weekly hours'!T43/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T43" s="1">
+      <c r="U43" s="1">
         <f>IF('weekly hours'!U43=0," ",'weekly hours'!U43/8*'weekly hours'!U$2)</f>
         <v>1876</v>
       </c>
-      <c r="U43" s="1" t="str">
+      <c r="V43" s="1" t="str">
         <f>IF('weekly hours'!V43=0," ",'weekly hours'!V43/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V43" s="1" t="str">
-        <f>IF('weekly hours'!W43=0," ",'weekly hours'!W43/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W43" s="1">
-        <f>IF('weekly hours'!S43=0," ",'weekly hours'!S43/8*'weekly hours'!S$2)</f>
-        <v>2144</v>
-      </c>
+      <c r="W43" s="1"/>
     </row>
     <row r="44" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A44">
@@ -7684,9 +7576,9 @@
         <f>IF('weekly hours'!K44=0," ",'weekly hours'!K44/8*'weekly hours'!K$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="L44" s="1" t="str">
+      <c r="L44" s="1">
         <f>IF('weekly hours'!L44=0," ",'weekly hours'!L44/8*'weekly hours'!L$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>3355</v>
       </c>
       <c r="M44" s="1" t="str">
         <f>IF('weekly hours'!M44=0," ",'weekly hours'!M44/8*'weekly hours'!M$2)</f>
@@ -7700,38 +7592,35 @@
         <f>IF('weekly hours'!O44=0," ",'weekly hours'!O44/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P44" s="1" t="str">
+      <c r="P44" s="1">
         <f>IF('weekly hours'!P44=0," ",'weekly hours'!P44/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q44" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q44" s="1">
         <f>IF('weekly hours'!Q44=0," ",'weekly hours'!Q44/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2280</v>
       </c>
       <c r="R44" s="1" t="str">
         <f>IF('weekly hours'!R44=0," ",'weekly hours'!R44/8*'weekly hours'!R$2)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="S44" s="1" t="str">
+        <f>IF('weekly hours'!S44=0," ",'weekly hours'!S44/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T44" s="1">
         <f>IF('weekly hours'!T44=0," ",'weekly hours'!T44/8*'weekly hours'!T$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="T44" s="1" t="str">
+        <v>1608</v>
+      </c>
+      <c r="U44" s="1">
         <f>IF('weekly hours'!U44=0," ",'weekly hours'!U44/8*'weekly hours'!U$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="U44" s="1" t="str">
+        <v>1407</v>
+      </c>
+      <c r="V44" s="1" t="str">
         <f>IF('weekly hours'!V44=0," ",'weekly hours'!V44/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V44" s="1" t="str">
-        <f>IF('weekly hours'!W44=0," ",'weekly hours'!W44/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W44" s="1" t="str">
-        <f>IF('weekly hours'!S44=0," ",'weekly hours'!S44/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W44" s="1"/>
     </row>
     <row r="45" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A45">
@@ -7778,9 +7667,9 @@
         <f>IF('weekly hours'!K45=0," ",'weekly hours'!K45/8*'weekly hours'!K$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="L45" s="1" t="str">
+      <c r="L45" s="1">
         <f>IF('weekly hours'!L45=0," ",'weekly hours'!L45/8*'weekly hours'!L$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>3355</v>
       </c>
       <c r="M45" s="1" t="str">
         <f>IF('weekly hours'!M45=0," ",'weekly hours'!M45/8*'weekly hours'!M$2)</f>
@@ -7794,38 +7683,35 @@
         <f>IF('weekly hours'!O45=0," ",'weekly hours'!O45/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P45" s="1" t="str">
+      <c r="P45" s="1">
         <f>IF('weekly hours'!P45=0," ",'weekly hours'!P45/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q45" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q45" s="1">
         <f>IF('weekly hours'!Q45=0," ",'weekly hours'!Q45/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2280</v>
       </c>
       <c r="R45" s="1" t="str">
         <f>IF('weekly hours'!R45=0," ",'weekly hours'!R45/8*'weekly hours'!R$2)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="S45" s="1" t="str">
+        <f>IF('weekly hours'!S45=0," ",'weekly hours'!S45/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T45" s="1">
         <f>IF('weekly hours'!T45=0," ",'weekly hours'!T45/8*'weekly hours'!T$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="T45" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="U45" s="1" t="str">
         <f>IF('weekly hours'!U45=0," ",'weekly hours'!U45/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U45" s="1" t="str">
+      <c r="V45" s="1" t="str">
         <f>IF('weekly hours'!V45=0," ",'weekly hours'!V45/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V45" s="1" t="str">
-        <f>IF('weekly hours'!W45=0," ",'weekly hours'!W45/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W45" s="1" t="str">
-        <f>IF('weekly hours'!S45=0," ",'weekly hours'!S45/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W45" s="1"/>
     </row>
     <row r="46" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A46">
@@ -7856,13 +7742,13 @@
         <f>IF('weekly hours'!G46=0," ",'weekly hours'!G46/8*'weekly hours'!G$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="H46" s="1" t="str">
+      <c r="H46" s="1">
         <f>IF('weekly hours'!H46=0," ",'weekly hours'!H46/8*'weekly hours'!H$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="I46" s="1" t="str">
+        <v>268</v>
+      </c>
+      <c r="I46" s="1">
         <f>IF('weekly hours'!I46=0," ",'weekly hours'!I46/8*'weekly hours'!I$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>67</v>
       </c>
       <c r="J46" s="1" t="str">
         <f>IF('weekly hours'!J46=0," ",'weekly hours'!J46/8*'weekly hours'!J$2)</f>
@@ -7872,9 +7758,9 @@
         <f>IF('weekly hours'!K46=0," ",'weekly hours'!K46/8*'weekly hours'!K$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="L46" s="1" t="str">
+      <c r="L46" s="1">
         <f>IF('weekly hours'!L46=0," ",'weekly hours'!L46/8*'weekly hours'!L$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>3355</v>
       </c>
       <c r="M46" s="1" t="str">
         <f>IF('weekly hours'!M46=0," ",'weekly hours'!M46/8*'weekly hours'!M$2)</f>
@@ -7888,38 +7774,35 @@
         <f>IF('weekly hours'!O46=0," ",'weekly hours'!O46/8*'weekly hours'!O$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="P46" s="1" t="str">
+      <c r="P46" s="1">
         <f>IF('weekly hours'!P46=0," ",'weekly hours'!P46/8*'weekly hours'!P$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="Q46" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="Q46" s="1">
         <f>IF('weekly hours'!Q46=0," ",'weekly hours'!Q46/8*'weekly hours'!Q$2)</f>
-        <v xml:space="preserve"> </v>
+        <v>2280</v>
       </c>
       <c r="R46" s="1" t="str">
         <f>IF('weekly hours'!R46=0," ",'weekly hours'!R46/8*'weekly hours'!R$2)</f>
         <v xml:space="preserve"> </v>
       </c>
       <c r="S46" s="1" t="str">
+        <f>IF('weekly hours'!S46=0," ",'weekly hours'!S46/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T46" s="1">
         <f>IF('weekly hours'!T46=0," ",'weekly hours'!T46/8*'weekly hours'!T$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="T46" s="1" t="str">
+        <v>2680</v>
+      </c>
+      <c r="U46" s="1" t="str">
         <f>IF('weekly hours'!U46=0," ",'weekly hours'!U46/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U46" s="1" t="str">
+      <c r="V46" s="1" t="str">
         <f>IF('weekly hours'!V46=0," ",'weekly hours'!V46/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V46" s="1" t="str">
-        <f>IF('weekly hours'!W46=0," ",'weekly hours'!W46/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W46" s="1" t="str">
-        <f>IF('weekly hours'!S46=0," ",'weekly hours'!S46/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W46" s="1"/>
     </row>
     <row r="47" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A47">
@@ -7995,25 +7878,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S47" s="1" t="str">
+        <f>IF('weekly hours'!S47=0," ",'weekly hours'!S47/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T47" s="1" t="str">
         <f>IF('weekly hours'!T47=0," ",'weekly hours'!T47/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T47" s="1" t="str">
+      <c r="U47" s="1" t="str">
         <f>IF('weekly hours'!U47=0," ",'weekly hours'!U47/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U47" s="1" t="str">
+      <c r="V47" s="1" t="str">
         <f>IF('weekly hours'!V47=0," ",'weekly hours'!V47/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V47" s="1" t="str">
-        <f>IF('weekly hours'!W47=0," ",'weekly hours'!W47/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W47" s="1" t="str">
-        <f>IF('weekly hours'!S47=0," ",'weekly hours'!S47/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W47" s="1"/>
     </row>
     <row r="48" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A48">
@@ -8089,25 +7969,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S48" s="1" t="str">
+        <f>IF('weekly hours'!S48=0," ",'weekly hours'!S48/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T48" s="1" t="str">
         <f>IF('weekly hours'!T48=0," ",'weekly hours'!T48/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T48" s="1" t="str">
+      <c r="U48" s="1" t="str">
         <f>IF('weekly hours'!U48=0," ",'weekly hours'!U48/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U48" s="1" t="str">
+      <c r="V48" s="1" t="str">
         <f>IF('weekly hours'!V48=0," ",'weekly hours'!V48/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V48" s="1" t="str">
-        <f>IF('weekly hours'!W48=0," ",'weekly hours'!W48/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W48" s="1" t="str">
-        <f>IF('weekly hours'!S48=0," ",'weekly hours'!S48/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W48" s="1"/>
     </row>
     <row r="49" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A49">
@@ -8183,25 +8060,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S49" s="1" t="str">
+        <f>IF('weekly hours'!S49=0," ",'weekly hours'!S49/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T49" s="1" t="str">
         <f>IF('weekly hours'!T49=0," ",'weekly hours'!T49/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T49" s="1" t="str">
+      <c r="U49" s="1" t="str">
         <f>IF('weekly hours'!U49=0," ",'weekly hours'!U49/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U49" s="1" t="str">
+      <c r="V49" s="1" t="str">
         <f>IF('weekly hours'!V49=0," ",'weekly hours'!V49/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V49" s="1" t="str">
-        <f>IF('weekly hours'!W49=0," ",'weekly hours'!W49/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W49" s="1" t="str">
-        <f>IF('weekly hours'!S49=0," ",'weekly hours'!S49/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W49" s="1"/>
     </row>
     <row r="50" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A50">
@@ -8277,25 +8151,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S50" s="1" t="str">
+        <f>IF('weekly hours'!S50=0," ",'weekly hours'!S50/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T50" s="1" t="str">
         <f>IF('weekly hours'!T50=0," ",'weekly hours'!T50/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T50" s="1" t="str">
+      <c r="U50" s="1" t="str">
         <f>IF('weekly hours'!U50=0," ",'weekly hours'!U50/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U50" s="1" t="str">
+      <c r="V50" s="1" t="str">
         <f>IF('weekly hours'!V50=0," ",'weekly hours'!V50/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V50" s="1" t="str">
-        <f>IF('weekly hours'!W50=0," ",'weekly hours'!W50/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W50" s="1" t="str">
-        <f>IF('weekly hours'!S50=0," ",'weekly hours'!S50/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W50" s="1"/>
     </row>
     <row r="51" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A51">
@@ -8371,25 +8242,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S51" s="1" t="str">
+        <f>IF('weekly hours'!S51=0," ",'weekly hours'!S51/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T51" s="1" t="str">
         <f>IF('weekly hours'!T51=0," ",'weekly hours'!T51/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T51" s="1" t="str">
+      <c r="U51" s="1" t="str">
         <f>IF('weekly hours'!U51=0," ",'weekly hours'!U51/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U51" s="1" t="str">
+      <c r="V51" s="1" t="str">
         <f>IF('weekly hours'!V51=0," ",'weekly hours'!V51/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V51" s="1" t="str">
-        <f>IF('weekly hours'!W51=0," ",'weekly hours'!W51/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W51" s="1" t="str">
-        <f>IF('weekly hours'!S51=0," ",'weekly hours'!S51/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W51" s="1"/>
     </row>
     <row r="52" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A52">
@@ -8465,25 +8333,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S52" s="1" t="str">
+        <f>IF('weekly hours'!S52=0," ",'weekly hours'!S52/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T52" s="1" t="str">
         <f>IF('weekly hours'!T52=0," ",'weekly hours'!T52/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T52" s="1" t="str">
+      <c r="U52" s="1" t="str">
         <f>IF('weekly hours'!U52=0," ",'weekly hours'!U52/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U52" s="1" t="str">
+      <c r="V52" s="1" t="str">
         <f>IF('weekly hours'!V52=0," ",'weekly hours'!V52/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V52" s="1" t="str">
-        <f>IF('weekly hours'!W52=0," ",'weekly hours'!W52/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W52" s="1" t="str">
-        <f>IF('weekly hours'!S52=0," ",'weekly hours'!S52/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W52" s="1"/>
     </row>
     <row r="53" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A53">
@@ -8559,25 +8424,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S53" s="1" t="str">
+        <f>IF('weekly hours'!S53=0," ",'weekly hours'!S53/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T53" s="1" t="str">
         <f>IF('weekly hours'!T53=0," ",'weekly hours'!T53/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T53" s="1" t="str">
+      <c r="U53" s="1" t="str">
         <f>IF('weekly hours'!U53=0," ",'weekly hours'!U53/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U53" s="1" t="str">
+      <c r="V53" s="1" t="str">
         <f>IF('weekly hours'!V53=0," ",'weekly hours'!V53/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V53" s="1" t="str">
-        <f>IF('weekly hours'!W53=0," ",'weekly hours'!W53/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W53" s="1" t="str">
-        <f>IF('weekly hours'!S53=0," ",'weekly hours'!S53/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W53" s="1"/>
     </row>
     <row r="54" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A54">
@@ -8653,25 +8515,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S54" s="1" t="str">
+        <f>IF('weekly hours'!S54=0," ",'weekly hours'!S54/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T54" s="1" t="str">
         <f>IF('weekly hours'!T54=0," ",'weekly hours'!T54/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T54" s="1" t="str">
+      <c r="U54" s="1" t="str">
         <f>IF('weekly hours'!U54=0," ",'weekly hours'!U54/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U54" s="1" t="str">
+      <c r="V54" s="1" t="str">
         <f>IF('weekly hours'!V54=0," ",'weekly hours'!V54/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V54" s="1" t="str">
-        <f>IF('weekly hours'!W54=0," ",'weekly hours'!W54/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W54" s="1" t="str">
-        <f>IF('weekly hours'!S54=0," ",'weekly hours'!S54/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W54" s="1"/>
     </row>
     <row r="55" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A55">
@@ -8747,25 +8606,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S55" s="1" t="str">
+        <f>IF('weekly hours'!S55=0," ",'weekly hours'!S55/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T55" s="1" t="str">
         <f>IF('weekly hours'!T55=0," ",'weekly hours'!T55/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T55" s="1" t="str">
+      <c r="U55" s="1" t="str">
         <f>IF('weekly hours'!U55=0," ",'weekly hours'!U55/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U55" s="1" t="str">
+      <c r="V55" s="1" t="str">
         <f>IF('weekly hours'!V55=0," ",'weekly hours'!V55/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V55" s="1" t="str">
-        <f>IF('weekly hours'!W55=0," ",'weekly hours'!W55/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W55" s="1" t="str">
-        <f>IF('weekly hours'!S55=0," ",'weekly hours'!S55/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W55" s="1"/>
     </row>
     <row r="56" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A56">
@@ -8841,25 +8697,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S56" s="1" t="str">
+        <f>IF('weekly hours'!S56=0," ",'weekly hours'!S56/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T56" s="1" t="str">
         <f>IF('weekly hours'!T56=0," ",'weekly hours'!T56/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T56" s="1" t="str">
+      <c r="U56" s="1" t="str">
         <f>IF('weekly hours'!U56=0," ",'weekly hours'!U56/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U56" s="1" t="str">
+      <c r="V56" s="1" t="str">
         <f>IF('weekly hours'!V56=0," ",'weekly hours'!V56/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V56" s="1" t="str">
-        <f>IF('weekly hours'!W56=0," ",'weekly hours'!W56/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W56" s="1" t="str">
-        <f>IF('weekly hours'!S56=0," ",'weekly hours'!S56/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W56" s="1"/>
     </row>
     <row r="57" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A57">
@@ -8935,25 +8788,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S57" s="1" t="str">
+        <f>IF('weekly hours'!S57=0," ",'weekly hours'!S57/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T57" s="1" t="str">
         <f>IF('weekly hours'!T57=0," ",'weekly hours'!T57/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T57" s="1" t="str">
+      <c r="U57" s="1" t="str">
         <f>IF('weekly hours'!U57=0," ",'weekly hours'!U57/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U57" s="1" t="str">
+      <c r="V57" s="1" t="str">
         <f>IF('weekly hours'!V57=0," ",'weekly hours'!V57/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V57" s="1" t="str">
-        <f>IF('weekly hours'!W57=0," ",'weekly hours'!W57/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W57" s="1" t="str">
-        <f>IF('weekly hours'!S57=0," ",'weekly hours'!S57/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W57" s="1"/>
     </row>
     <row r="58" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A58">
@@ -9029,25 +8879,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S58" s="1" t="str">
+        <f>IF('weekly hours'!S58=0," ",'weekly hours'!S58/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T58" s="1" t="str">
         <f>IF('weekly hours'!T58=0," ",'weekly hours'!T58/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T58" s="1" t="str">
+      <c r="U58" s="1" t="str">
         <f>IF('weekly hours'!U58=0," ",'weekly hours'!U58/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U58" s="1" t="str">
+      <c r="V58" s="1" t="str">
         <f>IF('weekly hours'!V58=0," ",'weekly hours'!V58/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V58" s="1" t="str">
-        <f>IF('weekly hours'!W58=0," ",'weekly hours'!W58/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W58" s="1" t="str">
-        <f>IF('weekly hours'!S58=0," ",'weekly hours'!S58/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W58" s="1"/>
     </row>
     <row r="59" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A59">
@@ -9123,25 +8970,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S59" s="1" t="str">
+        <f>IF('weekly hours'!S59=0," ",'weekly hours'!S59/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T59" s="1" t="str">
         <f>IF('weekly hours'!T59=0," ",'weekly hours'!T59/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T59" s="1" t="str">
+      <c r="U59" s="1" t="str">
         <f>IF('weekly hours'!U59=0," ",'weekly hours'!U59/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U59" s="1" t="str">
+      <c r="V59" s="1" t="str">
         <f>IF('weekly hours'!V59=0," ",'weekly hours'!V59/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V59" s="1" t="str">
-        <f>IF('weekly hours'!W59=0," ",'weekly hours'!W59/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W59" s="1" t="str">
-        <f>IF('weekly hours'!S59=0," ",'weekly hours'!S59/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W59" s="1"/>
     </row>
     <row r="60" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A60">
@@ -9217,25 +9061,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S60" s="1" t="str">
+        <f>IF('weekly hours'!S60=0," ",'weekly hours'!S60/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T60" s="1" t="str">
         <f>IF('weekly hours'!T60=0," ",'weekly hours'!T60/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T60" s="1" t="str">
+      <c r="U60" s="1" t="str">
         <f>IF('weekly hours'!U60=0," ",'weekly hours'!U60/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U60" s="1" t="str">
+      <c r="V60" s="1" t="str">
         <f>IF('weekly hours'!V60=0," ",'weekly hours'!V60/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V60" s="1" t="str">
-        <f>IF('weekly hours'!W60=0," ",'weekly hours'!W60/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W60" s="1" t="str">
-        <f>IF('weekly hours'!S60=0," ",'weekly hours'!S60/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W60" s="1"/>
     </row>
     <row r="61" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A61">
@@ -9311,25 +9152,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S61" s="1" t="str">
+        <f>IF('weekly hours'!S61=0," ",'weekly hours'!S61/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T61" s="1" t="str">
         <f>IF('weekly hours'!T61=0," ",'weekly hours'!T61/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T61" s="1" t="str">
+      <c r="U61" s="1" t="str">
         <f>IF('weekly hours'!U61=0," ",'weekly hours'!U61/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U61" s="1" t="str">
+      <c r="V61" s="1" t="str">
         <f>IF('weekly hours'!V61=0," ",'weekly hours'!V61/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V61" s="1" t="str">
-        <f>IF('weekly hours'!W61=0," ",'weekly hours'!W61/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W61" s="1" t="str">
-        <f>IF('weekly hours'!S61=0," ",'weekly hours'!S61/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W61" s="1"/>
     </row>
     <row r="62" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A62">
@@ -9405,25 +9243,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S62" s="1" t="str">
+        <f>IF('weekly hours'!S62=0," ",'weekly hours'!S62/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T62" s="1" t="str">
         <f>IF('weekly hours'!T62=0," ",'weekly hours'!T62/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T62" s="1" t="str">
+      <c r="U62" s="1" t="str">
         <f>IF('weekly hours'!U62=0," ",'weekly hours'!U62/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U62" s="1" t="str">
+      <c r="V62" s="1" t="str">
         <f>IF('weekly hours'!V62=0," ",'weekly hours'!V62/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V62" s="1" t="str">
-        <f>IF('weekly hours'!W62=0," ",'weekly hours'!W62/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W62" s="1" t="str">
-        <f>IF('weekly hours'!S62=0," ",'weekly hours'!S62/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W62" s="1"/>
     </row>
     <row r="63" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A63">
@@ -9499,25 +9334,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S63" s="1" t="str">
+        <f>IF('weekly hours'!S63=0," ",'weekly hours'!S63/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T63" s="1" t="str">
         <f>IF('weekly hours'!T63=0," ",'weekly hours'!T63/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T63" s="1" t="str">
+      <c r="U63" s="1" t="str">
         <f>IF('weekly hours'!U63=0," ",'weekly hours'!U63/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U63" s="1" t="str">
+      <c r="V63" s="1" t="str">
         <f>IF('weekly hours'!V63=0," ",'weekly hours'!V63/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V63" s="1" t="str">
-        <f>IF('weekly hours'!W63=0," ",'weekly hours'!W63/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W63" s="1" t="str">
-        <f>IF('weekly hours'!S63=0," ",'weekly hours'!S63/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W63" s="1"/>
     </row>
     <row r="64" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A64">
@@ -9593,25 +9425,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S64" s="1" t="str">
+        <f>IF('weekly hours'!S64=0," ",'weekly hours'!S64/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T64" s="1" t="str">
         <f>IF('weekly hours'!T64=0," ",'weekly hours'!T64/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T64" s="1" t="str">
+      <c r="U64" s="1" t="str">
         <f>IF('weekly hours'!U64=0," ",'weekly hours'!U64/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U64" s="1" t="str">
+      <c r="V64" s="1" t="str">
         <f>IF('weekly hours'!V64=0," ",'weekly hours'!V64/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V64" s="1" t="str">
-        <f>IF('weekly hours'!W64=0," ",'weekly hours'!W64/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W64" s="1" t="str">
-        <f>IF('weekly hours'!S64=0," ",'weekly hours'!S64/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W64" s="1"/>
     </row>
     <row r="65" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A65">
@@ -9687,25 +9516,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S65" s="1" t="str">
+        <f>IF('weekly hours'!S65=0," ",'weekly hours'!S65/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T65" s="1" t="str">
         <f>IF('weekly hours'!T65=0," ",'weekly hours'!T65/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T65" s="1" t="str">
+      <c r="U65" s="1" t="str">
         <f>IF('weekly hours'!U65=0," ",'weekly hours'!U65/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U65" s="1" t="str">
+      <c r="V65" s="1" t="str">
         <f>IF('weekly hours'!V65=0," ",'weekly hours'!V65/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V65" s="1" t="str">
-        <f>IF('weekly hours'!W65=0," ",'weekly hours'!W65/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W65" s="1" t="str">
-        <f>IF('weekly hours'!S65=0," ",'weekly hours'!S65/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W65" s="1"/>
     </row>
     <row r="66" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A66">
@@ -9781,25 +9607,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S66" s="1" t="str">
+        <f>IF('weekly hours'!S66=0," ",'weekly hours'!S66/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T66" s="1" t="str">
         <f>IF('weekly hours'!T66=0," ",'weekly hours'!T66/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T66" s="1" t="str">
+      <c r="U66" s="1" t="str">
         <f>IF('weekly hours'!U66=0," ",'weekly hours'!U66/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U66" s="1" t="str">
+      <c r="V66" s="1" t="str">
         <f>IF('weekly hours'!V66=0," ",'weekly hours'!V66/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V66" s="1" t="str">
-        <f>IF('weekly hours'!W66=0," ",'weekly hours'!W66/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W66" s="1" t="str">
-        <f>IF('weekly hours'!S66=0," ",'weekly hours'!S66/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W66" s="1"/>
     </row>
     <row r="67" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A67">
@@ -9875,25 +9698,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S67" s="1" t="str">
+        <f>IF('weekly hours'!S67=0," ",'weekly hours'!S67/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T67" s="1" t="str">
         <f>IF('weekly hours'!T67=0," ",'weekly hours'!T67/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T67" s="1" t="str">
+      <c r="U67" s="1" t="str">
         <f>IF('weekly hours'!U67=0," ",'weekly hours'!U67/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U67" s="1" t="str">
+      <c r="V67" s="1" t="str">
         <f>IF('weekly hours'!V67=0," ",'weekly hours'!V67/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V67" s="1" t="str">
-        <f>IF('weekly hours'!W67=0," ",'weekly hours'!W67/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W67" s="1" t="str">
-        <f>IF('weekly hours'!S67=0," ",'weekly hours'!S67/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W67" s="1"/>
     </row>
     <row r="68" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A68">
@@ -9969,25 +9789,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S68" s="1" t="str">
+        <f>IF('weekly hours'!S68=0," ",'weekly hours'!S68/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T68" s="1" t="str">
         <f>IF('weekly hours'!T68=0," ",'weekly hours'!T68/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T68" s="1" t="str">
+      <c r="U68" s="1" t="str">
         <f>IF('weekly hours'!U68=0," ",'weekly hours'!U68/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U68" s="1" t="str">
+      <c r="V68" s="1" t="str">
         <f>IF('weekly hours'!V68=0," ",'weekly hours'!V68/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V68" s="1" t="str">
-        <f>IF('weekly hours'!W68=0," ",'weekly hours'!W68/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W68" s="1" t="str">
-        <f>IF('weekly hours'!S68=0," ",'weekly hours'!S68/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W68" s="1"/>
     </row>
     <row r="69" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A69">
@@ -10063,25 +9880,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S69" s="1" t="str">
+        <f>IF('weekly hours'!S69=0," ",'weekly hours'!S69/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T69" s="1" t="str">
         <f>IF('weekly hours'!T69=0," ",'weekly hours'!T69/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T69" s="1" t="str">
+      <c r="U69" s="1" t="str">
         <f>IF('weekly hours'!U69=0," ",'weekly hours'!U69/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U69" s="1" t="str">
+      <c r="V69" s="1" t="str">
         <f>IF('weekly hours'!V69=0," ",'weekly hours'!V69/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V69" s="1" t="str">
-        <f>IF('weekly hours'!W69=0," ",'weekly hours'!W69/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W69" s="1" t="str">
-        <f>IF('weekly hours'!S69=0," ",'weekly hours'!S69/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W69" s="1"/>
     </row>
     <row r="70" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A70">
@@ -10157,25 +9971,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S70" s="1" t="str">
+        <f>IF('weekly hours'!S70=0," ",'weekly hours'!S70/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T70" s="1" t="str">
         <f>IF('weekly hours'!T70=0," ",'weekly hours'!T70/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T70" s="1" t="str">
+      <c r="U70" s="1" t="str">
         <f>IF('weekly hours'!U70=0," ",'weekly hours'!U70/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U70" s="1" t="str">
+      <c r="V70" s="1" t="str">
         <f>IF('weekly hours'!V70=0," ",'weekly hours'!V70/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V70" s="1" t="str">
-        <f>IF('weekly hours'!W70=0," ",'weekly hours'!W70/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W70" s="1" t="str">
-        <f>IF('weekly hours'!S70=0," ",'weekly hours'!S70/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W70" s="1"/>
     </row>
     <row r="71" spans="1:23" x14ac:dyDescent="0.55000000000000004">
       <c r="A71">
@@ -10251,25 +10062,22 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="S71" s="1" t="str">
+        <f>IF('weekly hours'!S71=0," ",'weekly hours'!S71/8*'weekly hours'!S$2)</f>
+        <v xml:space="preserve"> </v>
+      </c>
+      <c r="T71" s="1" t="str">
         <f>IF('weekly hours'!T71=0," ",'weekly hours'!T71/8*'weekly hours'!T$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="T71" s="1" t="str">
+      <c r="U71" s="1" t="str">
         <f>IF('weekly hours'!U71=0," ",'weekly hours'!U71/8*'weekly hours'!U$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="U71" s="1" t="str">
+      <c r="V71" s="1" t="str">
         <f>IF('weekly hours'!V71=0," ",'weekly hours'!V71/8*'weekly hours'!V$2)</f>
         <v xml:space="preserve"> </v>
       </c>
-      <c r="V71" s="1" t="str">
-        <f>IF('weekly hours'!W71=0," ",'weekly hours'!W71/8*'weekly hours'!W$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
-      <c r="W71" s="1" t="str">
-        <f>IF('weekly hours'!S71=0," ",'weekly hours'!S71/8*'weekly hours'!S$2)</f>
-        <v xml:space="preserve"> </v>
-      </c>
+      <c r="W71" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>